<commit_message>
altered the names on the plot
</commit_message>
<xml_diff>
--- a/combiningMuscleGroups_metabolics.xlsx
+++ b/combiningMuscleGroups_metabolics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JP\code\repos\Stanford\delplab\projects\muscleModel\muscleEnergyModel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{119766C3-FF83-4C0F-8C69-BCBF5342A1E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6DB660E-6747-41F0-B85A-D8AF017F9E14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="11385" xr2:uid="{CE15F475-ED09-4E78-B0C4-C13E019F565F}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="96">
   <si>
     <t>'metabolics_combined_addbrev_r_TOTAL'</t>
   </si>
@@ -296,6 +296,33 @@
   </si>
   <si>
     <t>average</t>
+  </si>
+  <si>
+    <t>plantarflexors</t>
+  </si>
+  <si>
+    <t>Glut. Med.</t>
+  </si>
+  <si>
+    <t>Hip Flexors</t>
+  </si>
+  <si>
+    <t>Hip Adductors</t>
+  </si>
+  <si>
+    <t>Glut. Min.</t>
+  </si>
+  <si>
+    <t>Glut. Max.</t>
+  </si>
+  <si>
+    <t>Hamstrings</t>
+  </si>
+  <si>
+    <t>Quads</t>
+  </si>
+  <si>
+    <t>Dorsiflexors</t>
   </si>
 </sst>
 </file>
@@ -525,31 +552,31 @@
               <c:strCache>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>plantarflex_r</c:v>
+                  <c:v>plantarflexors</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>glmed_r</c:v>
+                  <c:v>Glut. Med.</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>hipflexors_r</c:v>
+                  <c:v>Hip Flexors</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>hipadductors_r</c:v>
+                  <c:v>Hip Adductors</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>glmin_r</c:v>
+                  <c:v>Glut. Min.</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>glmax_r</c:v>
+                  <c:v>Glut. Max.</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>hamstrings_r</c:v>
+                  <c:v>Hamstrings</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>quads_r</c:v>
+                  <c:v>Quads</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>dorsiflex_r</c:v>
+                  <c:v>Dorsiflexors</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1736,7 +1763,7 @@
   <dimension ref="A1:Q42"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="J11" zoomScale="57" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="R72" sqref="R72"/>
+      <selection activeCell="M27" sqref="M27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2533,7 +2560,7 @@
         <v>1.1971549515368701E-2</v>
       </c>
       <c r="M18" t="s">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="N18">
         <f>N5-P5</f>
@@ -2580,7 +2607,7 @@
         <v>3.9931231429446497E-2</v>
       </c>
       <c r="M19" t="s">
-        <v>58</v>
+        <v>88</v>
       </c>
       <c r="N19">
         <f>N7-P7</f>
@@ -2627,7 +2654,7 @@
         <v>1.23793135674809E-2</v>
       </c>
       <c r="M20" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="N20">
         <f>N11-P11</f>
@@ -2674,7 +2701,7 @@
         <v>6.3599147861742505E-2</v>
       </c>
       <c r="M21" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="N21">
         <f>N3-P3</f>
@@ -2721,7 +2748,7 @@
         <v>0.13766045224279599</v>
       </c>
       <c r="M22" t="s">
-        <v>59</v>
+        <v>91</v>
       </c>
       <c r="N22">
         <f>N8-P8</f>
@@ -2768,7 +2795,7 @@
         <v>0.23913295813053501</v>
       </c>
       <c r="M23" t="s">
-        <v>57</v>
+        <v>92</v>
       </c>
       <c r="N23">
         <f>N6-P6</f>
@@ -2815,7 +2842,7 @@
         <v>8.4929063683891498E-2</v>
       </c>
       <c r="M24" t="s">
-        <v>79</v>
+        <v>93</v>
       </c>
       <c r="N24">
         <f>N9-P9</f>
@@ -2862,7 +2889,7 @@
         <v>0.62463811980739403</v>
       </c>
       <c r="M25" t="s">
-        <v>80</v>
+        <v>94</v>
       </c>
       <c r="N25">
         <f>N10-P10</f>
@@ -2909,7 +2936,7 @@
         <v>2.77162108162698E-2</v>
       </c>
       <c r="M26" t="s">
-        <v>77</v>
+        <v>95</v>
       </c>
       <c r="N26">
         <f>N4-P4</f>

</xml_diff>

<commit_message>
two bar graphs of the musle savings.
</commit_message>
<xml_diff>
--- a/combiningMuscleGroups_metabolics.xlsx
+++ b/combiningMuscleGroups_metabolics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JP\code\repos\Stanford\delplab\projects\muscleModel\muscleEnergyModel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6DB660E-6747-41F0-B85A-D8AF017F9E14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BC5D1C4-E7B7-4697-9067-5F7C99CC8B0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="11385" xr2:uid="{CE15F475-ED09-4E78-B0C4-C13E019F565F}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="96">
   <si>
     <t>'metabolics_combined_addbrev_r_TOTAL'</t>
   </si>
@@ -298,9 +298,6 @@
     <t>average</t>
   </si>
   <si>
-    <t>plantarflexors</t>
-  </si>
-  <si>
     <t>Glut. Med.</t>
   </si>
   <si>
@@ -323,6 +320,9 @@
   </si>
   <si>
     <t>Dorsiflexors</t>
+  </si>
+  <si>
+    <t>Plantarflexors</t>
   </si>
 </sst>
 </file>
@@ -546,13 +546,32 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="8"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="C00000"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000B-7426-4B70-89BA-6AA6B21BDFD1}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
           <c:cat>
             <c:strRef>
               <c:f>Sheet1!$M$18:$M$26</c:f>
               <c:strCache>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>plantarflexors</c:v>
+                  <c:v>Plantarflexors</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>Glut. Med.</c:v>
@@ -682,8 +701,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.87707797048025782"/>
-              <c:y val="0.39295708117367806"/>
+              <c:x val="0.82471935762539461"/>
+              <c:y val="0.43717539078270645"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -785,7 +804,7 @@
                 <a:pPr>
                   <a:defRPr sz="3200" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx2"/>
+                      <a:sysClr val="windowText" lastClr="000000"/>
                     </a:solidFill>
                     <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                     <a:ea typeface="+mn-ea"/>
@@ -794,6 +813,9 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US" sz="3200">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
                     <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                     <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                   </a:rPr>
@@ -817,7 +839,7 @@
               <a:pPr>
                 <a:defRPr sz="3200" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
-                    <a:schemeClr val="tx2"/>
+                    <a:sysClr val="windowText" lastClr="000000"/>
                   </a:solidFill>
                   <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                   <a:ea typeface="+mn-ea"/>
@@ -914,7 +936,726 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="4000" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mj-lt"/>
+                <a:ea typeface="+mj-ea"/>
+                <a:cs typeface="+mj-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="4000">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Metabolic Savings [W/kg]</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="4000" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mj-lt"/>
+              <a:ea typeface="+mj-ea"/>
+              <a:cs typeface="+mj-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="5.858768560870594E-2"/>
+          <c:y val="0.10768514373486546"/>
+          <c:w val="0.83620440044324129"/>
+          <c:h val="0.88143290317811451"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="19"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="C00000"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000B-DF43-4186-B19B-F4C974EDBD43}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="20"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="C00000"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000A-DF43-4186-B19B-F4C974EDBD43}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="21"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="C00000"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000009-DF43-4186-B19B-F4C974EDBD43}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="22"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="C00000"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000008-DF43-4186-B19B-F4C974EDBD43}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="23"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="C00000"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-DF43-4186-B19B-F4C974EDBD43}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="24"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="C00000"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000006-DF43-4186-B19B-F4C974EDBD43}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="25"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="C00000"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-DF43-4186-B19B-F4C974EDBD43}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="26"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="C00000"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000004-DF43-4186-B19B-F4C974EDBD43}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="27"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="C00000"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-DF43-4186-B19B-F4C974EDBD43}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="28"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="C00000"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000002-DF43-4186-B19B-F4C974EDBD43}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$G$38:$G$66</c:f>
+              <c:strCache>
+                <c:ptCount val="29"/>
+                <c:pt idx="0">
+                  <c:v>glmed_r</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>gastroc_r</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>soleus_r</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>glmin_r</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>iliopsoas_r</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>addlong_r</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>glmax_r</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>bflh_r</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>recfem_r</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>grac_r</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>semiten_r</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>addbrev_r</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>tfl_r</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>addmag_r</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>vaslat_r</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>piri_r</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>sart_r</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>vasint_r</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>fdl_r</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>bfsh_r</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>perbrev_r</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>fhl_r</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>tibpost_r</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>ehl_r</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>perlong_r</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>vasmed_r</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>semimem_r</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>edl_r</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>tibant_r</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$J$38:$J$66</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="29"/>
+                <c:pt idx="0">
+                  <c:v>7.5209242026738954E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.9836063795169536E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.4665573797224023E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.2242431615998053E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.1676495550654549E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.9258105112709001E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.3092656959581841E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.1182060659515202E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.4850214914313795E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.4035276696262457E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.3209940170816E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.0105470147435399E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>9.1654973857755E-3</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>7.032197436332252E-3</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>4.7992810111035511E-3</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2.7440462030560494E-3</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2.0530929815953114E-3</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.3255786036606015E-3</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>4.2032324920247008E-4</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>-2.7215386688995286E-4</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>-8.6090460607114987E-4</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>-1.4842240355961468E-3</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>-2.6928150138243005E-3</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>-4.1096917282433497E-3</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>-6.5040627559118484E-3</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>-7.1359477316770142E-3</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>-1.3950190982223012E-2</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>-1.836982139057735E-2</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>-6.1718467600211505E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-DF43-4186-B19B-F4C974EDBD43}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="10"/>
+        <c:axId val="836823680"/>
+        <c:axId val="836821384"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="836823680"/>
+        <c:scaling>
+          <c:orientation val="maxMin"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="high"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="dk1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="2400" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="836821384"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="836821384"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="t"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="2400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="836823680"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:pattFill prst="ltDnDiag">
+          <a:fgClr>
+            <a:schemeClr val="dk1">
+              <a:lumMod val="15000"/>
+              <a:lumOff val="85000"/>
+            </a:schemeClr>
+          </a:fgClr>
+          <a:bgClr>
+            <a:schemeClr val="lt1"/>
+          </a:bgClr>
+        </a:pattFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="lt1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1422,20 +2163,569 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="221">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="22225" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="15875">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="800" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltDnDiag">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltDnDiag">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
+    </cs:spPr>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="major">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltDnDiag">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>535780</xdr:colOff>
+      <xdr:colOff>535779</xdr:colOff>
       <xdr:row>28</xdr:row>
       <xdr:rowOff>110725</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>27</xdr:col>
-      <xdr:colOff>551447</xdr:colOff>
-      <xdr:row>67</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:col>34</xdr:col>
+      <xdr:colOff>150395</xdr:colOff>
+      <xdr:row>81</xdr:row>
+      <xdr:rowOff>133684</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1455,6 +2745,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>957131</xdr:colOff>
+      <xdr:row>83</xdr:row>
+      <xdr:rowOff>112178</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>630561</xdr:colOff>
+      <xdr:row>154</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{47D45D86-2720-4424-9738-045ED1D8E48F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1760,23 +3086,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB7901D6-903F-4996-A78B-1108649D94A1}">
-  <dimension ref="A1:Q42"/>
+  <dimension ref="A1:Q66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J11" zoomScale="57" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="M27" sqref="M27"/>
+    <sheetView tabSelected="1" topLeftCell="N11" zoomScale="54" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="42.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="24.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="24.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="19" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="15" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="24.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -2560,7 +3885,7 @@
         <v>1.1971549515368701E-2</v>
       </c>
       <c r="M18" t="s">
-        <v>87</v>
+        <v>95</v>
       </c>
       <c r="N18">
         <f>N5-P5</f>
@@ -2607,7 +3932,7 @@
         <v>3.9931231429446497E-2</v>
       </c>
       <c r="M19" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="N19">
         <f>N7-P7</f>
@@ -2654,7 +3979,7 @@
         <v>1.23793135674809E-2</v>
       </c>
       <c r="M20" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="N20">
         <f>N11-P11</f>
@@ -2701,7 +4026,7 @@
         <v>6.3599147861742505E-2</v>
       </c>
       <c r="M21" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="N21">
         <f>N3-P3</f>
@@ -2748,7 +4073,7 @@
         <v>0.13766045224279599</v>
       </c>
       <c r="M22" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="N22">
         <f>N8-P8</f>
@@ -2795,7 +4120,7 @@
         <v>0.23913295813053501</v>
       </c>
       <c r="M23" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="N23">
         <f>N6-P6</f>
@@ -2842,7 +4167,7 @@
         <v>8.4929063683891498E-2</v>
       </c>
       <c r="M24" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="N24">
         <f>N9-P9</f>
@@ -2889,7 +4214,7 @@
         <v>0.62463811980739403</v>
       </c>
       <c r="M25" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="N25">
         <f>N10-P10</f>
@@ -2936,7 +4261,7 @@
         <v>2.77162108162698E-2</v>
       </c>
       <c r="M26" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="N26">
         <f>N4-P4</f>
@@ -3128,7 +4453,7 @@
         <v>6.3599147861742505E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>30</v>
       </c>
@@ -3145,7 +4470,7 @@
         <v>0.13766045224279599</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>31</v>
       </c>
@@ -3162,7 +4487,7 @@
         <v>0.23913295813053501</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>32</v>
       </c>
@@ -3179,7 +4504,7 @@
         <v>8.4929063683891498E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>33</v>
       </c>
@@ -3195,8 +4520,11 @@
       <c r="E36">
         <v>0.62463811980739403</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G36" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>34</v>
       </c>
@@ -3212,8 +4540,21 @@
       <c r="E37">
         <v>2.77162108162698E-2</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G37" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H37" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="I37" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="J37" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="K37" s="1"/>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>35</v>
       </c>
@@ -3229,8 +4570,23 @@
       <c r="E38">
         <v>0.32241986326164801</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G38" t="s">
+        <v>58</v>
+      </c>
+      <c r="H38">
+        <f>H14-J14</f>
+        <v>0.12597674155529737</v>
+      </c>
+      <c r="I38">
+        <f>I14-K14</f>
+        <v>2.4441742498180541E-2</v>
+      </c>
+      <c r="J38">
+        <f>AVERAGE(H38:I38)</f>
+        <v>7.5209242026738954E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>36</v>
       </c>
@@ -3246,8 +4602,23 @@
       <c r="E39">
         <v>7.5214946751856596E-2</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G39" t="s">
+        <v>56</v>
+      </c>
+      <c r="H39">
+        <f>H12-J12</f>
+        <v>2.3876326054454111E-2</v>
+      </c>
+      <c r="I39">
+        <f>I12-K12</f>
+        <v>9.5795801535884961E-2</v>
+      </c>
+      <c r="J39">
+        <f>AVERAGE(H39:I39)</f>
+        <v>5.9836063795169536E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>37</v>
       </c>
@@ -3263,8 +4634,23 @@
       <c r="E40">
         <v>7.2882831158641997E-2</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G40" t="s">
+        <v>69</v>
+      </c>
+      <c r="H40">
+        <f>H25-J25</f>
+        <v>3.9966238379833041E-2</v>
+      </c>
+      <c r="I40">
+        <f>I25-K25</f>
+        <v>4.9364909214615005E-2</v>
+      </c>
+      <c r="J40">
+        <f>AVERAGE(H40:I40)</f>
+        <v>4.4665573797224023E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>38</v>
       </c>
@@ -3280,8 +4666,23 @@
       <c r="E41">
         <v>0.56312647087532497</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G41" t="s">
+        <v>59</v>
+      </c>
+      <c r="H41">
+        <f>H15-J15</f>
+        <v>5.9248549155514113E-2</v>
+      </c>
+      <c r="I41">
+        <f>I15-K15</f>
+        <v>5.2363140764819932E-3</v>
+      </c>
+      <c r="J41">
+        <f>AVERAGE(H41:I41)</f>
+        <v>3.2242431615998053E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>39</v>
       </c>
@@ -3296,6 +4697,429 @@
       </c>
       <c r="E42">
         <v>0.16069641294079301</v>
+      </c>
+      <c r="G42" t="s">
+        <v>61</v>
+      </c>
+      <c r="H42">
+        <f>H17-J17</f>
+        <v>3.2598443083486028E-2</v>
+      </c>
+      <c r="I42">
+        <f>I17-K17</f>
+        <v>3.0754548017823069E-2</v>
+      </c>
+      <c r="J42">
+        <f>AVERAGE(H42:I42)</f>
+        <v>3.1676495550654549E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G43" t="s">
+        <v>48</v>
+      </c>
+      <c r="H43">
+        <f>H4-J4</f>
+        <v>2.0657175569811004E-2</v>
+      </c>
+      <c r="I43">
+        <f>I4-K4</f>
+        <v>3.7859034655606999E-2</v>
+      </c>
+      <c r="J43">
+        <f>AVERAGE(H43:I43)</f>
+        <v>2.9258105112709001E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G44" t="s">
+        <v>57</v>
+      </c>
+      <c r="H44">
+        <f>H13-J13</f>
+        <v>3.8894973659715879E-2</v>
+      </c>
+      <c r="I44">
+        <f>I13-K13</f>
+        <v>7.2903402594478028E-3</v>
+      </c>
+      <c r="J44">
+        <f>AVERAGE(H44:I44)</f>
+        <v>2.3092656959581841E-2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G45" t="s">
+        <v>50</v>
+      </c>
+      <c r="H45">
+        <f>H6-J6</f>
+        <v>2.9217141314681297E-2</v>
+      </c>
+      <c r="I45">
+        <f>I6-K6</f>
+        <v>1.3146980004349107E-2</v>
+      </c>
+      <c r="J45">
+        <f>AVERAGE(H45:I45)</f>
+        <v>2.1182060659515202E-2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G46" t="s">
+        <v>65</v>
+      </c>
+      <c r="H46">
+        <f>H21-J21</f>
+        <v>-3.5544347341054904E-2</v>
+      </c>
+      <c r="I46">
+        <f>I21-K21</f>
+        <v>6.5244777169682494E-2</v>
+      </c>
+      <c r="J46">
+        <f>AVERAGE(H46:I46)</f>
+        <v>1.4850214914313795E-2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G47" t="s">
+        <v>60</v>
+      </c>
+      <c r="H47">
+        <f>H16-J16</f>
+        <v>1.7838664695353404E-2</v>
+      </c>
+      <c r="I47">
+        <f>I16-K16</f>
+        <v>1.023188869717151E-2</v>
+      </c>
+      <c r="J47">
+        <f>AVERAGE(H47:I47)</f>
+        <v>1.4035276696262457E-2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G48" t="s">
+        <v>68</v>
+      </c>
+      <c r="H48">
+        <f>H24-J24</f>
+        <v>1.4921727003982095E-2</v>
+      </c>
+      <c r="I48">
+        <f>I24-K24</f>
+        <v>1.1498153337649905E-2</v>
+      </c>
+      <c r="J48">
+        <f>AVERAGE(H48:I48)</f>
+        <v>1.3209940170816E-2</v>
+      </c>
+    </row>
+    <row r="49" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G49" t="s">
+        <v>47</v>
+      </c>
+      <c r="H49">
+        <f>H3-J3</f>
+        <v>8.6139232696491007E-3</v>
+      </c>
+      <c r="I49">
+        <f>I3-K3</f>
+        <v>1.1597017025221697E-2</v>
+      </c>
+      <c r="J49">
+        <f>AVERAGE(H49:I49)</f>
+        <v>1.0105470147435399E-2</v>
+      </c>
+    </row>
+    <row r="50" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G50" t="s">
+        <v>70</v>
+      </c>
+      <c r="H50">
+        <f>H26-J26</f>
+        <v>1.39500073732228E-2</v>
+      </c>
+      <c r="I50">
+        <f>I26-K26</f>
+        <v>4.3809873983281997E-3</v>
+      </c>
+      <c r="J50">
+        <f>AVERAGE(H50:I50)</f>
+        <v>9.1654973857755E-3</v>
+      </c>
+    </row>
+    <row r="51" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G51" t="s">
+        <v>49</v>
+      </c>
+      <c r="H51">
+        <f>H5-J5</f>
+        <v>6.4637272559078945E-3</v>
+      </c>
+      <c r="I51">
+        <f>I5-K5</f>
+        <v>7.6006676167566095E-3</v>
+      </c>
+      <c r="J51">
+        <f>AVERAGE(H51:I51)</f>
+        <v>7.032197436332252E-3</v>
+      </c>
+    </row>
+    <row r="52" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G52" t="s">
+        <v>74</v>
+      </c>
+      <c r="H52">
+        <f>H30-J30</f>
+        <v>-9.2342115537791258E-4</v>
+      </c>
+      <c r="I52">
+        <f>I30-K30</f>
+        <v>1.0521983177585015E-2</v>
+      </c>
+      <c r="J52">
+        <f>AVERAGE(H52:I52)</f>
+        <v>4.7992810111035511E-3</v>
+      </c>
+    </row>
+    <row r="53" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G53" t="s">
+        <v>64</v>
+      </c>
+      <c r="H53">
+        <f>H20-J20</f>
+        <v>4.6299019847542994E-3</v>
+      </c>
+      <c r="I53">
+        <f>I20-K20</f>
+        <v>8.5819042135779934E-4</v>
+      </c>
+      <c r="J53">
+        <f>AVERAGE(H53:I53)</f>
+        <v>2.7440462030560494E-3</v>
+      </c>
+    </row>
+    <row r="54" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G54" t="s">
+        <v>66</v>
+      </c>
+      <c r="H54">
+        <f>H22-J22</f>
+        <v>4.4103864439636042E-3</v>
+      </c>
+      <c r="I54">
+        <f>I22-K22</f>
+        <v>-3.0420048077298145E-4</v>
+      </c>
+      <c r="J54">
+        <f>AVERAGE(H54:I54)</f>
+        <v>2.0530929815953114E-3</v>
+      </c>
+    </row>
+    <row r="55" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G55" t="s">
+        <v>73</v>
+      </c>
+      <c r="H55">
+        <f>H29-J29</f>
+        <v>4.8710057793996953E-3</v>
+      </c>
+      <c r="I55">
+        <f>I29-K29</f>
+        <v>-2.2198485720784922E-3</v>
+      </c>
+      <c r="J55">
+        <f>AVERAGE(H55:I55)</f>
+        <v>1.3255786036606015E-3</v>
+      </c>
+    </row>
+    <row r="56" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G56" t="s">
+        <v>54</v>
+      </c>
+      <c r="H56">
+        <f>H10-J10</f>
+        <v>9.2531371218344035E-4</v>
+      </c>
+      <c r="I56">
+        <f>I10-K10</f>
+        <v>-8.4667213778500186E-5</v>
+      </c>
+      <c r="J56">
+        <f>AVERAGE(H56:I56)</f>
+        <v>4.2032324920247008E-4</v>
+      </c>
+    </row>
+    <row r="57" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G57" t="s">
+        <v>51</v>
+      </c>
+      <c r="H57">
+        <f>H7-J7</f>
+        <v>5.1444062054161049E-3</v>
+      </c>
+      <c r="I57">
+        <f>I7-K7</f>
+        <v>-5.6887139391960106E-3</v>
+      </c>
+      <c r="J57">
+        <f>AVERAGE(H57:I57)</f>
+        <v>-2.7215386688995286E-4</v>
+      </c>
+    </row>
+    <row r="58" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G58" t="s">
+        <v>62</v>
+      </c>
+      <c r="H58">
+        <f>H18-J18</f>
+        <v>-1.119594560945996E-4</v>
+      </c>
+      <c r="I58">
+        <f>I18-K18</f>
+        <v>-1.6098497560477001E-3</v>
+      </c>
+      <c r="J58">
+        <f>AVERAGE(H58:I58)</f>
+        <v>-8.6090460607114987E-4</v>
+      </c>
+    </row>
+    <row r="59" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G59" t="s">
+        <v>55</v>
+      </c>
+      <c r="H59">
+        <f>H11-J11</f>
+        <v>-1.8726072483839923E-4</v>
+      </c>
+      <c r="I59">
+        <f>I11-K11</f>
+        <v>-2.7811873463538944E-3</v>
+      </c>
+      <c r="J59">
+        <f>AVERAGE(H59:I59)</f>
+        <v>-1.4842240355961468E-3</v>
+      </c>
+    </row>
+    <row r="60" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G60" t="s">
+        <v>72</v>
+      </c>
+      <c r="H60">
+        <f>H28-J28</f>
+        <v>-2.746374923766802E-3</v>
+      </c>
+      <c r="I60">
+        <f>I28-K28</f>
+        <v>-2.6392551038817991E-3</v>
+      </c>
+      <c r="J60">
+        <f>AVERAGE(H60:I60)</f>
+        <v>-2.6928150138243005E-3</v>
+      </c>
+    </row>
+    <row r="61" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G61" t="s">
+        <v>53</v>
+      </c>
+      <c r="H61">
+        <f>H9-J9</f>
+        <v>-2.624312760175801E-3</v>
+      </c>
+      <c r="I61">
+        <f>I9-K9</f>
+        <v>-5.5950706963108984E-3</v>
+      </c>
+      <c r="J61">
+        <f>AVERAGE(H61:I61)</f>
+        <v>-4.1096917282433497E-3</v>
+      </c>
+    </row>
+    <row r="62" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G62" t="s">
+        <v>63</v>
+      </c>
+      <c r="H62">
+        <f>H19-J19</f>
+        <v>-4.8506078101632003E-3</v>
+      </c>
+      <c r="I62">
+        <f>I19-K19</f>
+        <v>-8.1575177016604966E-3</v>
+      </c>
+      <c r="J62">
+        <f>AVERAGE(H62:I62)</f>
+        <v>-6.5040627559118484E-3</v>
+      </c>
+    </row>
+    <row r="63" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G63" t="s">
+        <v>75</v>
+      </c>
+      <c r="H63">
+        <f>H31-J31</f>
+        <v>-6.2920820849140247E-3</v>
+      </c>
+      <c r="I63">
+        <f>I31-K31</f>
+        <v>-7.9798133784400038E-3</v>
+      </c>
+      <c r="J63">
+        <f>AVERAGE(H63:I63)</f>
+        <v>-7.1359477316770142E-3</v>
+      </c>
+    </row>
+    <row r="64" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G64" t="s">
+        <v>67</v>
+      </c>
+      <c r="H64">
+        <f>H23-J23</f>
+        <v>3.7250500623951993E-2</v>
+      </c>
+      <c r="I64">
+        <f>I23-K23</f>
+        <v>-6.5150882588398018E-2</v>
+      </c>
+      <c r="J64">
+        <f>AVERAGE(H64:I64)</f>
+        <v>-1.3950190982223012E-2</v>
+      </c>
+    </row>
+    <row r="65" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G65" t="s">
+        <v>52</v>
+      </c>
+      <c r="H65">
+        <f>H8-J8</f>
+        <v>-1.82949807867894E-2</v>
+      </c>
+      <c r="I65">
+        <f>I8-K8</f>
+        <v>-1.84446619943653E-2</v>
+      </c>
+      <c r="J65">
+        <f>AVERAGE(H65:I65)</f>
+        <v>-1.836982139057735E-2</v>
+      </c>
+    </row>
+    <row r="66" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G66" t="s">
+        <v>71</v>
+      </c>
+      <c r="H66">
+        <f>H27-J27</f>
+        <v>-4.2685459837906004E-2</v>
+      </c>
+      <c r="I66">
+        <f>I27-K27</f>
+        <v>-8.0751475362517006E-2</v>
+      </c>
+      <c r="J66">
+        <f>AVERAGE(H66:I66)</f>
+        <v>-6.1718467600211505E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
editing some of the names and plots.
</commit_message>
<xml_diff>
--- a/combiningMuscleGroups_metabolics.xlsx
+++ b/combiningMuscleGroups_metabolics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JP\code\repos\Stanford\delplab\projects\muscleModel\muscleEnergyModel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BC5D1C4-E7B7-4697-9067-5F7C99CC8B0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{557E2802-4F7E-4052-AA66-B86673F4038B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="11385" xr2:uid="{CE15F475-ED09-4E78-B0C4-C13E019F565F}"/>
   </bookViews>
@@ -3088,8 +3088,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB7901D6-903F-4996-A78B-1108649D94A1}">
   <dimension ref="A1:Q66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N11" zoomScale="54" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="M19" sqref="M19"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="93" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
few small calculations for the WCB 2022 abstract
</commit_message>
<xml_diff>
--- a/combiningMuscleGroups_metabolics.xlsx
+++ b/combiningMuscleGroups_metabolics.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JP\code\repos\Stanford\delplab\projects\muscleModel\muscleEnergyModel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC1F5E46-29D1-4A5C-90A8-AD0C90219B79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F9C3B2D4-410B-492D-B9E8-00633C3E698F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="11385" xr2:uid="{CE15F475-ED09-4E78-B0C4-C13E019F565F}"/>
+    <workbookView xWindow="1455" yWindow="1305" windowWidth="21600" windowHeight="11385" xr2:uid="{CE15F475-ED09-4E78-B0C4-C13E019F565F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="101">
   <si>
     <t>'metabolics_combined_addbrev_r_TOTAL'</t>
   </si>
@@ -323,6 +324,21 @@
   </si>
   <si>
     <t>Plantarflexors</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Glut. Med. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gastroc. </t>
+  </si>
+  <si>
+    <t>Soleus</t>
+  </si>
+  <si>
+    <t>Tib. Ant.</t>
+  </si>
+  <si>
+    <t>Ext. Dig. Longus</t>
   </si>
 </sst>
 </file>
@@ -1011,9 +1027,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="5.858768560870594E-2"/>
-          <c:y val="0.10768514373486546"/>
+          <c:y val="0.18210350495813191"/>
           <c:w val="0.83620440044324129"/>
-          <c:h val="0.88143290317811451"/>
+          <c:h val="0.80701445979810482"/>
         </c:manualLayout>
       </c:layout>
       <c:barChart>
@@ -1034,159 +1050,7 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dPt>
-            <c:idx val="19"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="C00000"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{0000000B-DF43-4186-B19B-F4C974EDBD43}"/>
-              </c:ext>
-            </c:extLst>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="20"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="C00000"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{0000000A-DF43-4186-B19B-F4C974EDBD43}"/>
-              </c:ext>
-            </c:extLst>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="21"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="C00000"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000009-DF43-4186-B19B-F4C974EDBD43}"/>
-              </c:ext>
-            </c:extLst>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="22"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="C00000"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000008-DF43-4186-B19B-F4C974EDBD43}"/>
-              </c:ext>
-            </c:extLst>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="23"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="C00000"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000007-DF43-4186-B19B-F4C974EDBD43}"/>
-              </c:ext>
-            </c:extLst>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="24"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="C00000"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000006-DF43-4186-B19B-F4C974EDBD43}"/>
-              </c:ext>
-            </c:extLst>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="25"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="C00000"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000005-DF43-4186-B19B-F4C974EDBD43}"/>
-              </c:ext>
-            </c:extLst>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="26"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="C00000"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000004-DF43-4186-B19B-F4C974EDBD43}"/>
-              </c:ext>
-            </c:extLst>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="27"/>
+            <c:idx val="3"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
             <c:spPr>
@@ -1205,7 +1069,7 @@
             </c:extLst>
           </c:dPt>
           <c:dPt>
-            <c:idx val="28"/>
+            <c:idx val="4"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
             <c:spPr>
@@ -1225,105 +1089,47 @@
           </c:dPt>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$G$38:$G$66</c:f>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Sheet1!$G$38:$G$66</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>(Sheet1!$G$38:$G$40,Sheet1!$G$65:$G$66)</c:f>
               <c:strCache>
-                <c:ptCount val="29"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>glmed_r</c:v>
+                  <c:v>Glut. Med. </c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>gastroc_r</c:v>
+                  <c:v>Gastroc. </c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>soleus_r</c:v>
+                  <c:v>Soleus</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>glmin_r</c:v>
+                  <c:v>Ext. Dig. Longus</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>iliopsoas_r</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>addlong_r</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>glmax_r</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>bflh_r</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>recfem_r</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>grac_r</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>semiten_r</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>addbrev_r</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>tfl_r</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>addmag_r</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>vaslat_r</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>piri_r</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>sart_r</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>vasint_r</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>fdl_r</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>bfsh_r</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>perbrev_r</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>fhl_r</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>tibpost_r</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>ehl_r</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>perlong_r</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>vasmed_r</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>semimem_r</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>edl_r</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>tibant_r</c:v>
+                  <c:v>Tib. Ant.</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$J$38:$J$66</c:f>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Sheet1!$J$38:$J$66</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>(Sheet1!$J$38:$J$40,Sheet1!$J$65:$J$66)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="29"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>7.5209242026738954E-2</c:v>
                 </c:pt>
@@ -1334,87 +1140,131 @@
                   <c:v>4.4665573797224023E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.2242431615998053E-2</c:v>
+                  <c:v>-1.836982139057735E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.1676495550654549E-2</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2.9258105112709001E-2</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>2.3092656959581841E-2</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>2.1182060659515202E-2</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1.4850214914313795E-2</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1.4035276696262457E-2</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>1.3209940170816E-2</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>1.0105470147435399E-2</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>9.1654973857755E-3</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>7.032197436332252E-3</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>4.7992810111035511E-3</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>2.7440462030560494E-3</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>2.0530929815953114E-3</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>1.3255786036606015E-3</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>4.2032324920247008E-4</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>-2.7215386688995286E-4</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>-8.6090460607114987E-4</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>-1.4842240355961468E-3</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>-2.6928150138243005E-3</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>-4.1096917282433497E-3</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>-6.5040627559118484E-3</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>-7.1359477316770142E-3</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>-1.3950190982223012E-2</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>-1.836982139057735E-2</c:v>
-                </c:pt>
-                <c:pt idx="28">
                   <c:v>-6.1718467600211505E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+              <c15:categoryFilterExceptions>
+                <c15:categoryFilterException>
+                  <c15:sqref>Sheet1!$J$57</c15:sqref>
+                  <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                    <a:solidFill>
+                      <a:srgbClr val="C00000"/>
+                    </a:solidFill>
+                    <a:ln>
+                      <a:noFill/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c15:spPr>
+                  <c15:invertIfNegative val="0"/>
+                  <c15:bubble3D val="0"/>
+                </c15:categoryFilterException>
+                <c15:categoryFilterException>
+                  <c15:sqref>Sheet1!$J$58</c15:sqref>
+                  <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                    <a:solidFill>
+                      <a:srgbClr val="C00000"/>
+                    </a:solidFill>
+                    <a:ln>
+                      <a:noFill/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c15:spPr>
+                  <c15:invertIfNegative val="0"/>
+                  <c15:bubble3D val="0"/>
+                </c15:categoryFilterException>
+                <c15:categoryFilterException>
+                  <c15:sqref>Sheet1!$J$59</c15:sqref>
+                  <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                    <a:solidFill>
+                      <a:srgbClr val="C00000"/>
+                    </a:solidFill>
+                    <a:ln>
+                      <a:noFill/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c15:spPr>
+                  <c15:invertIfNegative val="0"/>
+                  <c15:bubble3D val="0"/>
+                </c15:categoryFilterException>
+                <c15:categoryFilterException>
+                  <c15:sqref>Sheet1!$J$60</c15:sqref>
+                  <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                    <a:solidFill>
+                      <a:srgbClr val="C00000"/>
+                    </a:solidFill>
+                    <a:ln>
+                      <a:noFill/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c15:spPr>
+                  <c15:invertIfNegative val="0"/>
+                  <c15:bubble3D val="0"/>
+                </c15:categoryFilterException>
+                <c15:categoryFilterException>
+                  <c15:sqref>Sheet1!$J$61</c15:sqref>
+                  <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                    <a:solidFill>
+                      <a:srgbClr val="C00000"/>
+                    </a:solidFill>
+                    <a:ln>
+                      <a:noFill/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c15:spPr>
+                  <c15:invertIfNegative val="0"/>
+                  <c15:bubble3D val="0"/>
+                </c15:categoryFilterException>
+                <c15:categoryFilterException>
+                  <c15:sqref>Sheet1!$J$62</c15:sqref>
+                  <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                    <a:solidFill>
+                      <a:srgbClr val="C00000"/>
+                    </a:solidFill>
+                    <a:ln>
+                      <a:noFill/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c15:spPr>
+                  <c15:invertIfNegative val="0"/>
+                  <c15:bubble3D val="0"/>
+                </c15:categoryFilterException>
+                <c15:categoryFilterException>
+                  <c15:sqref>Sheet1!$J$63</c15:sqref>
+                  <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                    <a:solidFill>
+                      <a:srgbClr val="C00000"/>
+                    </a:solidFill>
+                    <a:ln>
+                      <a:noFill/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c15:spPr>
+                  <c15:invertIfNegative val="0"/>
+                  <c15:bubble3D val="0"/>
+                </c15:categoryFilterException>
+                <c15:categoryFilterException>
+                  <c15:sqref>Sheet1!$J$64</c15:sqref>
+                  <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                    <a:solidFill>
+                      <a:srgbClr val="C00000"/>
+                    </a:solidFill>
+                    <a:ln>
+                      <a:noFill/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c15:spPr>
+                  <c15:invertIfNegative val="0"/>
+                  <c15:bubble3D val="0"/>
+                </c15:categoryFilterException>
+              </c15:categoryFilterExceptions>
+            </c:ext>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-DF43-4186-B19B-F4C974EDBD43}"/>
             </c:ext>
@@ -2753,15 +2603,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>957131</xdr:colOff>
-      <xdr:row>83</xdr:row>
-      <xdr:rowOff>112178</xdr:rowOff>
+      <xdr:colOff>1319082</xdr:colOff>
+      <xdr:row>84</xdr:row>
+      <xdr:rowOff>35978</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>630561</xdr:colOff>
-      <xdr:row>154</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>530680</xdr:colOff>
+      <xdr:row>123</xdr:row>
+      <xdr:rowOff>54429</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3088,8 +2938,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB7901D6-903F-4996-A78B-1108649D94A1}">
   <dimension ref="A1:Q66"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="93" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="N12" sqref="N12"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="89" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="S111" sqref="S111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3201,15 +3051,15 @@
         <v>0.29409495082989451</v>
       </c>
       <c r="O3">
-        <f t="shared" ref="O3:Q3" si="0">SUM(I3:I5)</f>
+        <f>SUM(I3:I5)</f>
         <v>0.27905160716980709</v>
       </c>
       <c r="P3">
-        <f t="shared" si="0"/>
+        <f>SUM(J3:J5)</f>
         <v>0.25836012473452652</v>
       </c>
       <c r="Q3">
-        <f t="shared" si="0"/>
+        <f>SUM(K3:K5)</f>
         <v>0.22199488787222177</v>
       </c>
     </row>
@@ -3252,15 +3102,15 @@
         <v>0.31078908559959717</v>
       </c>
       <c r="O4">
-        <f t="shared" ref="O4:Q4" si="1">SUM(I8:I9,I27)</f>
+        <f>SUM(I8:I9,I27)</f>
         <v>0.32815028097230969</v>
       </c>
       <c r="P4">
-        <f t="shared" si="1"/>
+        <f>SUM(J8:J9,J27)</f>
         <v>0.37439383898446843</v>
       </c>
       <c r="Q4">
-        <f t="shared" si="1"/>
+        <f>SUM(K8:K9,K27)</f>
         <v>0.43294148902550289</v>
       </c>
     </row>
@@ -3288,15 +3138,15 @@
         <v>9.7378891563382905E-2</v>
       </c>
       <c r="I5">
-        <f t="shared" ref="I5:K5" si="2">SUM(C5:C8)</f>
+        <f>SUM(C5:C8)</f>
         <v>9.3702599316393104E-2</v>
       </c>
       <c r="J5">
-        <f t="shared" si="2"/>
+        <f>SUM(D5:D8)</f>
         <v>9.091516430747501E-2</v>
       </c>
       <c r="K5">
-        <f t="shared" si="2"/>
+        <f>SUM(E5:E8)</f>
         <v>8.6101931699636494E-2</v>
       </c>
       <c r="M5" t="s">
@@ -3307,15 +3157,15 @@
         <v>0.95308205611647612</v>
       </c>
       <c r="O5">
-        <f t="shared" ref="O5:Q5" si="3">SUM(I10:I11,I12,I18:I19,I25,I28)</f>
+        <f>SUM(I10:I11,I12,I18:I19,I25,I28)</f>
         <v>1.3576614469420909</v>
       </c>
       <c r="P5">
-        <f t="shared" si="3"/>
+        <f>SUM(J10:J11,J12,J18:J19,J25,J28)</f>
         <v>0.89621038088486848</v>
       </c>
       <c r="Q5">
-        <f t="shared" si="3"/>
+        <f>SUM(K10:K11,K12,K18:K19,K25,K28)</f>
         <v>1.2277732133133135</v>
       </c>
     </row>
@@ -3354,19 +3204,19 @@
         <v>57</v>
       </c>
       <c r="N6">
-        <f>H13</f>
+        <f t="shared" ref="N6:Q7" si="0">H13</f>
         <v>0.13822277934839369</v>
       </c>
       <c r="O6">
-        <f t="shared" ref="O6:Q6" si="4">I13</f>
+        <f t="shared" si="0"/>
         <v>0.14551864270180881</v>
       </c>
       <c r="P6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>9.9327805688677814E-2</v>
       </c>
       <c r="Q6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>0.13822830244236101</v>
       </c>
     </row>
@@ -3405,19 +3255,19 @@
         <v>58</v>
       </c>
       <c r="N7">
-        <f>H14</f>
+        <f t="shared" si="0"/>
         <v>0.54092588158624955</v>
       </c>
       <c r="O7">
-        <f t="shared" ref="O7:Q7" si="5">I14</f>
+        <f t="shared" si="0"/>
         <v>0.50031033766522182</v>
       </c>
       <c r="P7">
-        <f t="shared" si="5"/>
+        <f t="shared" si="0"/>
         <v>0.41494914003095218</v>
       </c>
       <c r="Q7">
-        <f t="shared" si="5"/>
+        <f t="shared" si="0"/>
         <v>0.47586859516704128</v>
       </c>
     </row>
@@ -3460,15 +3310,15 @@
         <v>0.15048126581133359</v>
       </c>
       <c r="O8">
-        <f t="shared" ref="O8:Q8" si="6">SUM(I15,I20)</f>
+        <f>SUM(I15,I20)</f>
         <v>0.1158879969683453</v>
       </c>
       <c r="P8">
-        <f t="shared" si="6"/>
+        <f>SUM(J15,J20)</f>
         <v>8.6602814671065176E-2</v>
       </c>
       <c r="Q8">
-        <f t="shared" si="6"/>
+        <f>SUM(K15,K20)</f>
         <v>0.1097934924705055</v>
       </c>
     </row>
@@ -3613,15 +3463,15 @@
         <v>0.74393149274886039</v>
       </c>
       <c r="O11">
-        <f t="shared" ref="O11:Q11" si="7">SUM(I16,I17,I22,I26)</f>
+        <f>SUM(I16,I17,I22,I26)</f>
         <v>0.83549716832213838</v>
       </c>
       <c r="P11">
-        <f t="shared" si="7"/>
+        <f>SUM(J16,J17,J22,J26)</f>
         <v>0.67513399115283457</v>
       </c>
       <c r="Q11">
-        <f t="shared" si="7"/>
+        <f>SUM(K16,K17,K22,K26)</f>
         <v>0.79043394468958861</v>
       </c>
     </row>
@@ -3649,15 +3499,15 @@
         <v>0.359150188901036</v>
       </c>
       <c r="I12">
-        <f t="shared" ref="I12:K12" si="8">SUM(C15:C16)</f>
+        <f>SUM(C15:C16)</f>
         <v>0.52764076926951797</v>
       </c>
       <c r="J12">
-        <f t="shared" si="8"/>
+        <f>SUM(D15:D16)</f>
         <v>0.33527386284658189</v>
       </c>
       <c r="K12">
-        <f t="shared" si="8"/>
+        <f>SUM(E15:E16)</f>
         <v>0.43184496773363301</v>
       </c>
     </row>
@@ -3685,15 +3535,15 @@
         <v>0.13822277934839369</v>
       </c>
       <c r="I13">
-        <f t="shared" ref="I13:K13" si="9">SUM(C17:C19)</f>
+        <f>SUM(C17:C19)</f>
         <v>0.14551864270180881</v>
       </c>
       <c r="J13">
-        <f t="shared" si="9"/>
+        <f>SUM(D17:D19)</f>
         <v>9.9327805688677814E-2</v>
       </c>
       <c r="K13">
-        <f t="shared" si="9"/>
+        <f>SUM(E17:E19)</f>
         <v>0.13822830244236101</v>
       </c>
     </row>
@@ -3721,15 +3571,15 @@
         <v>0.54092588158624955</v>
       </c>
       <c r="I14">
-        <f t="shared" ref="I14:M14" si="10">SUM(C20:C22)</f>
+        <f>SUM(C20:C22)</f>
         <v>0.50031033766522182</v>
       </c>
       <c r="J14">
-        <f t="shared" si="10"/>
+        <f>SUM(D20:D22)</f>
         <v>0.41494914003095218</v>
       </c>
       <c r="K14">
-        <f t="shared" si="10"/>
+        <f>SUM(E20:E22)</f>
         <v>0.47586859516704128</v>
       </c>
     </row>
@@ -3757,15 +3607,15 @@
         <v>0.13546237120570009</v>
       </c>
       <c r="I15">
-        <f t="shared" ref="I15:K15" si="11">SUM(C23:C25)</f>
+        <f>SUM(C23:C25)</f>
         <v>0.1026504929795066</v>
       </c>
       <c r="J15">
-        <f t="shared" si="11"/>
+        <f>SUM(D23:D25)</f>
         <v>7.6213822050185981E-2</v>
       </c>
       <c r="K15">
-        <f t="shared" si="11"/>
+        <f>SUM(E23:E25)</f>
         <v>9.7414178903024604E-2</v>
       </c>
     </row>
@@ -3828,15 +3678,15 @@
         <v>0.53534423223405203</v>
       </c>
       <c r="I17">
-        <f t="shared" ref="I17:K17" si="12">SUM(C27,C31)</f>
+        <f>SUM(C27,C31)</f>
         <v>0.58867129043722</v>
       </c>
       <c r="J17">
-        <f t="shared" si="12"/>
+        <f>SUM(D27,D31)</f>
         <v>0.502745789150566</v>
       </c>
       <c r="K17">
-        <f t="shared" si="12"/>
+        <f>SUM(E27,E31)</f>
         <v>0.55791674241939693</v>
       </c>
       <c r="M17" s="1" t="s">
@@ -3896,7 +3746,7 @@
         <v>0.12988823362877744</v>
       </c>
       <c r="P18">
-        <f>AVERAGE(N18:O18)</f>
+        <f t="shared" ref="P18:P26" si="1">AVERAGE(N18:O18)</f>
         <v>9.3379954430192535E-2</v>
       </c>
     </row>
@@ -3943,7 +3793,7 @@
         <v>2.4441742498180541E-2</v>
       </c>
       <c r="P19">
-        <f>AVERAGE(N19:O19)</f>
+        <f t="shared" si="1"/>
         <v>7.5209242026738954E-2</v>
       </c>
     </row>
@@ -3990,7 +3840,7 @@
         <v>4.5063223632549776E-2</v>
       </c>
       <c r="P20">
-        <f>AVERAGE(N20:O20)</f>
+        <f t="shared" si="1"/>
         <v>5.6930362614287799E-2</v>
       </c>
     </row>
@@ -4037,7 +3887,7 @@
         <v>5.7056719297585323E-2</v>
       </c>
       <c r="P21">
-        <f>AVERAGE(N21:O21)</f>
+        <f t="shared" si="1"/>
         <v>4.6395772696476656E-2</v>
       </c>
     </row>
@@ -4084,7 +3934,7 @@
         <v>6.0945044978397978E-3</v>
       </c>
       <c r="P22">
-        <f>AVERAGE(N22:O22)</f>
+        <f t="shared" si="1"/>
         <v>3.4986477819054104E-2</v>
       </c>
     </row>
@@ -4131,7 +3981,7 @@
         <v>7.2903402594478028E-3</v>
       </c>
       <c r="P23">
-        <f>AVERAGE(N23:O23)</f>
+        <f t="shared" si="1"/>
         <v>2.3092656959581841E-2</v>
       </c>
     </row>
@@ -4178,7 +4028,7 @@
         <v>-4.6194463185595003E-2</v>
       </c>
       <c r="P24">
-        <f>AVERAGE(N24:O24)</f>
+        <f t="shared" si="1"/>
         <v>2.0169655981218254E-2</v>
       </c>
     </row>
@@ -4225,7 +4075,7 @@
         <v>6.5567098396749124E-2</v>
       </c>
       <c r="P25">
-        <f>AVERAGE(N25:O25)</f>
+        <f t="shared" si="1"/>
         <v>1.3839126797400958E-2</v>
       </c>
     </row>
@@ -4272,7 +4122,7 @@
         <v>-0.1047912080531932</v>
       </c>
       <c r="P26">
-        <f>AVERAGE(N26:O26)</f>
+        <f t="shared" si="1"/>
         <v>-8.4197980719032228E-2</v>
       </c>
     </row>
@@ -4571,7 +4421,7 @@
         <v>0.32241986326164801</v>
       </c>
       <c r="G38" t="s">
-        <v>58</v>
+        <v>96</v>
       </c>
       <c r="H38">
         <f>H14-J14</f>
@@ -4582,7 +4432,7 @@
         <v>2.4441742498180541E-2</v>
       </c>
       <c r="J38">
-        <f>AVERAGE(H38:I38)</f>
+        <f t="shared" ref="J38:J66" si="2">AVERAGE(H38:I38)</f>
         <v>7.5209242026738954E-2</v>
       </c>
     </row>
@@ -4603,7 +4453,7 @@
         <v>7.5214946751856596E-2</v>
       </c>
       <c r="G39" t="s">
-        <v>56</v>
+        <v>97</v>
       </c>
       <c r="H39">
         <f>H12-J12</f>
@@ -4614,7 +4464,7 @@
         <v>9.5795801535884961E-2</v>
       </c>
       <c r="J39">
-        <f>AVERAGE(H39:I39)</f>
+        <f t="shared" si="2"/>
         <v>5.9836063795169536E-2</v>
       </c>
     </row>
@@ -4635,7 +4485,7 @@
         <v>7.2882831158641997E-2</v>
       </c>
       <c r="G40" t="s">
-        <v>69</v>
+        <v>98</v>
       </c>
       <c r="H40">
         <f>H25-J25</f>
@@ -4646,7 +4496,7 @@
         <v>4.9364909214615005E-2</v>
       </c>
       <c r="J40">
-        <f>AVERAGE(H40:I40)</f>
+        <f t="shared" si="2"/>
         <v>4.4665573797224023E-2</v>
       </c>
     </row>
@@ -4678,7 +4528,7 @@
         <v>5.2363140764819932E-3</v>
       </c>
       <c r="J41">
-        <f>AVERAGE(H41:I41)</f>
+        <f t="shared" si="2"/>
         <v>3.2242431615998053E-2</v>
       </c>
     </row>
@@ -4710,7 +4560,7 @@
         <v>3.0754548017823069E-2</v>
       </c>
       <c r="J42">
-        <f>AVERAGE(H42:I42)</f>
+        <f t="shared" si="2"/>
         <v>3.1676495550654549E-2</v>
       </c>
     </row>
@@ -4727,7 +4577,7 @@
         <v>3.7859034655606999E-2</v>
       </c>
       <c r="J43">
-        <f>AVERAGE(H43:I43)</f>
+        <f t="shared" si="2"/>
         <v>2.9258105112709001E-2</v>
       </c>
     </row>
@@ -4744,7 +4594,7 @@
         <v>7.2903402594478028E-3</v>
       </c>
       <c r="J44">
-        <f>AVERAGE(H44:I44)</f>
+        <f t="shared" si="2"/>
         <v>2.3092656959581841E-2</v>
       </c>
     </row>
@@ -4761,7 +4611,7 @@
         <v>1.3146980004349107E-2</v>
       </c>
       <c r="J45">
-        <f>AVERAGE(H45:I45)</f>
+        <f t="shared" si="2"/>
         <v>2.1182060659515202E-2</v>
       </c>
     </row>
@@ -4778,7 +4628,7 @@
         <v>6.5244777169682494E-2</v>
       </c>
       <c r="J46">
-        <f>AVERAGE(H46:I46)</f>
+        <f t="shared" si="2"/>
         <v>1.4850214914313795E-2</v>
       </c>
     </row>
@@ -4795,7 +4645,7 @@
         <v>1.023188869717151E-2</v>
       </c>
       <c r="J47">
-        <f>AVERAGE(H47:I47)</f>
+        <f t="shared" si="2"/>
         <v>1.4035276696262457E-2</v>
       </c>
     </row>
@@ -4812,7 +4662,7 @@
         <v>1.1498153337649905E-2</v>
       </c>
       <c r="J48">
-        <f>AVERAGE(H48:I48)</f>
+        <f t="shared" si="2"/>
         <v>1.3209940170816E-2</v>
       </c>
     </row>
@@ -4829,7 +4679,7 @@
         <v>1.1597017025221697E-2</v>
       </c>
       <c r="J49">
-        <f>AVERAGE(H49:I49)</f>
+        <f t="shared" si="2"/>
         <v>1.0105470147435399E-2</v>
       </c>
     </row>
@@ -4846,7 +4696,7 @@
         <v>4.3809873983281997E-3</v>
       </c>
       <c r="J50">
-        <f>AVERAGE(H50:I50)</f>
+        <f t="shared" si="2"/>
         <v>9.1654973857755E-3</v>
       </c>
     </row>
@@ -4863,7 +4713,7 @@
         <v>7.6006676167566095E-3</v>
       </c>
       <c r="J51">
-        <f>AVERAGE(H51:I51)</f>
+        <f t="shared" si="2"/>
         <v>7.032197436332252E-3</v>
       </c>
     </row>
@@ -4880,7 +4730,7 @@
         <v>1.0521983177585015E-2</v>
       </c>
       <c r="J52">
-        <f>AVERAGE(H52:I52)</f>
+        <f t="shared" si="2"/>
         <v>4.7992810111035511E-3</v>
       </c>
     </row>
@@ -4897,7 +4747,7 @@
         <v>8.5819042135779934E-4</v>
       </c>
       <c r="J53">
-        <f>AVERAGE(H53:I53)</f>
+        <f t="shared" si="2"/>
         <v>2.7440462030560494E-3</v>
       </c>
     </row>
@@ -4914,7 +4764,7 @@
         <v>-3.0420048077298145E-4</v>
       </c>
       <c r="J54">
-        <f>AVERAGE(H54:I54)</f>
+        <f t="shared" si="2"/>
         <v>2.0530929815953114E-3</v>
       </c>
     </row>
@@ -4931,7 +4781,7 @@
         <v>-2.2198485720784922E-3</v>
       </c>
       <c r="J55">
-        <f>AVERAGE(H55:I55)</f>
+        <f t="shared" si="2"/>
         <v>1.3255786036606015E-3</v>
       </c>
     </row>
@@ -4948,7 +4798,7 @@
         <v>-8.4667213778500186E-5</v>
       </c>
       <c r="J56">
-        <f>AVERAGE(H56:I56)</f>
+        <f t="shared" si="2"/>
         <v>4.2032324920247008E-4</v>
       </c>
     </row>
@@ -4965,7 +4815,7 @@
         <v>-5.6887139391960106E-3</v>
       </c>
       <c r="J57">
-        <f>AVERAGE(H57:I57)</f>
+        <f t="shared" si="2"/>
         <v>-2.7215386688995286E-4</v>
       </c>
     </row>
@@ -4982,7 +4832,7 @@
         <v>-1.6098497560477001E-3</v>
       </c>
       <c r="J58">
-        <f>AVERAGE(H58:I58)</f>
+        <f t="shared" si="2"/>
         <v>-8.6090460607114987E-4</v>
       </c>
     </row>
@@ -4999,7 +4849,7 @@
         <v>-2.7811873463538944E-3</v>
       </c>
       <c r="J59">
-        <f>AVERAGE(H59:I59)</f>
+        <f t="shared" si="2"/>
         <v>-1.4842240355961468E-3</v>
       </c>
     </row>
@@ -5016,7 +4866,7 @@
         <v>-2.6392551038817991E-3</v>
       </c>
       <c r="J60">
-        <f>AVERAGE(H60:I60)</f>
+        <f t="shared" si="2"/>
         <v>-2.6928150138243005E-3</v>
       </c>
     </row>
@@ -5033,7 +4883,7 @@
         <v>-5.5950706963108984E-3</v>
       </c>
       <c r="J61">
-        <f>AVERAGE(H61:I61)</f>
+        <f t="shared" si="2"/>
         <v>-4.1096917282433497E-3</v>
       </c>
     </row>
@@ -5050,7 +4900,7 @@
         <v>-8.1575177016604966E-3</v>
       </c>
       <c r="J62">
-        <f>AVERAGE(H62:I62)</f>
+        <f t="shared" si="2"/>
         <v>-6.5040627559118484E-3</v>
       </c>
     </row>
@@ -5067,7 +4917,7 @@
         <v>-7.9798133784400038E-3</v>
       </c>
       <c r="J63">
-        <f>AVERAGE(H63:I63)</f>
+        <f t="shared" si="2"/>
         <v>-7.1359477316770142E-3</v>
       </c>
     </row>
@@ -5084,13 +4934,13 @@
         <v>-6.5150882588398018E-2</v>
       </c>
       <c r="J64">
-        <f>AVERAGE(H64:I64)</f>
+        <f t="shared" si="2"/>
         <v>-1.3950190982223012E-2</v>
       </c>
     </row>
     <row r="65" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G65" t="s">
-        <v>52</v>
+        <v>100</v>
       </c>
       <c r="H65">
         <f>H8-J8</f>
@@ -5101,13 +4951,13 @@
         <v>-1.84446619943653E-2</v>
       </c>
       <c r="J65">
-        <f>AVERAGE(H65:I65)</f>
+        <f t="shared" si="2"/>
         <v>-1.836982139057735E-2</v>
       </c>
     </row>
     <row r="66" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G66" t="s">
-        <v>71</v>
+        <v>99</v>
       </c>
       <c r="H66">
         <f>H27-J27</f>
@@ -5118,7 +4968,7 @@
         <v>-8.0751475362517006E-2</v>
       </c>
       <c r="J66">
-        <f>AVERAGE(H66:I66)</f>
+        <f t="shared" si="2"/>
         <v>-6.1718467600211505E-2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updating figures and numbers for the WCB abstract
</commit_message>
<xml_diff>
--- a/combiningMuscleGroups_metabolics.xlsx
+++ b/combiningMuscleGroups_metabolics.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JP\code\repos\Stanford\delplab\projects\muscleModel\muscleEnergyModel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8B7AB92-B47D-460E-9266-0CF9CD8F9C86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{797EA41F-2333-40E2-B852-D0AF15D6F245}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CE15F475-ED09-4E78-B0C4-C13E019F565F}"/>
   </bookViews>
@@ -17,6 +17,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="112">
   <si>
     <t>'metabolics_combined_addbrev_r_TOTAL'</t>
   </si>
@@ -367,6 +368,12 @@
   <si>
     <t xml:space="preserve">Semiten. </t>
   </si>
+  <si>
+    <t>SE</t>
+  </si>
+  <si>
+    <t>sttdev</t>
+  </si>
 </sst>
 </file>
 
@@ -514,9 +521,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="4.9286509299567828E-2"/>
-          <c:y val="0.21680834172451727"/>
-          <c:w val="0.65006937643688489"/>
-          <c:h val="0.76366232226312147"/>
+          <c:y val="0.14276286904270277"/>
+          <c:w val="0.75455632164623831"/>
+          <c:h val="0.68415079141140112"/>
         </c:manualLayout>
       </c:layout>
       <c:barChart>
@@ -525,7 +532,7 @@
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
-          <c:order val="0"/>
+          <c:order val="1"/>
           <c:spPr>
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -555,7 +562,7 @@
             </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000006-C86D-4278-B4D7-A432F22147C5}"/>
+                <c16:uniqueId val="{0000000B-CB43-4D67-B75E-F284F931084E}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
@@ -576,7 +583,7 @@
             </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000005-C86D-4278-B4D7-A432F22147C5}"/>
+                <c16:uniqueId val="{0000000D-CB43-4D67-B75E-F284F931084E}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
@@ -597,7 +604,7 @@
             </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000004-C86D-4278-B4D7-A432F22147C5}"/>
+                <c16:uniqueId val="{0000000F-CB43-4D67-B75E-F284F931084E}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
@@ -616,6 +623,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000011-CB43-4D67-B75E-F284F931084E}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:cat>
             <c:strRef>
@@ -726,7 +738,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-C86D-4278-B4D7-A432F22147C5}"/>
+              <c16:uniqueId val="{00000012-CB43-4D67-B75E-F284F931084E}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -741,6 +753,236 @@
         <c:gapWidth val="10"/>
         <c:axId val="762762984"/>
         <c:axId val="762764952"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredBarSeries>
+              <c15:ser>
+                <c:idx val="1"/>
+                <c:order val="0"/>
+                <c:spPr>
+                  <a:solidFill>
+                    <a:schemeClr val="accent1"/>
+                  </a:solidFill>
+                  <a:ln>
+                    <a:solidFill>
+                      <a:schemeClr val="accent1"/>
+                    </a:solidFill>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:invertIfNegative val="0"/>
+                <c:dPt>
+                  <c:idx val="11"/>
+                  <c:invertIfNegative val="0"/>
+                  <c:bubble3D val="0"/>
+                  <c:spPr>
+                    <a:solidFill>
+                      <a:srgbClr val="C00000"/>
+                    </a:solidFill>
+                    <a:ln>
+                      <a:solidFill>
+                        <a:srgbClr val="C00000"/>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                  <c:extLst>
+                    <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                      <c16:uniqueId val="{00000014-CB43-4D67-B75E-F284F931084E}"/>
+                    </c:ext>
+                  </c:extLst>
+                </c:dPt>
+                <c:dPt>
+                  <c:idx val="12"/>
+                  <c:invertIfNegative val="0"/>
+                  <c:bubble3D val="0"/>
+                  <c:spPr>
+                    <a:solidFill>
+                      <a:srgbClr val="C00000"/>
+                    </a:solidFill>
+                    <a:ln>
+                      <a:solidFill>
+                        <a:srgbClr val="C00000"/>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                  <c:extLst>
+                    <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                      <c16:uniqueId val="{00000015-CB43-4D67-B75E-F284F931084E}"/>
+                    </c:ext>
+                  </c:extLst>
+                </c:dPt>
+                <c:dPt>
+                  <c:idx val="13"/>
+                  <c:invertIfNegative val="0"/>
+                  <c:bubble3D val="0"/>
+                  <c:spPr>
+                    <a:solidFill>
+                      <a:srgbClr val="C00000"/>
+                    </a:solidFill>
+                    <a:ln>
+                      <a:solidFill>
+                        <a:srgbClr val="C00000"/>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                  <c:extLst>
+                    <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                      <c16:uniqueId val="{00000016-CB43-4D67-B75E-F284F931084E}"/>
+                    </c:ext>
+                  </c:extLst>
+                </c:dPt>
+                <c:dPt>
+                  <c:idx val="14"/>
+                  <c:invertIfNegative val="0"/>
+                  <c:bubble3D val="0"/>
+                  <c:spPr>
+                    <a:solidFill>
+                      <a:srgbClr val="C00000"/>
+                    </a:solidFill>
+                    <a:ln>
+                      <a:solidFill>
+                        <a:srgbClr val="C00000"/>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                  <c:extLst>
+                    <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                      <c16:uniqueId val="{00000017-CB43-4D67-B75E-F284F931084E}"/>
+                    </c:ext>
+                  </c:extLst>
+                </c:dPt>
+                <c:cat>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'Sheet1 (2)'!$M$21:$M$35</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="15"/>
+                      <c:pt idx="0">
+                        <c:v>Plantarflexors</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>Glut. Med.</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>Hip Flexors</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>Hip Adductors</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>Glut. Min.</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>Glut. Max.</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>Bifem. Long Head</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>Rec. Fem. </c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>Semiten. </c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>Vas. Lat</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>Vas Int. </c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>Bifem. Short Head</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>Vas Med. </c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>Semimem. </c:v>
+                      </c:pt>
+                      <c:pt idx="14">
+                        <c:v>Dorsiflexors</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'Sheet1 (2)'!$P$21:$P$35</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="15"/>
+                      <c:pt idx="0">
+                        <c:v>9.3379954430192535E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>7.5209242026738954E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>5.6930362614287799E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>4.6395772696476656E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>3.4986477819054104E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>2.3092656959581841E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>2.1182060659515202E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>1.4850214914313795E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>1.3209940170816E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>4.7992810111035511E-3</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>1.3255786036606015E-3</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>-2.7215386688995286E-4</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>-7.1359477316770142E-3</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>-1.3950190982223012E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="14">
+                        <c:v>-8.4197980719032228E-2</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000013-CB43-4D67-B75E-F284F931084E}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredBarSeries>
+          </c:ext>
+        </c:extLst>
       </c:barChart>
       <c:catAx>
         <c:axId val="762762984"/>
@@ -776,20 +1018,22 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="2800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="3200" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1"/>
                     </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
+                    <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                     <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
+                    <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US" sz="2800">
+                  <a:rPr lang="en-US" sz="3200">
                     <a:solidFill>
                       <a:schemeClr val="tx1"/>
                     </a:solidFill>
+                    <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                    <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                   </a:rPr>
                   <a:t>Muscle Groups</a:t>
                 </a:r>
@@ -800,8 +1044,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.85235895107878468"/>
-              <c:y val="0.43717534702200977"/>
+              <c:x val="0.96011911867665989"/>
+              <c:y val="0.43215531581283151"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -817,13 +1061,13 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="2800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="3200" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1"/>
                   </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
+                  <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                   <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
+                  <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 </a:defRPr>
               </a:pPr>
               <a:endParaRPr lang="en-US"/>
@@ -877,6 +1121,7 @@
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.1"/>
+          <c:min val="-0.1"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="t"/>
@@ -913,11 +1158,39 @@
                     <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                     <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                   </a:rPr>
-                  <a:t>Metabolic Savings [W/kg]</a:t>
+                  <a:t>Reduction in Metabolic Rate per Gait Cycle</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="3200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                    <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                    <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                  </a:rPr>
+                  <a:t> </a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="3200">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                    <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                    <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                  </a:rPr>
+                  <a:t>[W/kg]</a:t>
                 </a:r>
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.16529098361096503"/>
+              <c:y val="2.7818680820783009E-2"/>
+            </c:manualLayout>
+          </c:layout>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -958,7 +1231,7 @@
           <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="t" anchorCtr="0"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
@@ -975,7 +1248,7 @@
           </a:p>
         </c:txPr>
         <c:crossAx val="762762984"/>
-        <c:crosses val="autoZero"/>
+        <c:crossesAt val="0"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:spPr>
@@ -988,25 +1261,15 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
     <c:showDLblsOverMax val="0"/>
+    <c:extLst/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
       <a:schemeClr val="bg1"/>
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="accent1">
-          <a:alpha val="93000"/>
-        </a:schemeClr>
-      </a:solidFill>
+      <a:noFill/>
       <a:round/>
     </a:ln>
     <a:effectLst/>
@@ -1026,6 +1289,7 @@
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
+  <c:userShapes r:id="rId3"/>
 </c:chartSpace>
 </file>
 
@@ -1556,6 +1820,1007 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="4.9286509299567828E-2"/>
+          <c:y val="0.21680834172451727"/>
+          <c:w val="0.65006937643688489"/>
+          <c:h val="0.76366232226312147"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="11"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="C00000"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:srgbClr val="C00000"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-94F6-4801-828A-03AC22CF8FCF}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="12"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="C00000"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:srgbClr val="C00000"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-94F6-4801-828A-03AC22CF8FCF}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="13"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="C00000"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:srgbClr val="C00000"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-94F6-4801-828A-03AC22CF8FCF}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="14"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="C00000"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:srgbClr val="C00000"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-94F6-4801-828A-03AC22CF8FCF}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>'Sheet1 (2)'!$R$21:$R$35</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="15"/>
+                  <c:pt idx="0">
+                    <c:v>2.5815251790771168E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>3.5898043180528499E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>8.3913344472701813E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>7.5384276355116133E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>2.0429710257291449E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>1.1173925297122205E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>5.6816600186487924E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>3.5634336705698842E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>1.2104160776775909E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>4.0465615086299894E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>2.5069955981681822E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>3.8300863578319094E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>5.9670312123648165E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>3.6204356236167488E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>1.4561610694501383E-2</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>'Sheet1 (2)'!$R$21:$R$35</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="15"/>
+                  <c:pt idx="0">
+                    <c:v>2.5815251790771168E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>3.5898043180528499E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>8.3913344472701813E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>7.5384276355116133E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>2.0429710257291449E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>1.1173925297122205E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>5.6816600186487924E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>3.5634336705698842E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>1.2104160776775909E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>4.0465615086299894E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>2.5069955981681822E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>3.8300863578319094E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>5.9670312123648165E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>3.6204356236167488E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>1.4561610694501383E-2</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="tx2">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Sheet1 (2)'!$M$21:$M$35</c:f>
+              <c:strCache>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>Plantarflexors</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Glut. Med.</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Hip Flexors</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Hip Adductors</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Glut. Min.</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Glut. Max.</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Bifem. Long Head</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Rec. Fem. </c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Semiten. </c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Vas. Lat</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Vas Int. </c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Bifem. Short Head</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Vas Med. </c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Semimem. </c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Dorsiflexors</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sheet1 (2)'!$P$21:$P$35</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>9.3379954430192535E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.5209242026738954E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.6930362614287799E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.6395772696476656E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.4986477819054104E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.3092656959581841E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.1182060659515202E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.4850214914313795E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.3209940170816E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4.7992810111035511E-3</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.3255786036606015E-3</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-2.7215386688995286E-4</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-7.1359477316770142E-3</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-1.3950190982223012E-2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-8.4197980719032228E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000008-94F6-4801-828A-03AC22CF8FCF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="11"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="C00000"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:srgbClr val="C00000"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000A-94F6-4801-828A-03AC22CF8FCF}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="12"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="C00000"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:srgbClr val="C00000"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000C-94F6-4801-828A-03AC22CF8FCF}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="13"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="C00000"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:srgbClr val="C00000"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000E-94F6-4801-828A-03AC22CF8FCF}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="14"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="C00000"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:srgbClr val="C00000"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000010-94F6-4801-828A-03AC22CF8FCF}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>'Sheet1 (2)'!$R$21:$R$35</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="15"/>
+                  <c:pt idx="0">
+                    <c:v>2.5815251790771168E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>3.5898043180528499E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>8.3913344472701813E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>7.5384276355116133E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>2.0429710257291449E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>1.1173925297122205E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>5.6816600186487924E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>3.5634336705698842E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>1.2104160776775909E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>4.0465615086299894E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>2.5069955981681822E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>3.8300863578319094E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>5.9670312123648165E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>3.6204356236167488E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>1.4561610694501383E-2</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>'Sheet1 (2)'!$R$21:$R$35</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="15"/>
+                  <c:pt idx="0">
+                    <c:v>2.5815251790771168E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>3.5898043180528499E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>8.3913344472701813E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>7.5384276355116133E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>2.0429710257291449E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>1.1173925297122205E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>5.6816600186487924E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>3.5634336705698842E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>1.2104160776775909E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>4.0465615086299894E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>2.5069955981681822E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>3.8300863578319094E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>5.9670312123648165E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>3.6204356236167488E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>1.4561610694501383E-2</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="tx2">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Sheet1 (2)'!$M$21:$M$35</c:f>
+              <c:strCache>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>Plantarflexors</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Glut. Med.</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Hip Flexors</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Hip Adductors</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Glut. Min.</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Glut. Max.</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Bifem. Long Head</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Rec. Fem. </c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Semiten. </c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Vas. Lat</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Vas Int. </c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Bifem. Short Head</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Vas Med. </c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Semimem. </c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Dorsiflexors</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sheet1 (2)'!$P$21:$P$35</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>9.3379954430192535E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.5209242026738954E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.6930362614287799E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.6395772696476656E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.4986477819054104E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.3092656959581841E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.1182060659515202E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.4850214914313795E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.3209940170816E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4.7992810111035511E-3</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.3255786036606015E-3</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-2.7215386688995286E-4</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-7.1359477316770142E-3</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-1.3950190982223012E-2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-8.4197980719032228E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000011-94F6-4801-828A-03AC22CF8FCF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="10"/>
+        <c:axId val="762762984"/>
+        <c:axId val="762764952"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="762762984"/>
+        <c:scaling>
+          <c:orientation val="maxMin"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="12700">
+              <a:solidFill>
+                <a:schemeClr val="bg2">
+                  <a:lumMod val="90000"/>
+                  <a:alpha val="70000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw dist="50800" dir="5400000" sx="1000" sy="1000" algn="ctr" rotWithShape="0">
+                <a:schemeClr val="bg2">
+                  <a:lumMod val="90000"/>
+                  <a:alpha val="80000"/>
+                </a:schemeClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="3200" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                    <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="3200">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                    <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                    <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                  </a:rPr>
+                  <a:t>Muscle Groups</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.86724181756239616"/>
+              <c:y val="0.43717534702200977"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="3200" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="cross"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="high"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx2">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="2400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="762764952"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="10"/>
+        <c:tickMarkSkip val="2"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="762764952"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="0.13"/>
+          <c:min val="-0.1"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="t"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="3200" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                    <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="3200">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                    <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                    <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                  </a:rPr>
+                  <a:t>Metabolic Savings [W/kg]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="3200" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="cross"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="2400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="762762984"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="accent1">
+          <a:alpha val="93000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
     <c:title>
       <c:overlay val="0"/>
       <c:spPr>
@@ -2015,7 +3280,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -2688,6 +3953,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="220">
   <cs:axisTitle>
@@ -4174,6 +5479,474 @@
 </file>
 
 <file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="220">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk2">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="31750" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700">
+        <a:solidFill>
+          <a:schemeClr val="lt2"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="221">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -4727,15 +6500,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>535779</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>58383</xdr:rowOff>
+      <xdr:colOff>172098</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>75700</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>34</xdr:col>
-      <xdr:colOff>150395</xdr:colOff>
-      <xdr:row>93</xdr:row>
-      <xdr:rowOff>81342</xdr:rowOff>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>392851</xdr:colOff>
+      <xdr:row>104</xdr:row>
+      <xdr:rowOff>23811</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4800,10 +6573,420 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>34</xdr:col>
+      <xdr:colOff>535780</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>29765</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>65</xdr:col>
+      <xdr:colOff>388522</xdr:colOff>
+      <xdr:row>93</xdr:row>
+      <xdr:rowOff>52724</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0916D1F9-6652-4013-85BA-42BF9D44678E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.44944</cdr:x>
+      <cdr:y>0.83349</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.66059</cdr:x>
+      <cdr:y>0.88589</cdr:y>
+    </cdr:to>
+    <cdr:grpSp>
+      <cdr:nvGrpSpPr>
+        <cdr:cNvPr id="13" name="Group 12">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BDF08B08-980F-4586-8547-4C639A45B158}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvGrpSpPr/>
+      </cdr:nvGrpSpPr>
+      <cdr:grpSpPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="8362188" y="10831643"/>
+          <a:ext cx="3928661" cy="681031"/>
+          <a:chOff x="8946454" y="10627992"/>
+          <a:chExt cx="3927407" cy="587761"/>
+        </a:xfrm>
+      </cdr:grpSpPr>
+      <cdr:cxnSp macro="">
+        <cdr:nvCxnSpPr>
+          <cdr:cNvPr id="4" name="Straight Arrow Connector 3">
+            <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F8135C97-4429-4DA6-AAEF-EF68C8771CB9}"/>
+              </a:ext>
+            </a:extLst>
+          </cdr:cNvPr>
+          <cdr:cNvCxnSpPr/>
+        </cdr:nvCxnSpPr>
+        <cdr:spPr>
+          <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:off x="11220535" y="10866771"/>
+            <a:ext cx="1653326" cy="0"/>
+          </a:xfrm>
+          <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="straightConnector1">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="28575" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:prstDash val="solid"/>
+            <a:round/>
+            <a:headEnd type="none" w="med" len="med"/>
+            <a:tailEnd type="arrow" w="med" len="med"/>
+          </a:ln>
+        </cdr:spPr>
+        <cdr:style>
+          <a:lnRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </cdr:style>
+      </cdr:cxnSp>
+      <cdr:sp macro="" textlink="">
+        <cdr:nvSpPr>
+          <cdr:cNvPr id="5" name="TextBox 4">
+            <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{10E65D4E-0FF7-4053-8C11-D5DF1B740842}"/>
+              </a:ext>
+            </a:extLst>
+          </cdr:cNvPr>
+          <cdr:cNvSpPr txBox="1"/>
+        </cdr:nvSpPr>
+        <cdr:spPr>
+          <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:off x="8946454" y="10627992"/>
+            <a:ext cx="2349462" cy="587761"/>
+          </a:xfrm>
+          <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+        </cdr:spPr>
+        <cdr:txBody>
+          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="square" rtlCol="0"/>
+          <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:r>
+              <a:rPr lang="en-US" sz="2400">
+                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              </a:rPr>
+              <a:t>Energy savings</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1100">
+              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            </a:endParaRPr>
+          </a:p>
+        </cdr:txBody>
+      </cdr:sp>
+    </cdr:grpSp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.18647</cdr:x>
+      <cdr:y>0.83349</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.41359</cdr:x>
+      <cdr:y>0.88589</cdr:y>
+    </cdr:to>
+    <cdr:grpSp>
+      <cdr:nvGrpSpPr>
+        <cdr:cNvPr id="14" name="Group 13">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8B359406-6348-4B1F-9C6B-EADCF68E88F0}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvGrpSpPr/>
+      </cdr:nvGrpSpPr>
+      <cdr:grpSpPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="3469428" y="10831644"/>
+          <a:ext cx="4225718" cy="681031"/>
+          <a:chOff x="3397173" y="10627993"/>
+          <a:chExt cx="4224369" cy="587761"/>
+        </a:xfrm>
+      </cdr:grpSpPr>
+      <cdr:sp macro="" textlink="">
+        <cdr:nvSpPr>
+          <cdr:cNvPr id="6" name="TextBox 1">
+            <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3C00A7B4-B0DD-420A-B1B5-2F0412F78203}"/>
+              </a:ext>
+            </a:extLst>
+          </cdr:cNvPr>
+          <cdr:cNvSpPr txBox="1"/>
+        </cdr:nvSpPr>
+        <cdr:spPr>
+          <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:off x="5013278" y="10627993"/>
+            <a:ext cx="2608264" cy="587761"/>
+          </a:xfrm>
+          <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+        </cdr:spPr>
+        <cdr:txBody>
+          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="square" rtlCol="0"/>
+          <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:lvl1pPr marL="0" indent="0">
+              <a:defRPr sz="1100">
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl1pPr>
+            <a:lvl2pPr marL="457200" indent="0">
+              <a:defRPr sz="1100">
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl2pPr>
+            <a:lvl3pPr marL="914400" indent="0">
+              <a:defRPr sz="1100">
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl3pPr>
+            <a:lvl4pPr marL="1371600" indent="0">
+              <a:defRPr sz="1100">
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl4pPr>
+            <a:lvl5pPr marL="1828800" indent="0">
+              <a:defRPr sz="1100">
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl5pPr>
+            <a:lvl6pPr marL="2286000" indent="0">
+              <a:defRPr sz="1100">
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl6pPr>
+            <a:lvl7pPr marL="2743200" indent="0">
+              <a:defRPr sz="1100">
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl7pPr>
+            <a:lvl8pPr marL="3200400" indent="0">
+              <a:defRPr sz="1100">
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl8pPr>
+            <a:lvl9pPr marL="3657600" indent="0">
+              <a:defRPr sz="1100">
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl9pPr>
+          </a:lstStyle>
+          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:r>
+              <a:rPr lang="en-US" sz="2400">
+                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              </a:rPr>
+              <a:t>Energy </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="2400" baseline="0">
+                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              </a:rPr>
+              <a:t>increase</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1100">
+              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            </a:endParaRPr>
+          </a:p>
+        </cdr:txBody>
+      </cdr:sp>
+      <cdr:cxnSp macro="">
+        <cdr:nvCxnSpPr>
+          <cdr:cNvPr id="10" name="Straight Arrow Connector 9">
+            <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{192303DB-243A-4E2D-BFFF-7838492E24A2}"/>
+              </a:ext>
+            </a:extLst>
+          </cdr:cNvPr>
+          <cdr:cNvCxnSpPr/>
+        </cdr:nvCxnSpPr>
+        <cdr:spPr>
+          <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" flipH="1">
+            <a:off x="3397173" y="10882234"/>
+            <a:ext cx="1598794" cy="0"/>
+          </a:xfrm>
+          <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="straightConnector1">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="28575" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:prstDash val="solid"/>
+            <a:round/>
+            <a:headEnd type="none" w="med" len="med"/>
+            <a:tailEnd type="arrow" w="med" len="med"/>
+          </a:ln>
+        </cdr:spPr>
+        <cdr:style>
+          <a:lnRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </cdr:style>
+      </cdr:cxnSp>
+    </cdr:grpSp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.04401</cdr:x>
+      <cdr:y>0.91576</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.95453</cdr:x>
+      <cdr:y>0.99362</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="15" name="TextBox 14">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C3AD24EA-E114-4597-8CAA-7AA7EEE9EE7D}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="814020" y="11466359"/>
+          <a:ext cx="16842440" cy="974912"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="none" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="2000" b="1">
+              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>Figure 1:</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="2000">
+              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t> Each muscle</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="2000" baseline="0">
+              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t> group's  two-subject average savings in metabolic rate when running with the spring is plotted with positive values in blue </a:t>
+          </a:r>
+        </a:p>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="2000" baseline="0">
+              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>indicating a reduction in average metabolic rate and negative values in red indicationg an increase in metabolic rate. </a:t>
+          </a:r>
+        </a:p>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+</c:userShapes>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -5177,10 +7360,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{730AE58A-BFCC-47A5-850F-F7F52B044D8D}">
-  <dimension ref="A1:Q66"/>
+  <dimension ref="A1:S66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D33" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="P37" sqref="P37"/>
+    <sheetView tabSelected="1" topLeftCell="D46" zoomScale="53" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Q111" sqref="Q111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5193,6 +7376,7 @@
     <col min="10" max="11" width="24.7109375" bestFit="1" customWidth="1"/>
     <col min="13" max="15" width="20.42578125" bestFit="1" customWidth="1"/>
     <col min="16" max="17" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="18" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -5987,7 +8171,7 @@
         <v>0.23913295813053501</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>14</v>
       </c>
@@ -6042,7 +8226,7 @@
         <v>8.4929063683891498E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>15</v>
       </c>
@@ -6074,7 +8258,7 @@
         <v>1.1971549515368701E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>16</v>
       </c>
@@ -6109,7 +8293,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>17</v>
       </c>
@@ -6155,8 +8339,14 @@
       <c r="Q20" s="1" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R20" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="S20" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>18</v>
       </c>
@@ -6206,8 +8396,16 @@
         <f>P21/(AVERAGE(N5:O5))*100</f>
         <v>8.082243166027915</v>
       </c>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R21">
+        <f>_xlfn.STDEV.P(N21:O21)/SQRT(2)</f>
+        <v>2.5815251790771168E-2</v>
+      </c>
+      <c r="S21">
+        <f>_xlfn.STDEV.P(N21:O21)</f>
+        <v>3.6508279198584917E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>19</v>
       </c>
@@ -6257,8 +8455,16 @@
         <f>P22/(AVERAGE(N7:O7))*100</f>
         <v>14.446144042281919</v>
       </c>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R22">
+        <f t="shared" ref="R22:R35" si="10">_xlfn.STDEV.P(N22:O22)/SQRT(2)</f>
+        <v>3.5898043180528499E-2</v>
+      </c>
+      <c r="S22">
+        <f t="shared" ref="S22:S35" si="11">_xlfn.STDEV.P(N22:O22)</f>
+        <v>5.0767499528558406E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
         <v>20</v>
       </c>
@@ -6304,8 +8510,16 @@
         <f t="shared" si="9"/>
         <v>5.6930362614287799E-2</v>
       </c>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R23">
+        <f t="shared" si="10"/>
+        <v>8.3913344472701813E-3</v>
+      </c>
+      <c r="S23">
+        <f t="shared" si="11"/>
+        <v>1.186713898173803E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
         <v>21</v>
       </c>
@@ -6351,8 +8565,16 @@
         <f t="shared" si="9"/>
         <v>4.6395772696476656E-2</v>
       </c>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R24">
+        <f t="shared" si="10"/>
+        <v>7.5384276355116133E-3</v>
+      </c>
+      <c r="S24">
+        <f t="shared" si="11"/>
+        <v>1.0660946601108667E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
         <v>22</v>
       </c>
@@ -6398,8 +8620,16 @@
         <f t="shared" si="9"/>
         <v>3.4986477819054104E-2</v>
       </c>
-    </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R25">
+        <f t="shared" si="10"/>
+        <v>2.0429710257291449E-2</v>
+      </c>
+      <c r="S25">
+        <f t="shared" si="11"/>
+        <v>2.8891973321214303E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>23</v>
       </c>
@@ -6445,8 +8675,16 @@
         <f t="shared" si="9"/>
         <v>2.3092656959581841E-2</v>
       </c>
-    </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R26">
+        <f t="shared" si="10"/>
+        <v>1.1173925297122205E-2</v>
+      </c>
+      <c r="S26">
+        <f t="shared" si="11"/>
+        <v>1.5802316700134038E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
         <v>24</v>
       </c>
@@ -6492,8 +8730,16 @@
         <f>AVERAGE(N27:O27)</f>
         <v>2.1182060659515202E-2</v>
       </c>
-    </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R27">
+        <f t="shared" si="10"/>
+        <v>5.6816600186487924E-3</v>
+      </c>
+      <c r="S27">
+        <f t="shared" si="11"/>
+        <v>8.035080655166095E-3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>25</v>
       </c>
@@ -6539,8 +8785,16 @@
         <f>AVERAGE(N28:O28)</f>
         <v>1.4850214914313795E-2</v>
       </c>
-    </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R28">
+        <f t="shared" si="10"/>
+        <v>3.5634336705698842E-2</v>
+      </c>
+      <c r="S28">
+        <f t="shared" si="11"/>
+        <v>5.0394562255368702E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>26</v>
       </c>
@@ -6586,8 +8840,16 @@
         <f>AVERAGE(N29:O29)</f>
         <v>1.3209940170816E-2</v>
       </c>
-    </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R29">
+        <f t="shared" si="10"/>
+        <v>1.2104160776775909E-3</v>
+      </c>
+      <c r="S29">
+        <f t="shared" si="11"/>
+        <v>1.711786833166095E-3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>27</v>
       </c>
@@ -6633,8 +8895,16 @@
         <f>AVERAGE(N30:O30)</f>
         <v>4.7992810111035511E-3</v>
       </c>
-    </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R30">
+        <f t="shared" si="10"/>
+        <v>4.0465615086299894E-3</v>
+      </c>
+      <c r="S30">
+        <f t="shared" si="11"/>
+        <v>5.7227021664814637E-3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
         <v>28</v>
       </c>
@@ -6680,8 +8950,16 @@
         <f>AVERAGE(N31:O31)</f>
         <v>1.3255786036606015E-3</v>
       </c>
-    </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R31">
+        <f t="shared" si="10"/>
+        <v>2.5069955981681822E-3</v>
+      </c>
+      <c r="S31">
+        <f t="shared" si="11"/>
+        <v>3.5454271757390937E-3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>29</v>
       </c>
@@ -6712,8 +8990,16 @@
         <f t="shared" si="9"/>
         <v>-2.7215386688995286E-4</v>
       </c>
-    </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R32">
+        <f t="shared" si="10"/>
+        <v>3.8300863578319094E-3</v>
+      </c>
+      <c r="S32">
+        <f t="shared" si="11"/>
+        <v>5.4165600723060578E-3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>30</v>
       </c>
@@ -6744,8 +9030,16 @@
         <f>AVERAGE(N33:O33)</f>
         <v>-7.1359477316770142E-3</v>
       </c>
-    </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R33">
+        <f t="shared" si="10"/>
+        <v>5.9670312123648165E-4</v>
+      </c>
+      <c r="S33">
+        <f t="shared" si="11"/>
+        <v>8.4386564676298959E-4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>31</v>
       </c>
@@ -6773,11 +9067,19 @@
         <v>-6.5150882588398018E-2</v>
       </c>
       <c r="P34">
-        <f t="shared" ref="P34" si="10">AVERAGE(N34:O34)</f>
+        <f t="shared" ref="P34" si="12">AVERAGE(N34:O34)</f>
         <v>-1.3950190982223012E-2</v>
       </c>
-    </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R34">
+        <f t="shared" si="10"/>
+        <v>3.6204356236167488E-2</v>
+      </c>
+      <c r="S34">
+        <f t="shared" si="11"/>
+        <v>5.1200691606175006E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>32</v>
       </c>
@@ -6812,8 +9114,16 @@
         <f>P35/(AVERAGE(N4:O4))*100</f>
         <v>-26.355546433389627</v>
       </c>
-    </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R35">
+        <f t="shared" si="10"/>
+        <v>1.4561610694501383E-2</v>
+      </c>
+      <c r="S35">
+        <f t="shared" si="11"/>
+        <v>2.0593227334160961E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>33</v>
       </c>
@@ -6833,7 +9143,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>34</v>
       </c>
@@ -6863,7 +9173,7 @@
       </c>
       <c r="K37" s="1"/>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>35</v>
       </c>
@@ -6891,11 +9201,11 @@
         <v>2.4441742498180541E-2</v>
       </c>
       <c r="J38">
-        <f t="shared" ref="J38:J66" si="11">AVERAGE(H38:I38)</f>
+        <f t="shared" ref="J38:J66" si="13">AVERAGE(H38:I38)</f>
         <v>7.5209242026738954E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>36</v>
       </c>
@@ -6923,11 +9233,11 @@
         <v>9.5795801535884961E-2</v>
       </c>
       <c r="J39">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>5.9836063795169536E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>37</v>
       </c>
@@ -6955,11 +9265,11 @@
         <v>4.9364909214615005E-2</v>
       </c>
       <c r="J40">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>4.4665573797224023E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>38</v>
       </c>
@@ -6987,11 +9297,11 @@
         <v>5.2363140764819932E-3</v>
       </c>
       <c r="J41">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>3.2242431615998053E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>39</v>
       </c>
@@ -7019,11 +9329,11 @@
         <v>3.0754548017823069E-2</v>
       </c>
       <c r="J42">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>3.1676495550654549E-2</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:19" x14ac:dyDescent="0.25">
       <c r="G43" t="s">
         <v>48</v>
       </c>
@@ -7036,11 +9346,11 @@
         <v>3.7859034655606999E-2</v>
       </c>
       <c r="J43">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>2.9258105112709001E-2</v>
       </c>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:19" x14ac:dyDescent="0.25">
       <c r="G44" t="s">
         <v>57</v>
       </c>
@@ -7053,11 +9363,11 @@
         <v>7.2903402594478028E-3</v>
       </c>
       <c r="J44">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>2.3092656959581841E-2</v>
       </c>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:19" x14ac:dyDescent="0.25">
       <c r="G45" t="s">
         <v>50</v>
       </c>
@@ -7070,11 +9380,11 @@
         <v>1.3146980004349107E-2</v>
       </c>
       <c r="J45">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>2.1182060659515202E-2</v>
       </c>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:19" x14ac:dyDescent="0.25">
       <c r="G46" t="s">
         <v>65</v>
       </c>
@@ -7087,11 +9397,11 @@
         <v>6.5244777169682494E-2</v>
       </c>
       <c r="J46">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>1.4850214914313795E-2</v>
       </c>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:19" x14ac:dyDescent="0.25">
       <c r="G47" t="s">
         <v>60</v>
       </c>
@@ -7104,11 +9414,11 @@
         <v>1.023188869717151E-2</v>
       </c>
       <c r="J47">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>1.4035276696262457E-2</v>
       </c>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:19" x14ac:dyDescent="0.25">
       <c r="G48" t="s">
         <v>68</v>
       </c>
@@ -7121,7 +9431,7 @@
         <v>1.1498153337649905E-2</v>
       </c>
       <c r="J48">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>1.3209940170816E-2</v>
       </c>
     </row>
@@ -7138,7 +9448,7 @@
         <v>1.1597017025221697E-2</v>
       </c>
       <c r="J49">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>1.0105470147435399E-2</v>
       </c>
     </row>
@@ -7155,7 +9465,7 @@
         <v>4.3809873983281997E-3</v>
       </c>
       <c r="J50">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>9.1654973857755E-3</v>
       </c>
     </row>
@@ -7172,7 +9482,7 @@
         <v>7.6006676167566095E-3</v>
       </c>
       <c r="J51">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>7.032197436332252E-3</v>
       </c>
     </row>
@@ -7189,7 +9499,7 @@
         <v>1.0521983177585015E-2</v>
       </c>
       <c r="J52">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>4.7992810111035511E-3</v>
       </c>
     </row>
@@ -7206,7 +9516,7 @@
         <v>8.5819042135779934E-4</v>
       </c>
       <c r="J53">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>2.7440462030560494E-3</v>
       </c>
     </row>
@@ -7223,7 +9533,7 @@
         <v>-3.0420048077298145E-4</v>
       </c>
       <c r="J54">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>2.0530929815953114E-3</v>
       </c>
     </row>
@@ -7240,7 +9550,7 @@
         <v>-2.2198485720784922E-3</v>
       </c>
       <c r="J55">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>1.3255786036606015E-3</v>
       </c>
     </row>
@@ -7257,7 +9567,7 @@
         <v>-8.4667213778500186E-5</v>
       </c>
       <c r="J56">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>4.2032324920247008E-4</v>
       </c>
     </row>
@@ -7274,7 +9584,7 @@
         <v>-5.6887139391960106E-3</v>
       </c>
       <c r="J57">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>-2.7215386688995286E-4</v>
       </c>
     </row>
@@ -7291,7 +9601,7 @@
         <v>-1.6098497560477001E-3</v>
       </c>
       <c r="J58">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>-8.6090460607114987E-4</v>
       </c>
     </row>
@@ -7308,7 +9618,7 @@
         <v>-2.7811873463538944E-3</v>
       </c>
       <c r="J59">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>-1.4842240355961468E-3</v>
       </c>
     </row>
@@ -7325,7 +9635,7 @@
         <v>-2.6392551038817991E-3</v>
       </c>
       <c r="J60">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>-2.6928150138243005E-3</v>
       </c>
     </row>
@@ -7342,7 +9652,7 @@
         <v>-5.5950706963108984E-3</v>
       </c>
       <c r="J61">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>-4.1096917282433497E-3</v>
       </c>
     </row>
@@ -7359,7 +9669,7 @@
         <v>-8.1575177016604966E-3</v>
       </c>
       <c r="J62">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>-6.5040627559118484E-3</v>
       </c>
     </row>
@@ -7376,7 +9686,7 @@
         <v>-7.9798133784400038E-3</v>
       </c>
       <c r="J63">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>-7.1359477316770142E-3</v>
       </c>
     </row>
@@ -7393,7 +9703,7 @@
         <v>-6.5150882588398018E-2</v>
       </c>
       <c r="J64">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>-1.3950190982223012E-2</v>
       </c>
     </row>
@@ -7410,7 +9720,7 @@
         <v>-1.84446619943653E-2</v>
       </c>
       <c r="J65">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>-1.836982139057735E-2</v>
       </c>
     </row>
@@ -7427,7 +9737,7 @@
         <v>-8.0751475362517006E-2</v>
       </c>
       <c r="J66">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>-6.1718467600211505E-2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated figures for the PhD meeting. These are getting really close - just need updated with more subjects.
</commit_message>
<xml_diff>
--- a/combiningMuscleGroups_metabolics.xlsx
+++ b/combiningMuscleGroups_metabolics.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Shared drives\Exotendon\muscleModel\muscleEnergyModel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F67046CD-9F96-487D-B893-A2CF94F87329}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9DFE9A8-D2A5-4512-AD9A-D182C20A95F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3435" yWindow="2850" windowWidth="21600" windowHeight="11385" firstSheet="1" activeTab="1" xr2:uid="{CE15F475-ED09-4E78-B0C4-C13E019F565F}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="1" xr2:uid="{CE15F475-ED09-4E78-B0C4-C13E019F565F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1 - full" sheetId="2" r:id="rId1"/>
@@ -4447,7 +4447,7 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="7"/>
                   <c:pt idx="0">
-                    <c:v>2.9330352479636264</c:v>
+                    <c:v>2.9330352479636299</c:v>
                   </c:pt>
                   <c:pt idx="1">
                     <c:v>7.9926370022359494</c:v>
@@ -4477,7 +4477,7 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="7"/>
                   <c:pt idx="0">
-                    <c:v>2.9330352479636264</c:v>
+                    <c:v>2.9330352479636299</c:v>
                   </c:pt>
                   <c:pt idx="1">
                     <c:v>7.9926370022359494</c:v>
@@ -4724,12 +4724,7 @@
         <c:majorGridlines>
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
+              <a:noFill/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -13313,8 +13308,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB7901D6-903F-4996-A78B-1108649D94A1}">
   <dimension ref="A1:AC66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R31" zoomScale="72" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AM78" sqref="AM78"/>
+    <sheetView tabSelected="1" topLeftCell="AC40" zoomScale="72" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AA31" sqref="AA31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15666,7 +15661,7 @@
         <v>-16.298716740306375</v>
       </c>
       <c r="AA42">
-        <v>2.9330352479636264</v>
+        <v>2.9330352479636299</v>
       </c>
       <c r="AB42">
         <v>4.1479382265884945</v>

</xml_diff>

<commit_message>
Updated files from the weird corrupted github issues.
</commit_message>
<xml_diff>
--- a/combiningMuscleGroups_metabolics.xlsx
+++ b/combiningMuscleGroups_metabolics.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Shared drives\Exotendon\muscleModel\muscleEnergyModel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9DFE9A8-D2A5-4512-AD9A-D182C20A95F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABC862BF-44B5-4FA1-B62D-D7A937A3647B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="1" xr2:uid="{CE15F475-ED09-4E78-B0C4-C13E019F565F}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CE15F475-ED09-4E78-B0C4-C13E019F565F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1 - full" sheetId="2" r:id="rId1"/>
@@ -10552,7 +10552,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{730AE58A-BFCC-47A5-850F-F7F52B044D8D}">
   <dimension ref="A1:S66"/>
   <sheetViews>
-    <sheetView zoomScale="54" zoomScaleNormal="40" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="54" zoomScaleNormal="40" workbookViewId="0">
       <selection activeCell="R39" sqref="R39:R53"/>
     </sheetView>
   </sheetViews>
@@ -13308,7 +13308,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB7901D6-903F-4996-A78B-1108649D94A1}">
   <dimension ref="A1:AC66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AC40" zoomScale="72" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="AC40" zoomScale="72" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="AA31" sqref="AA31"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
just updates and changes as I have been working on the paper
</commit_message>
<xml_diff>
--- a/combiningMuscleGroups_metabolics.xlsx
+++ b/combiningMuscleGroups_metabolics.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20392"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Shared drives\Exotendon\muscleModel\muscleEnergyModel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9F98DCE-2E74-4A1B-9792-7ED179FFCB87}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88E16CE3-7897-40EF-BBFF-57193C248EC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="28920" windowHeight="12345" activeTab="2" xr2:uid="{CE15F475-ED09-4E78-B0C4-C13E019F565F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{CE15F475-ED09-4E78-B0C4-C13E019F565F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2 - abbrev" sheetId="1" r:id="rId1"/>
@@ -26,12 +26,23 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1767" uniqueCount="278">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1767" uniqueCount="279">
   <si>
     <t>'metabolics_combined_addbrev_r_TOTAL'</t>
   </si>
@@ -905,6 +916,9 @@
   <si>
     <t>normal</t>
   </si>
+  <si>
+    <t>gmed total</t>
+  </si>
 </sst>
 </file>
 
@@ -1216,7 +1230,7 @@
     <xf numFmtId="0" fontId="4" fillId="12" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -1236,11 +1250,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="12" borderId="3" xfId="2"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="11" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="11" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1259,10 +1268,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Calculation" xfId="2" builtinId="22"/>
@@ -45691,7 +45698,7 @@
       </c>
       <c r="AU40">
         <f t="shared" ref="AU40:AU53" si="114">_xlfn.STDEV.P(AL40:AM40)/SQRT(2)</f>
-        <v>4.0546702106952957</v>
+        <v>4.0546702106952965</v>
       </c>
       <c r="AV40">
         <f t="shared" si="110"/>
@@ -48462,8 +48469,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E51E147-5B7E-4DEB-BD87-6908B3B49696}">
   <dimension ref="A1:CL267"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BT1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="CA47" sqref="CA47"/>
+    <sheetView tabSelected="1" topLeftCell="A226" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J267" sqref="J267"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -48721,38 +48728,38 @@
       <c r="BO2" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="BQ2" s="18" t="s">
+      <c r="BQ2" s="15" t="s">
         <v>219</v>
       </c>
-      <c r="BR2" s="18"/>
-      <c r="BS2" s="18"/>
-      <c r="BT2" s="18" t="s">
+      <c r="BR2" s="15"/>
+      <c r="BS2" s="15"/>
+      <c r="BT2" s="15" t="s">
         <v>89</v>
       </c>
-      <c r="BU2" s="18"/>
-      <c r="BV2" s="18"/>
+      <c r="BU2" s="15"/>
+      <c r="BV2" s="15"/>
       <c r="BX2" t="s">
         <v>40</v>
       </c>
-      <c r="BY2" s="36" t="s">
+      <c r="BY2" s="32" t="s">
         <v>42</v>
       </c>
-      <c r="BZ2" s="36" t="s">
+      <c r="BZ2" s="32" t="s">
         <v>41</v>
       </c>
-      <c r="CA2" s="36" t="s">
+      <c r="CA2" s="32" t="s">
         <v>118</v>
       </c>
-      <c r="CB2" s="36" t="s">
+      <c r="CB2" s="32" t="s">
         <v>120</v>
       </c>
-      <c r="CC2" s="36" t="s">
+      <c r="CC2" s="32" t="s">
         <v>121</v>
       </c>
-      <c r="CD2" s="36" t="s">
+      <c r="CD2" s="32" t="s">
         <v>122</v>
       </c>
-      <c r="CE2" s="36" t="s">
+      <c r="CE2" s="32" t="s">
         <v>123</v>
       </c>
       <c r="CF2" t="s">
@@ -49000,38 +49007,38 @@
         <f t="shared" si="2"/>
         <v>0.38421210654356913</v>
       </c>
-      <c r="BQ3" s="18" t="s">
+      <c r="BQ3" s="15" t="s">
         <v>189</v>
       </c>
-      <c r="BR3" s="18"/>
-      <c r="BS3" s="18"/>
-      <c r="BT3" s="18" t="s">
+      <c r="BR3" s="15"/>
+      <c r="BS3" s="15"/>
+      <c r="BT3" s="15" t="s">
         <v>189</v>
       </c>
-      <c r="BU3" s="18"/>
-      <c r="BV3" s="18"/>
+      <c r="BU3" s="15"/>
+      <c r="BV3" s="15"/>
       <c r="BX3" t="s">
         <v>81</v>
       </c>
-      <c r="BY3" s="36">
+      <c r="BY3" s="32">
         <v>0.29409495082989451</v>
       </c>
-      <c r="BZ3" s="36">
+      <c r="BZ3" s="32">
         <v>0.27905160716980709</v>
       </c>
-      <c r="CA3" s="36">
+      <c r="CA3" s="32">
         <v>0.3624346617686488</v>
       </c>
-      <c r="CB3" s="36">
+      <c r="CB3" s="32">
         <v>0.34734727680012056</v>
       </c>
-      <c r="CC3" s="36">
+      <c r="CC3" s="32">
         <v>0.46424271431240732</v>
       </c>
-      <c r="CD3" s="36">
+      <c r="CD3" s="32">
         <v>0.5867294682501053</v>
       </c>
-      <c r="CE3" s="36">
+      <c r="CE3" s="32">
         <v>0.40357896540465549</v>
       </c>
       <c r="CF3">
@@ -49279,34 +49286,34 @@
         <f t="shared" si="2"/>
         <v>0.42169270058480124</v>
       </c>
-      <c r="BQ4" s="18"/>
-      <c r="BR4" s="18"/>
-      <c r="BS4" s="18"/>
-      <c r="BT4" s="18"/>
-      <c r="BU4" s="18"/>
-      <c r="BV4" s="18"/>
+      <c r="BQ4" s="15"/>
+      <c r="BR4" s="15"/>
+      <c r="BS4" s="15"/>
+      <c r="BT4" s="15"/>
+      <c r="BU4" s="15"/>
+      <c r="BV4" s="15"/>
       <c r="BX4" t="s">
         <v>77</v>
       </c>
-      <c r="BY4" s="36">
+      <c r="BY4" s="32">
         <v>0.31078908559959711</v>
       </c>
-      <c r="BZ4" s="36">
+      <c r="BZ4" s="32">
         <v>0.32815028097230969</v>
       </c>
-      <c r="CA4" s="36">
+      <c r="CA4" s="32">
         <v>0.44792458568924642</v>
       </c>
-      <c r="CB4" s="36">
+      <c r="CB4" s="32">
         <v>0.41776032228169607</v>
       </c>
-      <c r="CC4" s="36">
+      <c r="CC4" s="32">
         <v>0.49333433852181396</v>
       </c>
-      <c r="CD4" s="36">
+      <c r="CD4" s="32">
         <v>0.5248493496394635</v>
       </c>
-      <c r="CE4" s="36">
+      <c r="CE4" s="32">
         <v>0.37336724589213921</v>
       </c>
       <c r="CF4">
@@ -49554,42 +49561,42 @@
         <f t="shared" si="2"/>
         <v>0.8178398762913176</v>
       </c>
-      <c r="BQ5" s="19"/>
-      <c r="BR5" s="19" t="s">
+      <c r="BQ5" s="16"/>
+      <c r="BR5" s="16" t="s">
         <v>190</v>
       </c>
-      <c r="BS5" s="19" t="s">
+      <c r="BS5" s="16" t="s">
         <v>191</v>
       </c>
-      <c r="BT5" s="19"/>
-      <c r="BU5" s="19" t="s">
+      <c r="BT5" s="16"/>
+      <c r="BU5" s="16" t="s">
         <v>190</v>
       </c>
-      <c r="BV5" s="19" t="s">
+      <c r="BV5" s="16" t="s">
         <v>191</v>
       </c>
       <c r="BX5" t="s">
         <v>78</v>
       </c>
-      <c r="BY5" s="36">
+      <c r="BY5" s="32">
         <v>0.95308205611647612</v>
       </c>
-      <c r="BZ5" s="36">
+      <c r="BZ5" s="32">
         <v>1.357661446942092</v>
       </c>
-      <c r="CA5" s="36">
+      <c r="CA5" s="32">
         <v>0.84157298310802697</v>
       </c>
-      <c r="CB5" s="36">
+      <c r="CB5" s="32">
         <v>0.8627526116126466</v>
       </c>
-      <c r="CC5" s="36">
+      <c r="CC5" s="32">
         <v>0.92456235461897618</v>
       </c>
-      <c r="CD5" s="36">
+      <c r="CD5" s="32">
         <v>1.2624334646721922</v>
       </c>
-      <c r="CE5" s="36">
+      <c r="CE5" s="32">
         <v>1.1281060168838908</v>
       </c>
       <c r="CF5">
@@ -49837,46 +49844,46 @@
         <f t="shared" si="9"/>
         <v>0.28104070564762951</v>
       </c>
-      <c r="BQ6" s="20" t="s">
+      <c r="BQ6" s="17" t="s">
         <v>192</v>
       </c>
-      <c r="BR6" s="20">
+      <c r="BR6" s="17">
         <v>0.92198999276578064</v>
       </c>
-      <c r="BS6" s="20">
+      <c r="BS6" s="17">
         <v>0.77990892714599613</v>
       </c>
-      <c r="BT6" s="20" t="s">
+      <c r="BT6" s="17" t="s">
         <v>192</v>
       </c>
-      <c r="BU6" s="20">
+      <c r="BU6" s="17">
         <v>0.39106852064794839</v>
       </c>
-      <c r="BV6" s="20">
+      <c r="BV6" s="17">
         <v>0.32619228223745361</v>
       </c>
       <c r="BX6" t="s">
         <v>79</v>
       </c>
-      <c r="BY6" s="36">
+      <c r="BY6" s="32">
         <v>0.493632085920436</v>
       </c>
-      <c r="BZ6" s="36">
+      <c r="BZ6" s="32">
         <v>0.45650821448054818</v>
       </c>
-      <c r="CA6" s="36">
+      <c r="CA6" s="32">
         <v>0.66720643952170211</v>
       </c>
-      <c r="CB6" s="36">
+      <c r="CB6" s="32">
         <v>0.61458954797457732</v>
       </c>
-      <c r="CC6" s="36">
+      <c r="CC6" s="32">
         <v>0.52196510298117071</v>
       </c>
-      <c r="CD6" s="36">
+      <c r="CD6" s="32">
         <v>0.69143986827438797</v>
       </c>
-      <c r="CE6" s="36">
+      <c r="CE6" s="32">
         <v>0.45954237281404886</v>
       </c>
       <c r="CF6">
@@ -50124,46 +50131,46 @@
         <f t="shared" si="9"/>
         <v>0.91061511553776331</v>
       </c>
-      <c r="BQ7" s="20" t="s">
+      <c r="BQ7" s="17" t="s">
         <v>193</v>
       </c>
-      <c r="BR7" s="20">
+      <c r="BR7" s="17">
         <v>8.9908965492463185E-3</v>
       </c>
-      <c r="BS7" s="20">
+      <c r="BS7" s="17">
         <v>1.2562611439310848E-2</v>
       </c>
-      <c r="BT7" s="20" t="s">
+      <c r="BT7" s="17" t="s">
         <v>193</v>
       </c>
-      <c r="BU7" s="20">
+      <c r="BU7" s="17">
         <v>1.1412881241562664E-2</v>
       </c>
-      <c r="BV7" s="20">
+      <c r="BV7" s="17">
         <v>9.9240380553326877E-3</v>
       </c>
       <c r="BX7" t="s">
         <v>80</v>
       </c>
-      <c r="BY7" s="36">
+      <c r="BY7" s="32">
         <v>1.0430407317682979</v>
       </c>
-      <c r="BZ7" s="36">
+      <c r="BZ7" s="32">
         <v>0.92587196123325066</v>
       </c>
-      <c r="CA7" s="36">
+      <c r="CA7" s="32">
         <v>1.0936301894812519</v>
       </c>
-      <c r="CB7" s="36">
+      <c r="CB7" s="32">
         <v>1.0687936058597209</v>
       </c>
-      <c r="CC7" s="36">
+      <c r="CC7" s="32">
         <v>1.2216157021422631</v>
       </c>
-      <c r="CD7" s="36">
+      <c r="CD7" s="32">
         <v>1.227301830125106</v>
       </c>
-      <c r="CE7" s="36">
+      <c r="CE7" s="32">
         <v>1.0595519595804532</v>
       </c>
       <c r="CF7">
@@ -50411,46 +50418,46 @@
         <f t="shared" si="9"/>
         <v>0.91387559424645315</v>
       </c>
-      <c r="BQ8" s="20" t="s">
+      <c r="BQ8" s="17" t="s">
         <v>194</v>
       </c>
-      <c r="BR8" s="20">
+      <c r="BR8" s="17">
         <v>7</v>
       </c>
-      <c r="BS8" s="20">
+      <c r="BS8" s="17">
         <v>7</v>
       </c>
-      <c r="BT8" s="20" t="s">
+      <c r="BT8" s="17" t="s">
         <v>194</v>
       </c>
-      <c r="BU8" s="20">
+      <c r="BU8" s="17">
         <v>7</v>
       </c>
-      <c r="BV8" s="20">
+      <c r="BV8" s="17">
         <v>7</v>
       </c>
       <c r="BX8" t="s">
         <v>82</v>
       </c>
-      <c r="BY8" s="36">
+      <c r="BY8" s="32">
         <v>0.74393149274886039</v>
       </c>
-      <c r="BZ8" s="36">
+      <c r="BZ8" s="32">
         <v>0.83549716832213827</v>
       </c>
-      <c r="CA8" s="36">
+      <c r="CA8" s="32">
         <v>1.1369611832066382</v>
       </c>
-      <c r="CB8" s="36">
+      <c r="CB8" s="32">
         <v>0.80609312317786541</v>
       </c>
-      <c r="CC8" s="36">
+      <c r="CC8" s="32">
         <v>1.0998937228535808</v>
       </c>
-      <c r="CD8" s="36">
+      <c r="CD8" s="32">
         <v>0.86465057394214517</v>
       </c>
-      <c r="CE8" s="36">
+      <c r="CE8" s="32">
         <v>1.0112364878534665</v>
       </c>
       <c r="CF8">
@@ -50698,42 +50705,42 @@
         <f t="shared" si="12"/>
         <v>0.91565442322158774</v>
       </c>
-      <c r="BQ9" s="20" t="s">
+      <c r="BQ9" s="17" t="s">
         <v>195</v>
       </c>
-      <c r="BR9" s="20">
+      <c r="BR9" s="17">
         <v>0.74474500892037721</v>
       </c>
-      <c r="BS9" s="20"/>
-      <c r="BT9" s="20" t="s">
+      <c r="BS9" s="17"/>
+      <c r="BT9" s="17" t="s">
         <v>195</v>
       </c>
-      <c r="BU9" s="20">
+      <c r="BU9" s="17">
         <v>0.96125717822032464</v>
       </c>
-      <c r="BV9" s="20"/>
+      <c r="BV9" s="17"/>
       <c r="BX9" t="s">
         <v>117</v>
       </c>
-      <c r="BY9" s="36">
+      <c r="BY9" s="32">
         <v>0.8296299267459768</v>
       </c>
-      <c r="BZ9" s="36">
+      <c r="BZ9" s="32">
         <v>0.7617169773353758</v>
       </c>
-      <c r="CA9" s="36">
+      <c r="CA9" s="32">
         <v>0.97285885300363917</v>
       </c>
-      <c r="CB9" s="36">
+      <c r="CB9" s="32">
         <v>0.91657144065027163</v>
       </c>
-      <c r="CC9" s="36">
+      <c r="CC9" s="32">
         <v>0.9915772747932905</v>
       </c>
-      <c r="CD9" s="36">
+      <c r="CD9" s="32">
         <v>0.95335842541701754</v>
       </c>
-      <c r="CE9" s="36">
+      <c r="CE9" s="32">
         <v>1.0282170514148929</v>
       </c>
       <c r="CF9">
@@ -50922,20 +50929,20 @@
         <f>SUM(AE21,AE29:AE31)</f>
         <v>0.91061511553776331</v>
       </c>
-      <c r="BQ10" s="20" t="s">
+      <c r="BQ10" s="17" t="s">
         <v>196</v>
       </c>
-      <c r="BR10" s="20">
+      <c r="BR10" s="17">
         <v>0</v>
       </c>
-      <c r="BS10" s="20"/>
-      <c r="BT10" s="20" t="s">
+      <c r="BS10" s="17"/>
+      <c r="BT10" s="17" t="s">
         <v>196</v>
       </c>
-      <c r="BU10" s="20">
+      <c r="BU10" s="17">
         <v>0</v>
       </c>
-      <c r="BV10" s="20"/>
+      <c r="BV10" s="17"/>
     </row>
     <row r="11" spans="1:90" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -51131,20 +51138,20 @@
       <c r="BJ11" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="BQ11" s="20" t="s">
+      <c r="BQ11" s="17" t="s">
         <v>197</v>
       </c>
-      <c r="BR11" s="20">
+      <c r="BR11" s="17">
         <v>6</v>
       </c>
-      <c r="BS11" s="20"/>
-      <c r="BT11" s="20" t="s">
+      <c r="BS11" s="17"/>
+      <c r="BT11" s="17" t="s">
         <v>197</v>
       </c>
-      <c r="BU11" s="20">
+      <c r="BU11" s="17">
         <v>6</v>
       </c>
-      <c r="BV11" s="20"/>
+      <c r="BV11" s="17"/>
     </row>
     <row r="12" spans="1:90" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -51283,20 +51290,20 @@
         <f>(BI12-BI13)/BI13*100</f>
         <v>-12.108950005295792</v>
       </c>
-      <c r="BQ12" s="20" t="s">
+      <c r="BQ12" s="17" t="s">
         <v>198</v>
       </c>
-      <c r="BR12" s="20">
+      <c r="BR12" s="17">
         <v>4.9687999899115063</v>
       </c>
-      <c r="BS12" s="20"/>
-      <c r="BT12" s="20" t="s">
+      <c r="BS12" s="17"/>
+      <c r="BT12" s="17" t="s">
         <v>198</v>
       </c>
-      <c r="BU12" s="20">
+      <c r="BU12" s="17">
         <v>5.7972602192050431</v>
       </c>
-      <c r="BV12" s="20"/>
+      <c r="BV12" s="17"/>
     </row>
     <row r="13" spans="1:90" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
@@ -51431,20 +51438,20 @@
         <f>AVERAGE(BB13:BH13)</f>
         <v>11.623109642857145</v>
       </c>
-      <c r="BQ13" s="20" t="s">
+      <c r="BQ13" s="17" t="s">
         <v>199</v>
       </c>
-      <c r="BR13" s="20">
+      <c r="BR13" s="17">
         <v>1.2649408377270984E-3</v>
       </c>
-      <c r="BS13" s="20"/>
-      <c r="BT13" s="20" t="s">
+      <c r="BS13" s="17"/>
+      <c r="BT13" s="17" t="s">
         <v>199</v>
       </c>
-      <c r="BU13" s="20">
+      <c r="BU13" s="17">
         <v>5.7713893854538338E-4</v>
       </c>
-      <c r="BV13" s="20"/>
+      <c r="BV13" s="17"/>
     </row>
     <row r="14" spans="1:90" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -51551,20 +51558,20 @@
         <f t="shared" si="17"/>
         <v>0.58255327614279395</v>
       </c>
-      <c r="BQ14" s="20" t="s">
+      <c r="BQ14" s="17" t="s">
         <v>200</v>
       </c>
-      <c r="BR14" s="20">
+      <c r="BR14" s="17">
         <v>1.9431802805153031</v>
       </c>
-      <c r="BS14" s="20"/>
-      <c r="BT14" s="20" t="s">
+      <c r="BS14" s="17"/>
+      <c r="BT14" s="17" t="s">
         <v>200</v>
       </c>
-      <c r="BU14" s="20">
+      <c r="BU14" s="17">
         <v>1.9431802805153031</v>
       </c>
-      <c r="BV14" s="20"/>
+      <c r="BV14" s="17"/>
     </row>
     <row r="15" spans="1:90" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
@@ -51671,20 +51678,20 @@
         <f t="shared" si="18"/>
         <v>0.126103855207302</v>
       </c>
-      <c r="BQ15" s="20" t="s">
+      <c r="BQ15" s="17" t="s">
         <v>201</v>
       </c>
-      <c r="BR15" s="20">
+      <c r="BR15" s="17">
         <v>2.5298816754541968E-3</v>
       </c>
-      <c r="BS15" s="20"/>
-      <c r="BT15" s="20" t="s">
+      <c r="BS15" s="17"/>
+      <c r="BT15" s="17" t="s">
         <v>201</v>
       </c>
-      <c r="BU15" s="20">
+      <c r="BU15" s="17">
         <v>1.1542778770907668E-3</v>
       </c>
-      <c r="BV15" s="20"/>
+      <c r="BV15" s="17"/>
     </row>
     <row r="16" spans="1:90" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
@@ -51797,20 +51804,20 @@
       <c r="BC16" t="s">
         <v>216</v>
       </c>
-      <c r="BQ16" s="21" t="s">
+      <c r="BQ16" s="18" t="s">
         <v>202</v>
       </c>
-      <c r="BR16" s="21">
+      <c r="BR16" s="18">
         <v>2.4469118511449697</v>
       </c>
-      <c r="BS16" s="21"/>
-      <c r="BT16" s="21" t="s">
+      <c r="BS16" s="18"/>
+      <c r="BT16" s="18" t="s">
         <v>202</v>
       </c>
-      <c r="BU16" s="21">
+      <c r="BU16" s="18">
         <v>2.4469118511449697</v>
       </c>
-      <c r="BV16" s="21"/>
+      <c r="BV16" s="18"/>
     </row>
     <row r="17" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
@@ -51992,9 +51999,9 @@
       <c r="BN17" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="BQ17" s="18"/>
-      <c r="BR17" s="18"/>
-      <c r="BS17" s="18"/>
+      <c r="BQ17" s="15"/>
+      <c r="BR17" s="15"/>
+      <c r="BS17" s="15"/>
     </row>
     <row r="18" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
@@ -52189,9 +52196,9 @@
       <c r="BN18">
         <v>9.4568924999999986</v>
       </c>
-      <c r="BQ18" s="18"/>
-      <c r="BR18" s="18"/>
-      <c r="BS18" s="18"/>
+      <c r="BQ18" s="15"/>
+      <c r="BR18" s="15"/>
+      <c r="BS18" s="15"/>
     </row>
     <row r="19" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
@@ -52386,11 +52393,11 @@
       <c r="BN19">
         <v>10.59634625</v>
       </c>
-      <c r="BQ19" s="18" t="s">
+      <c r="BQ19" s="15" t="s">
         <v>93</v>
       </c>
-      <c r="BR19" s="18"/>
-      <c r="BS19" s="18"/>
+      <c r="BR19" s="15"/>
+      <c r="BS19" s="15"/>
       <c r="BT19" s="1" t="s">
         <v>220</v>
       </c>
@@ -52588,11 +52595,11 @@
       <c r="BN20">
         <v>10.58502125</v>
       </c>
-      <c r="BQ20" s="18" t="s">
+      <c r="BQ20" s="15" t="s">
         <v>189</v>
       </c>
-      <c r="BR20" s="18"/>
-      <c r="BS20" s="18"/>
+      <c r="BR20" s="15"/>
+      <c r="BS20" s="15"/>
       <c r="BT20" t="s">
         <v>189</v>
       </c>
@@ -52790,9 +52797,9 @@
       <c r="BN21">
         <v>11.887410750000001</v>
       </c>
-      <c r="BQ21" s="18"/>
-      <c r="BR21" s="18"/>
-      <c r="BS21" s="18"/>
+      <c r="BQ21" s="15"/>
+      <c r="BR21" s="15"/>
+      <c r="BS21" s="15"/>
     </row>
     <row r="22" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
@@ -52987,18 +52994,18 @@
       <c r="BN22">
         <v>10.260292750000001</v>
       </c>
-      <c r="BQ22" s="19"/>
-      <c r="BR22" s="19" t="s">
+      <c r="BQ22" s="16"/>
+      <c r="BR22" s="16" t="s">
         <v>190</v>
       </c>
-      <c r="BS22" s="19" t="s">
+      <c r="BS22" s="16" t="s">
         <v>191</v>
       </c>
-      <c r="BT22" s="17"/>
-      <c r="BU22" s="17" t="s">
+      <c r="BT22" s="13"/>
+      <c r="BU22" s="13" t="s">
         <v>190</v>
       </c>
-      <c r="BV22" s="17" t="s">
+      <c r="BV22" s="13" t="s">
         <v>191</v>
       </c>
     </row>
@@ -53195,28 +53202,28 @@
       <c r="BN23">
         <v>10.952586750000002</v>
       </c>
-      <c r="BQ23" s="20" t="s">
+      <c r="BQ23" s="17" t="s">
         <v>192</v>
       </c>
-      <c r="BR23" s="20">
+      <c r="BR23" s="17">
         <v>1.0914008543129063</v>
       </c>
-      <c r="BS23" s="20">
+      <c r="BS23" s="17">
         <v>0.95602069896096575</v>
       </c>
-      <c r="BT23" s="15" t="s">
+      <c r="BT23" t="s">
         <v>192</v>
       </c>
-      <c r="BU23" s="15">
+      <c r="BU23">
         <v>1.0471672762791857</v>
       </c>
-      <c r="BV23" s="15">
+      <c r="BV23">
         <v>1.0560878527338382</v>
       </c>
-      <c r="BX23" s="22" t="s">
+      <c r="BX23" s="19" t="s">
         <v>251</v>
       </c>
-      <c r="BZ23" s="23" t="s">
+      <c r="BZ23" s="20" t="s">
         <v>252</v>
       </c>
     </row>
@@ -53413,25 +53420,25 @@
       <c r="BN24">
         <v>9.7877445000000005</v>
       </c>
-      <c r="BQ24" s="20" t="s">
+      <c r="BQ24" s="17" t="s">
         <v>193</v>
       </c>
-      <c r="BR24" s="20">
+      <c r="BR24" s="17">
         <v>1.1115651238705332E-2</v>
       </c>
-      <c r="BS24" s="20">
+      <c r="BS24" s="17">
         <v>1.214409674108167E-2</v>
       </c>
-      <c r="BT24" s="15" t="s">
+      <c r="BT24" t="s">
         <v>193</v>
       </c>
-      <c r="BU24" s="15">
+      <c r="BU24">
         <v>4.1576503168094948E-2</v>
       </c>
-      <c r="BV24" s="15">
+      <c r="BV24">
         <v>4.5308432836812962E-2</v>
       </c>
-      <c r="BZ24" s="23" t="s">
+      <c r="BZ24" s="20" t="s">
         <v>253</v>
       </c>
     </row>
@@ -53585,34 +53592,34 @@
       <c r="BN25">
         <v>10.429017250000001</v>
       </c>
-      <c r="BQ25" s="20" t="s">
+      <c r="BQ25" s="17" t="s">
         <v>194</v>
       </c>
-      <c r="BR25" s="20">
+      <c r="BR25" s="17">
         <v>7</v>
       </c>
-      <c r="BS25" s="20">
+      <c r="BS25" s="17">
         <v>7</v>
       </c>
-      <c r="BT25" s="15" t="s">
+      <c r="BT25" t="s">
         <v>194</v>
       </c>
-      <c r="BU25" s="15">
+      <c r="BU25">
         <v>7</v>
       </c>
-      <c r="BV25" s="15">
+      <c r="BV25">
         <v>7</v>
       </c>
-      <c r="BX25" s="22" t="s">
+      <c r="BX25" s="19" t="s">
         <v>254</v>
       </c>
-      <c r="BY25" s="22" t="s">
+      <c r="BY25" s="19" t="s">
         <v>255</v>
       </c>
-      <c r="CA25" s="22" t="s">
+      <c r="CA25" s="19" t="s">
         <v>256</v>
       </c>
-      <c r="CB25" s="24">
+      <c r="CB25" s="21">
         <v>7</v>
       </c>
     </row>
@@ -53766,20 +53773,19 @@
       <c r="BN26">
         <v>8.8028642500000007</v>
       </c>
-      <c r="BQ26" s="20" t="s">
+      <c r="BQ26" s="17" t="s">
         <v>195</v>
       </c>
-      <c r="BR26" s="20">
+      <c r="BR26" s="17">
         <v>0.46784395628384567</v>
       </c>
-      <c r="BS26" s="20"/>
-      <c r="BT26" s="15" t="s">
+      <c r="BS26" s="17"/>
+      <c r="BT26" t="s">
         <v>195</v>
       </c>
-      <c r="BU26" s="15">
+      <c r="BU26">
         <v>0.4243213621379609</v>
       </c>
-      <c r="BV26" s="15"/>
       <c r="BY26">
         <v>0.60087976039069524</v>
       </c>
@@ -53901,37 +53907,36 @@
       <c r="BN27">
         <v>10.962691500000002</v>
       </c>
-      <c r="BQ27" s="20" t="s">
+      <c r="BQ27" s="17" t="s">
         <v>196</v>
       </c>
-      <c r="BR27" s="20">
+      <c r="BR27" s="17">
         <v>0</v>
       </c>
-      <c r="BS27" s="20"/>
-      <c r="BT27" s="15" t="s">
+      <c r="BS27" s="17"/>
+      <c r="BT27" t="s">
         <v>196</v>
       </c>
-      <c r="BU27" s="15">
+      <c r="BU27">
         <v>0</v>
       </c>
-      <c r="BV27" s="15"/>
       <c r="BY27">
         <v>0.71457510001430524</v>
       </c>
-      <c r="CA27" s="22" t="s">
+      <c r="CA27" s="19" t="s">
         <v>259</v>
       </c>
-      <c r="CB27" s="25">
+      <c r="CB27" s="22">
         <v>0.62329999999999997</v>
       </c>
       <c r="CD27" t="s">
         <v>260</v>
       </c>
-      <c r="CE27" s="26">
+      <c r="CE27" s="23">
         <f>BY32-BY26</f>
         <v>0.3147746628308925</v>
       </c>
-      <c r="CF27" s="27">
+      <c r="CF27" s="24">
         <f>CE27*CB27</f>
         <v>0.1961990473424953</v>
       </c>
@@ -54047,37 +54052,36 @@
       <c r="BN28">
         <v>11.156119500000001</v>
       </c>
-      <c r="BQ28" s="20" t="s">
+      <c r="BQ28" s="17" t="s">
         <v>197</v>
       </c>
-      <c r="BR28" s="20">
+      <c r="BR28" s="17">
         <v>6</v>
       </c>
-      <c r="BS28" s="20"/>
-      <c r="BT28" s="15" t="s">
+      <c r="BS28" s="17"/>
+      <c r="BT28" t="s">
         <v>197</v>
       </c>
-      <c r="BU28" s="15">
+      <c r="BU28">
         <v>6</v>
       </c>
-      <c r="BV28" s="15"/>
       <c r="BY28">
         <v>0.72389039007990763</v>
       </c>
-      <c r="CA28" s="22" t="s">
+      <c r="CA28" s="19" t="s">
         <v>261</v>
       </c>
-      <c r="CB28" s="28">
+      <c r="CB28" s="25">
         <v>0.30309999999999998</v>
       </c>
       <c r="CD28" t="s">
         <v>262</v>
       </c>
-      <c r="CE28" s="29">
+      <c r="CE28" s="26">
         <f>BY31-BY27</f>
         <v>0.18668543836344387</v>
       </c>
-      <c r="CF28" s="30">
+      <c r="CF28" s="27">
         <f>CE28*CB28</f>
         <v>5.6584356367959832E-2</v>
       </c>
@@ -54199,37 +54203,36 @@
       <c r="BN29">
         <v>10.305246250000001</v>
       </c>
-      <c r="BQ29" s="20" t="s">
+      <c r="BQ29" s="17" t="s">
         <v>198</v>
       </c>
-      <c r="BR29" s="20">
+      <c r="BR29" s="17">
         <v>3.21806938356168</v>
       </c>
-      <c r="BS29" s="20"/>
-      <c r="BT29" s="15" t="s">
+      <c r="BS29" s="17"/>
+      <c r="BT29" t="s">
         <v>198</v>
       </c>
-      <c r="BU29" s="15">
+      <c r="BU29">
         <v>-0.10549502455611971</v>
       </c>
-      <c r="BV29" s="15"/>
       <c r="BY29">
         <v>0.77132022180161486</v>
       </c>
-      <c r="CA29" s="22" t="s">
+      <c r="CA29" s="19" t="s">
         <v>263</v>
       </c>
-      <c r="CB29" s="28">
+      <c r="CB29" s="25">
         <v>0.1401</v>
       </c>
       <c r="CD29" t="s">
         <v>264</v>
       </c>
-      <c r="CE29" s="29">
+      <c r="CE29" s="26">
         <f>BY30-BY28</f>
         <v>0.10789166605620548</v>
       </c>
-      <c r="CF29" s="30">
+      <c r="CF29" s="27">
         <f>CE29*CB29</f>
         <v>1.5115622414474388E-2</v>
       </c>
@@ -54421,27 +54424,26 @@
       <c r="BN30">
         <v>9.4641872500000002</v>
       </c>
-      <c r="BQ30" s="20" t="s">
+      <c r="BQ30" s="17" t="s">
         <v>199</v>
       </c>
-      <c r="BR30" s="20">
+      <c r="BR30" s="17">
         <v>9.0906572499629811E-3</v>
       </c>
-      <c r="BS30" s="20"/>
-      <c r="BT30" s="15" t="s">
+      <c r="BS30" s="17"/>
+      <c r="BT30" t="s">
         <v>199</v>
       </c>
-      <c r="BU30" s="15">
+      <c r="BU30">
         <v>0.45971075351065294</v>
       </c>
-      <c r="BV30" s="15"/>
       <c r="BY30">
         <v>0.83178205613611311</v>
       </c>
-      <c r="CA30" s="22"/>
-      <c r="CB30" s="31"/>
-      <c r="CE30" s="32"/>
-      <c r="CF30" s="33"/>
+      <c r="CA30" s="19"/>
+      <c r="CB30" s="28"/>
+      <c r="CE30" s="29"/>
+      <c r="CF30" s="30"/>
     </row>
     <row r="31" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
@@ -54643,20 +54645,19 @@
       <c r="BN31">
         <v>10.256770500000002</v>
       </c>
-      <c r="BQ31" s="20" t="s">
+      <c r="BQ31" s="17" t="s">
         <v>200</v>
       </c>
-      <c r="BR31" s="20">
+      <c r="BR31" s="17">
         <v>1.9431802805153031</v>
       </c>
-      <c r="BS31" s="20"/>
-      <c r="BT31" s="15" t="s">
+      <c r="BS31" s="17"/>
+      <c r="BT31" t="s">
         <v>200</v>
       </c>
-      <c r="BU31" s="15">
+      <c r="BU31">
         <v>1.9431802805153031</v>
       </c>
-      <c r="BV31" s="15"/>
       <c r="BY31">
         <v>0.90126053837774911</v>
       </c>
@@ -54806,20 +54807,19 @@
       <c r="BN32">
         <v>10.111613500000001</v>
       </c>
-      <c r="BQ32" s="20" t="s">
+      <c r="BQ32" s="17" t="s">
         <v>201</v>
       </c>
-      <c r="BR32" s="20">
+      <c r="BR32" s="17">
         <v>1.8181314499925962E-2</v>
       </c>
-      <c r="BS32" s="20"/>
-      <c r="BT32" s="15" t="s">
+      <c r="BS32" s="17"/>
+      <c r="BT32" t="s">
         <v>201</v>
       </c>
-      <c r="BU32" s="15">
+      <c r="BU32">
         <v>0.91942150702130587</v>
       </c>
-      <c r="BV32" s="15"/>
       <c r="BY32">
         <v>0.91565442322158774</v>
       </c>
@@ -54965,24 +54965,24 @@
       <c r="BN33">
         <v>11.580257500000002</v>
       </c>
-      <c r="BQ33" s="21" t="s">
+      <c r="BQ33" s="18" t="s">
         <v>202</v>
       </c>
-      <c r="BR33" s="21">
+      <c r="BR33" s="18">
         <v>2.4469118511449697</v>
       </c>
-      <c r="BS33" s="21"/>
-      <c r="BT33" s="16" t="s">
+      <c r="BS33" s="18"/>
+      <c r="BT33" s="12" t="s">
         <v>202</v>
       </c>
-      <c r="BU33" s="16">
+      <c r="BU33" s="12">
         <v>2.4469118511449697</v>
       </c>
-      <c r="BV33" s="16"/>
-      <c r="CA33" s="22" t="s">
+      <c r="BV33" s="12"/>
+      <c r="CA33" s="19" t="s">
         <v>265</v>
       </c>
-      <c r="CB33" s="25">
+      <c r="CB33" s="22">
         <f>DEVSQ(BY26:BY32)</f>
         <v>7.5375668635864632E-2</v>
       </c>
@@ -55128,13 +55128,13 @@
       <c r="BN34">
         <v>11.351310500000002</v>
       </c>
-      <c r="BQ34" s="18"/>
-      <c r="BR34" s="18"/>
-      <c r="BS34" s="18"/>
-      <c r="CA34" s="22" t="s">
+      <c r="BQ34" s="15"/>
+      <c r="BR34" s="15"/>
+      <c r="BS34" s="15"/>
+      <c r="CA34" s="19" t="s">
         <v>266</v>
       </c>
-      <c r="CB34" s="28">
+      <c r="CB34" s="25">
         <f>SUM(CF27:CF29)</f>
         <v>0.26789902612492955</v>
       </c>
@@ -55280,13 +55280,13 @@
       <c r="BN35">
         <v>12.40214525</v>
       </c>
-      <c r="BQ35" s="18"/>
-      <c r="BR35" s="18"/>
-      <c r="BS35" s="18"/>
-      <c r="CA35" s="22" t="s">
+      <c r="BQ35" s="15"/>
+      <c r="BR35" s="15"/>
+      <c r="BS35" s="15"/>
+      <c r="CA35" s="19" t="s">
         <v>267</v>
       </c>
-      <c r="CB35" s="28">
+      <c r="CB35" s="25">
         <f>(CB34^2)/CB33</f>
         <v>0.95216254127577615</v>
       </c>
@@ -55441,24 +55441,24 @@
       <c r="BN36">
         <v>10.934422250000001</v>
       </c>
-      <c r="BQ36" s="18" t="s">
+      <c r="BQ36" s="15" t="s">
         <v>88</v>
       </c>
-      <c r="BR36" s="18"/>
-      <c r="BS36" s="18"/>
+      <c r="BR36" s="15"/>
+      <c r="BS36" s="15"/>
       <c r="BT36" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="CA36" s="22">
+      <c r="CA36" s="19">
         <v>0.5</v>
       </c>
-      <c r="CB36" s="28">
+      <c r="CB36" s="25">
         <v>0.92800000000000005</v>
       </c>
-      <c r="CE36" s="22">
+      <c r="CE36" s="19">
         <v>0.5</v>
       </c>
-      <c r="CF36" s="28">
+      <c r="CF36" s="25">
         <v>0.92800000000000005</v>
       </c>
     </row>
@@ -55637,24 +55637,24 @@
       <c r="BN37">
         <v>13.319905250000001</v>
       </c>
-      <c r="BQ37" s="18" t="s">
+      <c r="BQ37" s="15" t="s">
         <v>189</v>
       </c>
-      <c r="BR37" s="18"/>
-      <c r="BS37" s="18"/>
+      <c r="BR37" s="15"/>
+      <c r="BS37" s="15"/>
       <c r="BT37" t="s">
         <v>189</v>
       </c>
-      <c r="CA37" s="22">
+      <c r="CA37" s="19">
         <v>0.9</v>
       </c>
-      <c r="CB37" s="28">
+      <c r="CB37" s="25">
         <v>0.97199999999999998</v>
       </c>
-      <c r="CE37" s="22">
+      <c r="CE37" s="19">
         <v>0.9</v>
       </c>
-      <c r="CF37" s="28">
+      <c r="CF37" s="25">
         <v>0.97199999999999998</v>
       </c>
     </row>
@@ -55782,13 +55782,13 @@
         <f t="shared" si="49"/>
         <v>#REF!</v>
       </c>
-      <c r="BQ38" s="18"/>
-      <c r="BR38" s="18"/>
-      <c r="BS38" s="18"/>
-      <c r="CA38" s="22" t="s">
+      <c r="BQ38" s="15"/>
+      <c r="BR38" s="15"/>
+      <c r="BS38" s="15"/>
+      <c r="CA38" s="19" t="s">
         <v>268</v>
       </c>
-      <c r="CB38" s="28">
+      <c r="CB38" s="25">
         <f>FORECAST(CB35,CA36:CA37,CB36:CB37)</f>
         <v>0.71965946614341991</v>
       </c>
@@ -55798,7 +55798,7 @@
       <c r="CE38">
         <v>0.95</v>
       </c>
-      <c r="CF38" s="37">
+      <c r="CF38">
         <v>0.97899999999999998</v>
       </c>
     </row>
@@ -55926,24 +55926,24 @@
         <f t="shared" si="49"/>
         <v>#REF!</v>
       </c>
-      <c r="BQ39" s="19"/>
-      <c r="BR39" s="19" t="s">
+      <c r="BQ39" s="16"/>
+      <c r="BR39" s="16" t="s">
         <v>190</v>
       </c>
-      <c r="BS39" s="19" t="s">
+      <c r="BS39" s="16" t="s">
         <v>191</v>
       </c>
-      <c r="BT39" s="17"/>
-      <c r="BU39" s="17" t="s">
+      <c r="BT39" s="13"/>
+      <c r="BU39" s="13" t="s">
         <v>190</v>
       </c>
-      <c r="BV39" s="17" t="s">
+      <c r="BV39" s="13" t="s">
         <v>191</v>
       </c>
-      <c r="CA39" s="22" t="s">
+      <c r="CA39" s="19" t="s">
         <v>270</v>
       </c>
-      <c r="CB39" s="28">
+      <c r="CB39" s="25">
         <v>0.05</v>
       </c>
       <c r="CC39" t="s">
@@ -55952,7 +55952,7 @@
       <c r="CE39">
         <v>0.98</v>
       </c>
-      <c r="CF39" s="37">
+      <c r="CF39">
         <v>0.98499999999999999</v>
       </c>
     </row>
@@ -56040,28 +56040,28 @@
       <c r="BA40" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="BQ40" s="20" t="s">
+      <c r="BQ40" s="17" t="s">
         <v>192</v>
       </c>
-      <c r="BR40" s="20">
+      <c r="BR40" s="17">
         <v>0.92832339315781354</v>
       </c>
-      <c r="BS40" s="20">
+      <c r="BS40" s="17">
         <v>0.81814696218532457</v>
       </c>
-      <c r="BT40" s="15" t="s">
+      <c r="BT40" t="s">
         <v>192</v>
       </c>
-      <c r="BU40" s="15">
+      <c r="BU40">
         <v>0.4137393155137522</v>
       </c>
-      <c r="BV40" s="15">
+      <c r="BV40">
         <v>0.44752026198074202</v>
       </c>
-      <c r="CA40" s="22" t="s">
+      <c r="CA40" s="19" t="s">
         <v>272</v>
       </c>
-      <c r="CB40" s="31" t="s">
+      <c r="CB40" s="28" t="s">
         <v>273</v>
       </c>
       <c r="CC40" t="s">
@@ -56070,7 +56070,7 @@
       <c r="CE40">
         <v>0.99</v>
       </c>
-      <c r="CF40" s="37">
+      <c r="CF40">
         <v>0.98799999999999999</v>
       </c>
     </row>
@@ -56191,27 +56191,27 @@
       <c r="BM41" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="BQ41" s="20" t="s">
+      <c r="BQ41" s="17" t="s">
         <v>193</v>
       </c>
-      <c r="BR41" s="20">
+      <c r="BR41" s="17">
         <v>2.3575372416715368E-2</v>
       </c>
-      <c r="BS41" s="20">
+      <c r="BS41" s="17">
         <v>2.7352488264559643E-2</v>
       </c>
-      <c r="BT41" s="15" t="s">
+      <c r="BT41" t="s">
         <v>193</v>
       </c>
-      <c r="BU41" s="15">
+      <c r="BU41">
         <v>6.5699575403527222E-3</v>
       </c>
-      <c r="BV41" s="15">
+      <c r="BV41">
         <v>4.5559963452942815E-3</v>
       </c>
-      <c r="BX41" s="34"/>
-      <c r="BY41" s="34"/>
-      <c r="BZ41" s="34"/>
+      <c r="BX41" s="1"/>
+      <c r="BY41" s="1"/>
+      <c r="BZ41" s="1"/>
     </row>
     <row r="42" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
@@ -56336,31 +56336,31 @@
       <c r="BN42" t="s">
         <v>221</v>
       </c>
-      <c r="BQ42" s="20" t="s">
+      <c r="BQ42" s="17" t="s">
         <v>194</v>
       </c>
-      <c r="BR42" s="20">
+      <c r="BR42" s="17">
         <v>7</v>
       </c>
-      <c r="BS42" s="20">
+      <c r="BS42" s="17">
         <v>7</v>
       </c>
-      <c r="BT42" s="15" t="s">
+      <c r="BT42" t="s">
         <v>194</v>
       </c>
-      <c r="BU42" s="15">
+      <c r="BU42">
         <v>7</v>
       </c>
-      <c r="BV42" s="15">
+      <c r="BV42">
         <v>7</v>
       </c>
-      <c r="BW42" s="35" t="s">
+      <c r="BW42" s="31" t="s">
         <v>276</v>
       </c>
-      <c r="BX42" s="35" t="s">
+      <c r="BX42" s="31" t="s">
         <v>188</v>
       </c>
-      <c r="BY42" s="35" t="s">
+      <c r="BY42" s="31" t="s">
         <v>187</v>
       </c>
     </row>
@@ -56440,20 +56440,19 @@
       <c r="BN43" t="s">
         <v>222</v>
       </c>
-      <c r="BQ43" s="20" t="s">
+      <c r="BQ43" s="17" t="s">
         <v>195</v>
       </c>
-      <c r="BR43" s="20">
+      <c r="BR43" s="17">
         <v>0.93753156819848704</v>
       </c>
-      <c r="BS43" s="20"/>
-      <c r="BT43" s="15" t="s">
+      <c r="BS43" s="17"/>
+      <c r="BT43" t="s">
         <v>195</v>
       </c>
-      <c r="BU43" s="15">
+      <c r="BU43">
         <v>0.68012461136873814</v>
       </c>
-      <c r="BV43" s="15"/>
       <c r="BW43" t="s">
         <v>81</v>
       </c>
@@ -56463,10 +56462,10 @@
       <c r="BY43" t="s">
         <v>277</v>
       </c>
-      <c r="CA43" s="22" t="s">
+      <c r="CA43" s="19" t="s">
         <v>275</v>
       </c>
-      <c r="CB43" s="18"/>
+      <c r="CB43" s="15"/>
     </row>
     <row r="44" spans="1:84" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
@@ -56547,20 +56546,19 @@
       <c r="BN44" t="s">
         <v>223</v>
       </c>
-      <c r="BQ44" s="20" t="s">
+      <c r="BQ44" s="17" t="s">
         <v>196</v>
       </c>
-      <c r="BR44" s="20">
+      <c r="BR44" s="17">
         <v>0</v>
       </c>
-      <c r="BS44" s="20"/>
-      <c r="BT44" s="15" t="s">
+      <c r="BS44" s="17"/>
+      <c r="BT44" t="s">
         <v>196</v>
       </c>
-      <c r="BU44" s="15">
+      <c r="BU44">
         <v>0</v>
       </c>
-      <c r="BV44" s="15"/>
       <c r="BW44" t="s">
         <v>77</v>
       </c>
@@ -56570,7 +56568,7 @@
       <c r="BY44" t="s">
         <v>277</v>
       </c>
-      <c r="CB44" s="18"/>
+      <c r="CB44" s="15"/>
     </row>
     <row r="45" spans="1:84" x14ac:dyDescent="0.25">
       <c r="B45">
@@ -56704,20 +56702,19 @@
       <c r="BN45" t="s">
         <v>224</v>
       </c>
-      <c r="BQ45" s="20" t="s">
+      <c r="BQ45" s="17" t="s">
         <v>197</v>
       </c>
-      <c r="BR45" s="20">
+      <c r="BR45" s="17">
         <v>6</v>
       </c>
-      <c r="BS45" s="20"/>
-      <c r="BT45" s="15" t="s">
+      <c r="BS45" s="17"/>
+      <c r="BT45" t="s">
         <v>197</v>
       </c>
-      <c r="BU45" s="15">
+      <c r="BU45">
         <v>6</v>
       </c>
-      <c r="BV45" s="15"/>
       <c r="BW45" t="s">
         <v>78</v>
       </c>
@@ -56807,20 +56804,19 @@
       <c r="BN46" t="s">
         <v>225</v>
       </c>
-      <c r="BQ46" s="20" t="s">
+      <c r="BQ46" s="17" t="s">
         <v>198</v>
       </c>
-      <c r="BR46" s="20">
+      <c r="BR46" s="17">
         <v>5.0644787738145078</v>
       </c>
-      <c r="BS46" s="20"/>
-      <c r="BT46" s="15" t="s">
+      <c r="BS46" s="17"/>
+      <c r="BT46" t="s">
         <v>198</v>
       </c>
-      <c r="BU46" s="15">
+      <c r="BU46">
         <v>-1.4725347229221819</v>
       </c>
-      <c r="BV46" s="15"/>
       <c r="BW46" t="s">
         <v>79</v>
       </c>
@@ -56925,20 +56921,19 @@
       <c r="BN47" t="s">
         <v>95</v>
       </c>
-      <c r="BQ47" s="20" t="s">
+      <c r="BQ47" s="17" t="s">
         <v>199</v>
       </c>
-      <c r="BR47" s="20">
+      <c r="BR47" s="17">
         <v>1.1502424256515484E-3</v>
       </c>
-      <c r="BS47" s="20"/>
-      <c r="BT47" s="15" t="s">
+      <c r="BS47" s="17"/>
+      <c r="BT47" t="s">
         <v>199</v>
       </c>
-      <c r="BU47" s="15">
+      <c r="BU47">
         <v>9.5649594522799058E-2</v>
       </c>
-      <c r="BV47" s="15"/>
       <c r="BW47" t="s">
         <v>80</v>
       </c>
@@ -57055,20 +57050,19 @@
       <c r="BN48" t="s">
         <v>94</v>
       </c>
-      <c r="BQ48" s="20" t="s">
+      <c r="BQ48" s="17" t="s">
         <v>200</v>
       </c>
-      <c r="BR48" s="20">
+      <c r="BR48" s="17">
         <v>1.9431802805153031</v>
       </c>
-      <c r="BS48" s="20"/>
-      <c r="BT48" s="15" t="s">
+      <c r="BS48" s="17"/>
+      <c r="BT48" t="s">
         <v>200</v>
       </c>
-      <c r="BU48" s="15">
+      <c r="BU48">
         <v>1.9431802805153031</v>
       </c>
-      <c r="BV48" s="15"/>
       <c r="BW48" t="s">
         <v>82</v>
       </c>
@@ -57147,20 +57141,19 @@
         <f t="shared" si="59"/>
         <v>5.6871271575581707E-3</v>
       </c>
-      <c r="BQ49" s="20" t="s">
+      <c r="BQ49" s="17" t="s">
         <v>201</v>
       </c>
-      <c r="BR49" s="20">
+      <c r="BR49" s="17">
         <v>2.3004848513030968E-3</v>
       </c>
-      <c r="BS49" s="20"/>
-      <c r="BT49" s="15" t="s">
+      <c r="BS49" s="17"/>
+      <c r="BT49" t="s">
         <v>201</v>
       </c>
-      <c r="BU49" s="15">
+      <c r="BU49">
         <v>0.19129918904559812</v>
       </c>
-      <c r="BV49" s="15"/>
       <c r="BW49" t="s">
         <v>117</v>
       </c>
@@ -57235,20 +57228,20 @@
         <f t="shared" si="59"/>
         <v>6.9656988192542428E-3</v>
       </c>
-      <c r="BQ50" s="21" t="s">
+      <c r="BQ50" s="18" t="s">
         <v>202</v>
       </c>
-      <c r="BR50" s="21">
+      <c r="BR50" s="18">
         <v>2.4469118511449697</v>
       </c>
-      <c r="BS50" s="21"/>
-      <c r="BT50" s="16" t="s">
+      <c r="BS50" s="18"/>
+      <c r="BT50" s="12" t="s">
         <v>202</v>
       </c>
-      <c r="BU50" s="16">
+      <c r="BU50" s="12">
         <v>2.4469118511449697</v>
       </c>
-      <c r="BV50" s="16"/>
+      <c r="BV50" s="12"/>
     </row>
     <row r="51" spans="1:77" x14ac:dyDescent="0.25">
       <c r="Q51" t="s">
@@ -57286,9 +57279,9 @@
         <f t="shared" si="59"/>
         <v>4.3453162130321521E-2</v>
       </c>
-      <c r="BQ51" s="18"/>
-      <c r="BR51" s="18"/>
-      <c r="BS51" s="18"/>
+      <c r="BQ51" s="15"/>
+      <c r="BR51" s="15"/>
+      <c r="BS51" s="15"/>
     </row>
     <row r="52" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
@@ -57329,9 +57322,9 @@
         <f t="shared" si="59"/>
         <v>7.2931237008914712E-2</v>
       </c>
-      <c r="BQ52" s="18"/>
-      <c r="BR52" s="18"/>
-      <c r="BS52" s="18"/>
+      <c r="BQ52" s="15"/>
+      <c r="BR52" s="15"/>
+      <c r="BS52" s="15"/>
     </row>
     <row r="53" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
@@ -57411,38 +57404,38 @@
         <f t="shared" si="59"/>
         <v>3.7106119856702559E-3</v>
       </c>
-      <c r="BQ53" s="18" t="s">
+      <c r="BQ53" s="15" t="s">
         <v>92</v>
       </c>
-      <c r="BR53" s="18"/>
-      <c r="BS53" s="18"/>
+      <c r="BR53" s="15"/>
+      <c r="BS53" s="15"/>
     </row>
     <row r="54" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>141</v>
       </c>
       <c r="B54">
-        <f t="shared" ref="B54:B93" si="76">B3-I3</f>
+        <f>B3-I3</f>
         <v>8.6139232696491007E-3</v>
       </c>
       <c r="C54">
-        <f t="shared" ref="C54:C93" si="77">C3-J3</f>
+        <f t="shared" ref="C54:C93" si="76">C3-J3</f>
         <v>1.1597017025221697E-2</v>
       </c>
       <c r="D54">
-        <f t="shared" ref="D54:D93" si="78">D3-K3</f>
+        <f t="shared" ref="D54:D93" si="77">D3-K3</f>
         <v>9.8678440838931014E-3</v>
       </c>
       <c r="E54">
-        <f t="shared" ref="E54:E93" si="79">E3-L3</f>
+        <f t="shared" ref="E54:E93" si="78">E3-L3</f>
         <v>5.4012244206910025E-3</v>
       </c>
       <c r="F54">
-        <f t="shared" ref="F54:F93" si="80">F3-M3</f>
+        <f t="shared" ref="F54:F93" si="79">F3-M3</f>
         <v>2.3479134898030038E-3</v>
       </c>
       <c r="G54">
-        <f t="shared" ref="G54:G93" si="81">G3-N3</f>
+        <f t="shared" ref="G54:G93" si="80">G3-N3</f>
         <v>-1.1113186620795024E-3</v>
       </c>
       <c r="H54">
@@ -57461,69 +57454,69 @@
         <v>66</v>
       </c>
       <c r="R54">
-        <f t="shared" ref="R54:X54" si="82">R22-Y22</f>
+        <f t="shared" ref="R54:X54" si="81">R22-Y22</f>
         <v>4.4103864439636042E-3</v>
       </c>
       <c r="S54">
-        <f t="shared" si="82"/>
+        <f t="shared" si="81"/>
         <v>-3.0420048077298145E-4</v>
       </c>
       <c r="T54">
-        <f t="shared" si="82"/>
+        <f t="shared" si="81"/>
         <v>4.2866215444997996E-2</v>
       </c>
       <c r="U54">
-        <f t="shared" si="82"/>
+        <f t="shared" si="81"/>
         <v>4.6793039541387305E-2</v>
       </c>
       <c r="V54">
-        <f t="shared" si="82"/>
+        <f t="shared" si="81"/>
         <v>6.6865107500427984E-2</v>
       </c>
       <c r="W54">
-        <f t="shared" si="82"/>
+        <f t="shared" si="81"/>
         <v>1.4855884845313E-2</v>
       </c>
       <c r="X54">
-        <f t="shared" si="82"/>
+        <f t="shared" si="81"/>
         <v>2.1882333811781007E-2</v>
       </c>
       <c r="Y54">
         <f t="shared" si="59"/>
         <v>2.8195538158156844E-2</v>
       </c>
-      <c r="BQ54" s="18" t="s">
+      <c r="BQ54" s="15" t="s">
         <v>189</v>
       </c>
-      <c r="BR54" s="18"/>
-      <c r="BS54" s="18"/>
+      <c r="BR54" s="15"/>
+      <c r="BS54" s="15"/>
     </row>
     <row r="55" spans="1:77" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>142</v>
       </c>
       <c r="B55">
+        <f t="shared" ref="B54:B93" si="82">B4-I4</f>
+        <v>2.0657175569811004E-2</v>
+      </c>
+      <c r="C55">
         <f t="shared" si="76"/>
-        <v>2.0657175569811004E-2</v>
-      </c>
-      <c r="C55">
+        <v>3.7859034655606999E-2</v>
+      </c>
+      <c r="D55">
         <f t="shared" si="77"/>
-        <v>3.7859034655606999E-2</v>
-      </c>
-      <c r="D55">
+        <v>3.1652426613510004E-2</v>
+      </c>
+      <c r="E55">
         <f t="shared" si="78"/>
-        <v>3.1652426613510004E-2</v>
-      </c>
-      <c r="E55">
+        <v>2.3262163771097008E-2</v>
+      </c>
+      <c r="F55">
         <f t="shared" si="79"/>
-        <v>2.3262163771097008E-2</v>
-      </c>
-      <c r="F55">
+        <v>2.4510679335849883E-3</v>
+      </c>
+      <c r="G55">
         <f t="shared" si="80"/>
-        <v>2.4510679335849883E-3</v>
-      </c>
-      <c r="G55">
-        <f t="shared" si="81"/>
         <v>1.2781582292334975E-2</v>
       </c>
       <c r="H55">
@@ -57573,36 +57566,36 @@
         <f t="shared" si="59"/>
         <v>1.4166071615354187E-2</v>
       </c>
-      <c r="BQ55" s="18"/>
-      <c r="BR55" s="18"/>
-      <c r="BS55" s="18"/>
+      <c r="BQ55" s="15"/>
+      <c r="BR55" s="15"/>
+      <c r="BS55" s="15"/>
     </row>
     <row r="56" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>143</v>
       </c>
       <c r="B56">
+        <f t="shared" si="82"/>
+        <v>4.1876864635944991E-3</v>
+      </c>
+      <c r="C56">
         <f t="shared" si="76"/>
-        <v>4.1876864635944991E-3</v>
-      </c>
-      <c r="C56">
+        <v>-1.0414688050575972E-3</v>
+      </c>
+      <c r="D56">
         <f t="shared" si="77"/>
-        <v>-1.0414688050575972E-3</v>
-      </c>
-      <c r="D56">
+        <v>1.0360512086995989E-3</v>
+      </c>
+      <c r="E56">
         <f t="shared" si="78"/>
-        <v>1.0360512086995989E-3</v>
-      </c>
-      <c r="E56">
+        <v>6.0432952096371E-3</v>
+      </c>
+      <c r="F56">
         <f t="shared" si="79"/>
-        <v>6.0432952096371E-3</v>
-      </c>
-      <c r="F56">
+        <v>8.1688553725731E-3</v>
+      </c>
+      <c r="G56">
         <f t="shared" si="80"/>
-        <v>8.1688553725731E-3</v>
-      </c>
-      <c r="G56">
-        <f t="shared" si="81"/>
         <v>7.7449865122941018E-3</v>
       </c>
       <c r="H56">
@@ -57652,43 +57645,43 @@
         <f t="shared" si="59"/>
         <v>9.7042688270447726E-4</v>
       </c>
-      <c r="BQ56" s="19"/>
-      <c r="BR56" s="19" t="s">
+      <c r="BQ56" s="16"/>
+      <c r="BR56" s="16" t="s">
         <v>190</v>
       </c>
-      <c r="BS56" s="19" t="s">
+      <c r="BS56" s="16" t="s">
         <v>191</v>
       </c>
-      <c r="BT56" s="17"/>
-      <c r="BU56" s="17"/>
-      <c r="BV56" s="17"/>
+      <c r="BT56" s="13"/>
+      <c r="BU56" s="13"/>
+      <c r="BV56" s="13"/>
     </row>
     <row r="57" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
         <v>144</v>
       </c>
       <c r="B57">
+        <f t="shared" si="82"/>
+        <v>-1.2384345692778201E-2</v>
+      </c>
+      <c r="C57">
         <f t="shared" si="76"/>
-        <v>-1.2384345692778201E-2</v>
-      </c>
-      <c r="C57">
+        <v>-2.9812150057632984E-3</v>
+      </c>
+      <c r="D57">
         <f t="shared" si="77"/>
-        <v>-2.9812150057632984E-3</v>
-      </c>
-      <c r="D57">
+        <v>1.317280818656702E-3</v>
+      </c>
+      <c r="E57">
         <f t="shared" si="78"/>
-        <v>1.317280818656702E-3</v>
-      </c>
-      <c r="E57">
+        <v>3.0931735699229197E-2</v>
+      </c>
+      <c r="F57">
         <f t="shared" si="79"/>
-        <v>3.0931735699229197E-2</v>
-      </c>
-      <c r="F57">
+        <v>2.24544997091848E-2</v>
+      </c>
+      <c r="G57">
         <f t="shared" si="80"/>
-        <v>2.24544997091848E-2</v>
-      </c>
-      <c r="G57">
-        <f t="shared" si="81"/>
         <v>3.5590570046045197E-2</v>
       </c>
       <c r="H57">
@@ -57738,45 +57731,42 @@
         <f t="shared" si="59"/>
         <v>7.6488066249835807E-3</v>
       </c>
-      <c r="BQ57" s="20" t="s">
+      <c r="BQ57" s="17" t="s">
         <v>192</v>
       </c>
-      <c r="BR57" s="20">
+      <c r="BR57" s="17">
         <v>0.55784051885241015</v>
       </c>
-      <c r="BS57" s="20">
+      <c r="BS57" s="17">
         <v>0.46489031788175111</v>
       </c>
-      <c r="BT57" s="15"/>
-      <c r="BU57" s="15"/>
-      <c r="BV57" s="15"/>
     </row>
     <row r="58" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>145</v>
       </c>
       <c r="B58">
+        <f t="shared" si="82"/>
+        <v>6.7118597565492995E-3</v>
+      </c>
+      <c r="C58">
         <f t="shared" si="76"/>
-        <v>6.7118597565492995E-3</v>
-      </c>
-      <c r="C58">
+        <v>3.3826828773638982E-3</v>
+      </c>
+      <c r="D58">
         <f t="shared" si="77"/>
-        <v>3.3826828773638982E-3</v>
-      </c>
-      <c r="D58">
+        <v>7.0924801618508018E-3</v>
+      </c>
+      <c r="E58">
         <f t="shared" si="78"/>
-        <v>7.0924801618508018E-3</v>
-      </c>
-      <c r="E58">
+        <v>1.0221762681394603E-2</v>
+      </c>
+      <c r="F58">
         <f t="shared" si="79"/>
-        <v>1.0221762681394603E-2</v>
-      </c>
-      <c r="F58">
+        <v>1.3344086263934997E-2</v>
+      </c>
+      <c r="G58">
         <f t="shared" si="80"/>
-        <v>1.3344086263934997E-2</v>
-      </c>
-      <c r="G58">
-        <f t="shared" si="81"/>
         <v>9.4408276162524993E-3</v>
       </c>
       <c r="H58">
@@ -57826,45 +57816,42 @@
         <f t="shared" si="59"/>
         <v>-1.1964345451702003E-3</v>
       </c>
-      <c r="BQ58" s="20" t="s">
+      <c r="BQ58" s="17" t="s">
         <v>193</v>
       </c>
-      <c r="BR58" s="20">
+      <c r="BR58" s="17">
         <v>9.7284454705884506E-3</v>
       </c>
-      <c r="BS58" s="20">
+      <c r="BS58" s="17">
         <v>1.4891400610146932E-2</v>
       </c>
-      <c r="BT58" s="15"/>
-      <c r="BU58" s="15"/>
-      <c r="BV58" s="15"/>
     </row>
     <row r="59" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
         <v>146</v>
       </c>
       <c r="B59">
+        <f t="shared" si="82"/>
+        <v>7.9485267285423003E-3</v>
+      </c>
+      <c r="C59">
         <f t="shared" si="76"/>
-        <v>7.9485267285423003E-3</v>
-      </c>
-      <c r="C59">
+        <v>8.2406685502136E-3</v>
+      </c>
+      <c r="D59">
         <f t="shared" si="77"/>
-        <v>8.2406685502136E-3</v>
-      </c>
-      <c r="D59">
+        <v>1.77497222346642E-2</v>
+      </c>
+      <c r="E59">
         <f t="shared" si="78"/>
-        <v>1.77497222346642E-2</v>
-      </c>
-      <c r="E59">
+        <v>1.8913900525784802E-2</v>
+      </c>
+      <c r="F59">
         <f t="shared" si="79"/>
-        <v>1.8913900525784802E-2</v>
-      </c>
-      <c r="F59">
+        <v>5.0024265667856907E-2</v>
+      </c>
+      <c r="G59">
         <f t="shared" si="80"/>
-        <v>5.0024265667856907E-2</v>
-      </c>
-      <c r="G59">
-        <f t="shared" si="81"/>
         <v>1.5248040948531008E-2</v>
       </c>
       <c r="H59">
@@ -57914,45 +57901,42 @@
         <f t="shared" si="59"/>
         <v>4.8773377701492159E-3</v>
       </c>
-      <c r="BQ59" s="20" t="s">
+      <c r="BQ59" s="17" t="s">
         <v>194</v>
       </c>
-      <c r="BR59" s="20">
+      <c r="BR59" s="17">
         <v>7</v>
       </c>
-      <c r="BS59" s="20">
+      <c r="BS59" s="17">
         <v>7</v>
       </c>
-      <c r="BT59" s="15"/>
-      <c r="BU59" s="15"/>
-      <c r="BV59" s="15"/>
     </row>
     <row r="60" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>147</v>
       </c>
       <c r="B60">
+        <f t="shared" si="82"/>
+        <v>2.9217141314681297E-2</v>
+      </c>
+      <c r="C60">
         <f t="shared" si="76"/>
-        <v>2.9217141314681297E-2</v>
-      </c>
-      <c r="C60">
+        <v>1.3146980004349107E-2</v>
+      </c>
+      <c r="D60">
         <f t="shared" si="77"/>
-        <v>1.3146980004349107E-2</v>
-      </c>
-      <c r="D60">
+        <v>9.0628478980154192E-2</v>
+      </c>
+      <c r="E60">
         <f t="shared" si="78"/>
-        <v>9.0628478980154192E-2</v>
-      </c>
-      <c r="E60">
+        <v>2.4897796687299009E-2</v>
+      </c>
+      <c r="F60">
         <f t="shared" si="79"/>
-        <v>2.4897796687299009E-2</v>
-      </c>
-      <c r="F60">
+        <v>6.2191813946259181E-2</v>
+      </c>
+      <c r="G60">
         <f t="shared" si="80"/>
-        <v>6.2191813946259181E-2</v>
-      </c>
-      <c r="G60">
-        <f t="shared" si="81"/>
         <v>6.8483622756936993E-2</v>
       </c>
       <c r="H60">
@@ -58002,43 +57986,40 @@
         <f t="shared" si="59"/>
         <v>1.9737862414309589E-3</v>
       </c>
-      <c r="BQ60" s="20" t="s">
+      <c r="BQ60" s="17" t="s">
         <v>195</v>
       </c>
-      <c r="BR60" s="20">
+      <c r="BR60" s="17">
         <v>0.70857784287754833</v>
       </c>
-      <c r="BS60" s="20"/>
-      <c r="BT60" s="15"/>
-      <c r="BU60" s="15"/>
-      <c r="BV60" s="15"/>
+      <c r="BS60" s="17"/>
     </row>
     <row r="61" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>148</v>
       </c>
       <c r="B61">
+        <f t="shared" si="82"/>
+        <v>5.1444062054161049E-3</v>
+      </c>
+      <c r="C61">
         <f t="shared" si="76"/>
-        <v>5.1444062054161049E-3</v>
-      </c>
-      <c r="C61">
+        <v>-5.6887139391960106E-3</v>
+      </c>
+      <c r="D61">
         <f t="shared" si="77"/>
-        <v>-5.6887139391960106E-3</v>
-      </c>
-      <c r="D61">
+        <v>1.5091957792702004E-2</v>
+      </c>
+      <c r="E61">
         <f t="shared" si="78"/>
-        <v>1.5091957792702004E-2</v>
-      </c>
-      <c r="E61">
+        <v>6.2389926271139012E-3</v>
+      </c>
+      <c r="F61">
         <f t="shared" si="79"/>
-        <v>6.2389926271139012E-3</v>
-      </c>
-      <c r="F61">
+        <v>2.2285688333313985E-2</v>
+      </c>
+      <c r="G61">
         <f t="shared" si="80"/>
-        <v>2.2285688333313985E-2</v>
-      </c>
-      <c r="G61">
-        <f t="shared" si="81"/>
         <v>3.2282853114493915E-3</v>
       </c>
       <c r="H61">
@@ -58088,43 +58069,40 @@
         <f t="shared" si="59"/>
         <v>5.9561954748622804E-4</v>
       </c>
-      <c r="BQ61" s="20" t="s">
+      <c r="BQ61" s="17" t="s">
         <v>196</v>
       </c>
-      <c r="BR61" s="20">
+      <c r="BR61" s="17">
         <v>0</v>
       </c>
-      <c r="BS61" s="20"/>
-      <c r="BT61" s="15"/>
-      <c r="BU61" s="15"/>
-      <c r="BV61" s="15"/>
+      <c r="BS61" s="17"/>
     </row>
     <row r="62" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>149</v>
       </c>
       <c r="B62">
+        <f t="shared" si="82"/>
+        <v>-1.82949807867894E-2</v>
+      </c>
+      <c r="C62">
         <f t="shared" si="76"/>
-        <v>-1.82949807867894E-2</v>
-      </c>
-      <c r="C62">
+        <v>-1.84446619943653E-2</v>
+      </c>
+      <c r="D62">
         <f t="shared" si="77"/>
-        <v>-1.84446619943653E-2</v>
-      </c>
-      <c r="D62">
+        <v>2.1941952555776703E-2</v>
+      </c>
+      <c r="E62">
         <f t="shared" si="78"/>
-        <v>2.1941952555776703E-2</v>
-      </c>
-      <c r="E62">
+        <v>-1.7306809856068903E-2</v>
+      </c>
+      <c r="F62">
         <f t="shared" si="79"/>
-        <v>-1.7306809856068903E-2</v>
-      </c>
-      <c r="F62">
+        <v>-5.7326470570119997E-3</v>
+      </c>
+      <c r="G62">
         <f t="shared" si="80"/>
-        <v>-5.7326470570119997E-3</v>
-      </c>
-      <c r="G62">
-        <f t="shared" si="81"/>
         <v>6.3677875703929687E-4</v>
       </c>
       <c r="H62">
@@ -58174,43 +58152,40 @@
         <f t="shared" si="59"/>
         <v>-1.0591003920092884E-2</v>
       </c>
-      <c r="BQ62" s="20" t="s">
+      <c r="BQ62" s="17" t="s">
         <v>197</v>
       </c>
-      <c r="BR62" s="20">
+      <c r="BR62" s="17">
         <v>6</v>
       </c>
-      <c r="BS62" s="20"/>
-      <c r="BT62" s="15"/>
-      <c r="BU62" s="15"/>
-      <c r="BV62" s="15"/>
+      <c r="BS62" s="17"/>
     </row>
     <row r="63" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>150</v>
       </c>
       <c r="B63">
+        <f t="shared" si="82"/>
+        <v>-2.6243127601759016E-3</v>
+      </c>
+      <c r="C63">
         <f t="shared" si="76"/>
-        <v>-2.6243127601759016E-3</v>
-      </c>
-      <c r="C63">
+        <v>-5.5950706963108984E-3</v>
+      </c>
+      <c r="D63">
         <f t="shared" si="77"/>
-        <v>-5.5950706963108984E-3</v>
-      </c>
-      <c r="D63">
+        <v>1.0034642878463597E-2</v>
+      </c>
+      <c r="E63">
         <f t="shared" si="78"/>
-        <v>1.0034642878463597E-2</v>
-      </c>
-      <c r="E63">
+        <v>1.3662137807904998E-3</v>
+      </c>
+      <c r="F63">
         <f t="shared" si="79"/>
-        <v>1.3662137807904998E-3</v>
-      </c>
-      <c r="F63">
+        <v>-7.1135012185339977E-3</v>
+      </c>
+      <c r="G63">
         <f t="shared" si="80"/>
-        <v>-7.1135012185339977E-3</v>
-      </c>
-      <c r="G63">
-        <f t="shared" si="81"/>
         <v>9.5621205674652973E-3</v>
       </c>
       <c r="H63">
@@ -58260,43 +58235,40 @@
         <f t="shared" si="59"/>
         <v>1.7698025282770997E-2</v>
       </c>
-      <c r="BQ63" s="20" t="s">
+      <c r="BQ63" s="17" t="s">
         <v>198</v>
       </c>
-      <c r="BR63" s="20">
+      <c r="BR63" s="17">
         <v>2.8278846979813896</v>
       </c>
-      <c r="BS63" s="20"/>
-      <c r="BT63" s="15"/>
-      <c r="BU63" s="15"/>
-      <c r="BV63" s="15"/>
+      <c r="BS63" s="17"/>
     </row>
     <row r="64" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>151</v>
       </c>
       <c r="B64">
+        <f t="shared" si="82"/>
+        <v>9.2531371218344035E-4</v>
+      </c>
+      <c r="C64">
         <f t="shared" si="76"/>
-        <v>9.2531371218344035E-4</v>
-      </c>
-      <c r="C64">
+        <v>-8.4667213778500186E-5</v>
+      </c>
+      <c r="D64">
         <f t="shared" si="77"/>
-        <v>-8.4667213778500186E-5</v>
-      </c>
-      <c r="D64">
+        <v>1.3462594195936799E-3</v>
+      </c>
+      <c r="E64">
         <f t="shared" si="78"/>
-        <v>1.3462594195936799E-3</v>
-      </c>
-      <c r="E64">
+        <v>3.2785547498211977E-4</v>
+      </c>
+      <c r="F64">
         <f t="shared" si="79"/>
-        <v>3.2785547498211977E-4</v>
-      </c>
-      <c r="F64">
+        <v>4.0876826126500128E-4</v>
+      </c>
+      <c r="G64">
         <f t="shared" si="80"/>
-        <v>4.0876826126500128E-4</v>
-      </c>
-      <c r="G64">
-        <f t="shared" si="81"/>
         <v>2.8780278276100031E-4</v>
       </c>
       <c r="H64">
@@ -58346,43 +58318,40 @@
         <f t="shared" si="59"/>
         <v>2.6547617536070267E-2</v>
       </c>
-      <c r="BQ64" s="20" t="s">
+      <c r="BQ64" s="17" t="s">
         <v>199</v>
       </c>
-      <c r="BR64" s="20">
+      <c r="BR64" s="17">
         <v>1.5020575128104436E-2</v>
       </c>
-      <c r="BS64" s="20"/>
-      <c r="BT64" s="15"/>
-      <c r="BU64" s="15"/>
-      <c r="BV64" s="15"/>
+      <c r="BS64" s="17"/>
     </row>
     <row r="65" spans="1:74" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>152</v>
       </c>
       <c r="B65">
+        <f t="shared" si="82"/>
+        <v>-1.8726072483839923E-4</v>
+      </c>
+      <c r="C65">
         <f t="shared" si="76"/>
-        <v>-1.8726072483839923E-4</v>
-      </c>
-      <c r="C65">
+        <v>-2.7811873463538944E-3</v>
+      </c>
+      <c r="D65">
         <f t="shared" si="77"/>
-        <v>-2.7811873463538944E-3</v>
-      </c>
-      <c r="D65">
+        <v>6.6010218757010797E-6</v>
+      </c>
+      <c r="E65">
         <f t="shared" si="78"/>
-        <v>6.6010218757010797E-6</v>
-      </c>
-      <c r="E65">
+        <v>1.3295363264692203E-2</v>
+      </c>
+      <c r="F65">
         <f t="shared" si="79"/>
-        <v>1.3295363264692203E-2</v>
-      </c>
-      <c r="F65">
+        <v>9.3076586786399601E-4</v>
+      </c>
+      <c r="G65">
         <f t="shared" si="80"/>
-        <v>9.3076586786399601E-4</v>
-      </c>
-      <c r="G65">
-        <f t="shared" si="81"/>
         <v>1.3768553987778404E-2</v>
       </c>
       <c r="H65">
@@ -58432,43 +58401,40 @@
         <f t="shared" si="59"/>
         <v>-6.0593470921663723E-3</v>
       </c>
-      <c r="BQ65" s="20" t="s">
+      <c r="BQ65" s="17" t="s">
         <v>200</v>
       </c>
-      <c r="BR65" s="20">
+      <c r="BR65" s="17">
         <v>1.9431802805153031</v>
       </c>
-      <c r="BS65" s="20"/>
-      <c r="BT65" s="15"/>
-      <c r="BU65" s="15"/>
-      <c r="BV65" s="15"/>
+      <c r="BS65" s="17"/>
     </row>
     <row r="66" spans="1:74" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
         <v>153</v>
       </c>
       <c r="B66">
+        <f t="shared" si="82"/>
+        <v>1.4492622332526212E-2</v>
+      </c>
+      <c r="C66">
         <f t="shared" si="76"/>
-        <v>1.4492622332526212E-2</v>
-      </c>
-      <c r="C66">
+        <v>4.0891704901205014E-2</v>
+      </c>
+      <c r="D66">
         <f t="shared" si="77"/>
-        <v>4.0891704901205014E-2</v>
-      </c>
-      <c r="D66">
+        <v>-8.4419317993275067E-3</v>
+      </c>
+      <c r="E66">
         <f t="shared" si="78"/>
-        <v>-8.4419317993275067E-3</v>
-      </c>
-      <c r="E66">
+        <v>-0.1559286516414492</v>
+      </c>
+      <c r="F66">
         <f t="shared" si="79"/>
-        <v>-0.1559286516414492</v>
-      </c>
-      <c r="F66">
+        <v>-1.2802824351719005E-2</v>
+      </c>
+      <c r="G66">
         <f t="shared" si="80"/>
-        <v>-1.2802824351719005E-2</v>
-      </c>
-      <c r="G66">
-        <f t="shared" si="81"/>
         <v>-1.5795246081807018E-2</v>
       </c>
       <c r="H66">
@@ -58518,43 +58484,40 @@
         <f t="shared" si="59"/>
         <v>-2.8317218922309727E-2</v>
       </c>
-      <c r="BQ66" s="20" t="s">
+      <c r="BQ66" s="17" t="s">
         <v>201</v>
       </c>
-      <c r="BR66" s="20">
+      <c r="BR66" s="17">
         <v>3.0041150256208873E-2</v>
       </c>
-      <c r="BS66" s="20"/>
-      <c r="BT66" s="15"/>
-      <c r="BU66" s="15"/>
-      <c r="BV66" s="15"/>
+      <c r="BS66" s="17"/>
     </row>
     <row r="67" spans="1:74" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A67" s="3" t="s">
         <v>154</v>
       </c>
       <c r="B67">
+        <f t="shared" si="82"/>
+        <v>9.3837037219279829E-3</v>
+      </c>
+      <c r="C67">
         <f t="shared" si="76"/>
-        <v>9.3837037219279829E-3</v>
-      </c>
-      <c r="C67">
+        <v>5.4904096634679989E-2</v>
+      </c>
+      <c r="D67">
         <f t="shared" si="77"/>
-        <v>5.4904096634679989E-2</v>
-      </c>
-      <c r="D67">
+        <v>6.8284591349959678E-3</v>
+      </c>
+      <c r="E67">
         <f t="shared" si="78"/>
-        <v>6.8284591349959678E-3</v>
-      </c>
-      <c r="E67">
+        <v>-0.16184638787515498</v>
+      </c>
+      <c r="F67">
         <f t="shared" si="79"/>
-        <v>-0.16184638787515498</v>
-      </c>
-      <c r="F67">
+        <v>8.7380893498854029E-2</v>
+      </c>
+      <c r="G67">
         <f t="shared" si="80"/>
-        <v>8.7380893498854029E-2</v>
-      </c>
-      <c r="G67">
-        <f t="shared" si="81"/>
         <v>-0.13309037048545203</v>
       </c>
       <c r="H67">
@@ -58569,43 +58532,43 @@
         <f t="shared" si="85"/>
         <v>4.0159550096958659E-2</v>
       </c>
-      <c r="BQ67" s="21" t="s">
+      <c r="BQ67" s="18" t="s">
         <v>202</v>
       </c>
-      <c r="BR67" s="21">
+      <c r="BR67" s="18">
         <v>2.4469118511449697</v>
       </c>
-      <c r="BS67" s="21"/>
-      <c r="BT67" s="16"/>
-      <c r="BU67" s="16"/>
-      <c r="BV67" s="16"/>
+      <c r="BS67" s="18"/>
+      <c r="BT67" s="12"/>
+      <c r="BU67" s="12"/>
+      <c r="BV67" s="12"/>
     </row>
     <row r="68" spans="1:74" x14ac:dyDescent="0.25">
       <c r="A68" s="4" t="s">
         <v>155</v>
       </c>
       <c r="B68">
+        <f t="shared" si="82"/>
+        <v>2.5125821376699997E-3</v>
+      </c>
+      <c r="C68">
         <f t="shared" si="76"/>
-        <v>2.5125821376699997E-3</v>
-      </c>
-      <c r="C68">
+        <v>3.3829521073781045E-3</v>
+      </c>
+      <c r="D68">
         <f t="shared" si="77"/>
-        <v>3.3829521073781045E-3</v>
-      </c>
-      <c r="D68">
+        <v>3.6569779670194008E-3</v>
+      </c>
+      <c r="E68">
         <f t="shared" si="78"/>
-        <v>3.6569779670194008E-3</v>
-      </c>
-      <c r="E68">
+        <v>9.5838222669059059E-3</v>
+      </c>
+      <c r="F68">
         <f t="shared" si="79"/>
-        <v>9.5838222669059059E-3</v>
-      </c>
-      <c r="F68">
+        <v>2.8142919301611988E-2</v>
+      </c>
+      <c r="G68">
         <f t="shared" si="80"/>
-        <v>2.8142919301611988E-2</v>
-      </c>
-      <c r="G68">
-        <f t="shared" si="81"/>
         <v>1.8221781526550497E-2</v>
       </c>
       <c r="H68">
@@ -58626,27 +58589,27 @@
         <v>156</v>
       </c>
       <c r="B69">
+        <f t="shared" si="82"/>
+        <v>2.36352341821391E-2</v>
+      </c>
+      <c r="C69">
         <f t="shared" si="76"/>
-        <v>2.36352341821391E-2</v>
-      </c>
-      <c r="C69">
+        <v>3.8955547704688925E-3</v>
+      </c>
+      <c r="D69">
         <f t="shared" si="77"/>
-        <v>3.8955547704688925E-3</v>
-      </c>
-      <c r="D69">
+        <v>1.1996889584206E-2</v>
+      </c>
+      <c r="E69">
         <f t="shared" si="78"/>
-        <v>1.1996889584206E-2</v>
-      </c>
-      <c r="E69">
+        <v>1.3634839037527199E-2</v>
+      </c>
+      <c r="F69">
         <f t="shared" si="79"/>
-        <v>1.3634839037527199E-2</v>
-      </c>
-      <c r="F69">
+        <v>6.366745267655699E-2</v>
+      </c>
+      <c r="G69">
         <f t="shared" si="80"/>
-        <v>6.366745267655699E-2</v>
-      </c>
-      <c r="G69">
-        <f t="shared" si="81"/>
         <v>3.8450150501876001E-2</v>
       </c>
       <c r="H69">
@@ -58667,27 +58630,27 @@
         <v>157</v>
       </c>
       <c r="B70">
+        <f t="shared" si="82"/>
+        <v>1.2747157339906796E-2</v>
+      </c>
+      <c r="C70">
         <f t="shared" si="76"/>
-        <v>1.2747157339906796E-2</v>
-      </c>
-      <c r="C70">
+        <v>1.1833381600802328E-5</v>
+      </c>
+      <c r="D70">
         <f t="shared" si="77"/>
-        <v>1.1833381600802328E-5</v>
-      </c>
-      <c r="D70">
+        <v>-1.8618122900814008E-3</v>
+      </c>
+      <c r="E70">
         <f t="shared" si="78"/>
-        <v>-1.8618122900814008E-3</v>
-      </c>
-      <c r="E70">
+        <v>1.8829930456393196E-2</v>
+      </c>
+      <c r="F70">
         <f t="shared" si="79"/>
-        <v>1.8829930456393196E-2</v>
-      </c>
-      <c r="F70">
+        <v>5.6144324964631703E-2</v>
+      </c>
+      <c r="G70">
         <f t="shared" si="80"/>
-        <v>5.6144324964631703E-2</v>
-      </c>
-      <c r="G70">
-        <f t="shared" si="81"/>
         <v>-5.1426798796641998E-3</v>
       </c>
       <c r="H70">
@@ -58708,27 +58671,27 @@
         <v>158</v>
       </c>
       <c r="B71">
+        <f t="shared" si="82"/>
+        <v>4.1723637549413994E-2</v>
+      </c>
+      <c r="C71">
         <f t="shared" si="76"/>
-        <v>4.1723637549413994E-2</v>
-      </c>
-      <c r="C71">
+        <v>9.8167436268560004E-3</v>
+      </c>
+      <c r="D71">
         <f t="shared" si="77"/>
-        <v>9.8167436268560004E-3</v>
-      </c>
-      <c r="D71">
+        <v>-1.3384615897210073E-3</v>
+      </c>
+      <c r="E71">
         <f t="shared" si="78"/>
-        <v>-1.3384615897210073E-3</v>
-      </c>
-      <c r="E71">
+        <v>2.8581899384723997E-2</v>
+      </c>
+      <c r="F71">
         <f t="shared" si="79"/>
-        <v>2.8581899384723997E-2</v>
-      </c>
-      <c r="F71">
+        <v>1.3972084387596978E-2</v>
+      </c>
+      <c r="G71">
         <f t="shared" si="80"/>
-        <v>1.3972084387596978E-2</v>
-      </c>
-      <c r="G71">
-        <f t="shared" si="81"/>
         <v>-5.8760730892679636E-3</v>
       </c>
       <c r="H71">
@@ -58742,14 +58705,6 @@
       <c r="K71">
         <f t="shared" si="85"/>
         <v>5.8074201146262588E-3</v>
-      </c>
-      <c r="M71">
-        <f>AVERAGE(B71:H73)</f>
-        <v>2.0292608270573723E-2</v>
-      </c>
-      <c r="N71">
-        <f>_xlfn.STDEV.P(B71:H73)/SQRT(COUNT(B71:H73))</f>
-        <v>4.091608966057543E-3</v>
       </c>
     </row>
     <row r="72" spans="1:74" x14ac:dyDescent="0.25">
@@ -58757,27 +58712,27 @@
         <v>159</v>
       </c>
       <c r="B72">
+        <f t="shared" si="82"/>
+        <v>7.3239259813421997E-2</v>
+      </c>
+      <c r="C72">
         <f t="shared" si="76"/>
-        <v>7.3239259813421997E-2</v>
-      </c>
-      <c r="C72">
+        <v>1.1256226083345006E-2</v>
+      </c>
+      <c r="D72">
         <f t="shared" si="77"/>
-        <v>1.1256226083345006E-2</v>
-      </c>
-      <c r="D72">
+        <v>1.4067169707795008E-2</v>
+      </c>
+      <c r="E72">
         <f t="shared" si="78"/>
-        <v>1.4067169707795008E-2</v>
-      </c>
-      <c r="E72">
+        <v>5.3697005956595004E-2</v>
+      </c>
+      <c r="F72">
         <f t="shared" si="79"/>
-        <v>5.3697005956595004E-2</v>
-      </c>
-      <c r="F72">
+        <v>2.3497832081419978E-3</v>
+      </c>
+      <c r="G72">
         <f t="shared" si="80"/>
-        <v>2.3497832081419978E-3</v>
-      </c>
-      <c r="G72">
-        <f t="shared" si="81"/>
         <v>2.7091968211745004E-2</v>
       </c>
       <c r="H72">
@@ -58798,27 +58753,27 @@
         <v>160</v>
       </c>
       <c r="B73">
+        <f t="shared" si="82"/>
+        <v>1.1013844192461403E-2</v>
+      </c>
+      <c r="C73">
         <f t="shared" si="76"/>
-        <v>1.1013844192461403E-2</v>
-      </c>
-      <c r="C73">
+        <v>3.3687727879795071E-3</v>
+      </c>
+      <c r="D73">
         <f t="shared" si="77"/>
-        <v>3.3687727879795071E-3</v>
-      </c>
-      <c r="D73">
+        <v>5.9577714780069957E-3</v>
+      </c>
+      <c r="E73">
         <f t="shared" si="78"/>
-        <v>5.9577714780069957E-3</v>
-      </c>
-      <c r="E73">
+        <v>2.0957266077438995E-2</v>
+      </c>
+      <c r="F73">
         <f t="shared" si="79"/>
-        <v>2.0957266077438995E-2</v>
-      </c>
-      <c r="F73">
+        <v>3.2827482856482404E-2</v>
+      </c>
+      <c r="G73">
         <f t="shared" si="80"/>
-        <v>3.2827482856482404E-2</v>
-      </c>
-      <c r="G73">
-        <f t="shared" si="81"/>
         <v>1.2902454896886795E-2</v>
       </c>
       <c r="H73">
@@ -58839,27 +58794,27 @@
         <v>161</v>
       </c>
       <c r="B74">
+        <f t="shared" si="82"/>
+        <v>2.0749923998273502E-2</v>
+      </c>
+      <c r="C74">
         <f t="shared" si="76"/>
-        <v>2.0749923998273502E-2</v>
-      </c>
-      <c r="C74">
+        <v>5.6058599700276983E-3</v>
+      </c>
+      <c r="D74">
         <f t="shared" si="77"/>
-        <v>5.6058599700276983E-3</v>
-      </c>
-      <c r="D74">
+        <v>8.8094618429953031E-3</v>
+      </c>
+      <c r="E74">
         <f t="shared" si="78"/>
-        <v>8.8094618429953031E-3</v>
-      </c>
-      <c r="E74">
+        <v>1.8621930012066197E-2</v>
+      </c>
+      <c r="F74">
         <f t="shared" si="79"/>
-        <v>1.8621930012066197E-2</v>
-      </c>
-      <c r="F74">
+        <v>6.2491425639949957E-4</v>
+      </c>
+      <c r="G74">
         <f t="shared" si="80"/>
-        <v>6.2491425639949957E-4</v>
-      </c>
-      <c r="G74">
-        <f t="shared" si="81"/>
         <v>2.3261623911740997E-2</v>
       </c>
       <c r="H74">
@@ -58880,27 +58835,27 @@
         <v>162</v>
       </c>
       <c r="B75">
+        <f t="shared" si="82"/>
+        <v>2.6414715253592999E-2</v>
+      </c>
+      <c r="C75">
         <f t="shared" si="76"/>
-        <v>2.6414715253592999E-2</v>
-      </c>
-      <c r="C75">
+        <v>4.2591626404313021E-3</v>
+      </c>
+      <c r="D75">
         <f t="shared" si="77"/>
-        <v>4.2591626404313021E-3</v>
-      </c>
-      <c r="D75">
+        <v>1.5961085918063798E-2</v>
+      </c>
+      <c r="E75">
         <f t="shared" si="78"/>
-        <v>1.5961085918063798E-2</v>
-      </c>
-      <c r="E75">
+        <v>2.57077716205595E-2</v>
+      </c>
+      <c r="F75">
         <f t="shared" si="79"/>
-        <v>2.57077716205595E-2</v>
-      </c>
-      <c r="F75">
+        <v>5.340722951386899E-3</v>
+      </c>
+      <c r="G75">
         <f t="shared" si="80"/>
-        <v>5.340722951386899E-3</v>
-      </c>
-      <c r="G75">
-        <f t="shared" si="81"/>
         <v>1.51668884795279E-2</v>
       </c>
       <c r="H75">
@@ -58921,27 +58876,27 @@
         <v>163</v>
       </c>
       <c r="B76">
+        <f t="shared" si="82"/>
+        <v>1.2083909903647619E-2</v>
+      </c>
+      <c r="C76">
         <f t="shared" si="76"/>
-        <v>1.2083909903647619E-2</v>
-      </c>
-      <c r="C76">
+        <v>-4.6287085339770002E-3</v>
+      </c>
+      <c r="D76">
         <f t="shared" si="77"/>
-        <v>-4.6287085339770002E-3</v>
-      </c>
-      <c r="D76">
+        <v>7.7505422032293006E-3</v>
+      </c>
+      <c r="E76">
         <f t="shared" si="78"/>
-        <v>7.7505422032293006E-3</v>
-      </c>
-      <c r="E76">
+        <v>9.7761604437799007E-3</v>
+      </c>
+      <c r="F76">
         <f t="shared" si="79"/>
-        <v>9.7761604437799007E-3</v>
-      </c>
-      <c r="F76">
+        <v>3.1004310688359862E-4</v>
+      </c>
+      <c r="G76">
         <f t="shared" si="80"/>
-        <v>3.1004310688359862E-4</v>
-      </c>
-      <c r="G76">
-        <f t="shared" si="81"/>
         <v>8.1903724172859883E-4</v>
       </c>
       <c r="H76">
@@ -58962,27 +58917,27 @@
         <v>164</v>
       </c>
       <c r="B77">
+        <f t="shared" si="82"/>
+        <v>1.7838664695353404E-2</v>
+      </c>
+      <c r="C77">
         <f t="shared" si="76"/>
-        <v>1.7838664695353404E-2</v>
-      </c>
-      <c r="C77">
+        <v>1.0231888697171398E-2</v>
+      </c>
+      <c r="D77">
         <f t="shared" si="77"/>
-        <v>1.0231888697171398E-2</v>
-      </c>
-      <c r="D77">
+        <v>6.8094279388450918E-3</v>
+      </c>
+      <c r="E77">
         <f t="shared" si="78"/>
-        <v>6.8094279388450918E-3</v>
-      </c>
-      <c r="E77">
+        <v>3.6439956571669208E-2</v>
+      </c>
+      <c r="F77">
         <f t="shared" si="79"/>
-        <v>3.6439956571669208E-2</v>
-      </c>
-      <c r="F77">
+        <v>3.0063255008164307E-2</v>
+      </c>
+      <c r="G77">
         <f t="shared" si="80"/>
-        <v>3.0063255008164307E-2</v>
-      </c>
-      <c r="G77">
-        <f t="shared" si="81"/>
         <v>1.2852173185283894E-2</v>
       </c>
       <c r="H77">
@@ -59003,27 +58958,27 @@
         <v>165</v>
       </c>
       <c r="B78">
+        <f t="shared" si="82"/>
+        <v>4.1417763100809746E-3</v>
+      </c>
+      <c r="C78">
         <f t="shared" si="76"/>
-        <v>4.1417763100809746E-3</v>
-      </c>
-      <c r="C78">
+        <v>1.0693462880769E-2</v>
+      </c>
+      <c r="D78">
         <f t="shared" si="77"/>
-        <v>1.0693462880769E-2</v>
-      </c>
-      <c r="D78">
+        <v>1.0373186738810991E-2</v>
+      </c>
+      <c r="E78">
         <f t="shared" si="78"/>
-        <v>1.0373186738810991E-2</v>
-      </c>
-      <c r="E78">
+        <v>4.697977624731009E-3</v>
+      </c>
+      <c r="F78">
         <f t="shared" si="79"/>
-        <v>4.697977624731009E-3</v>
-      </c>
-      <c r="F78">
+        <v>-4.4744807468962006E-2</v>
+      </c>
+      <c r="G78">
         <f t="shared" si="80"/>
-        <v>-4.4744807468962006E-2</v>
-      </c>
-      <c r="G78">
-        <f t="shared" si="81"/>
         <v>3.6899193695908994E-2</v>
       </c>
       <c r="H78">
@@ -59044,27 +58999,27 @@
         <v>166</v>
       </c>
       <c r="B79">
+        <f t="shared" si="82"/>
+        <v>-1.119594560945996E-4</v>
+      </c>
+      <c r="C79">
         <f t="shared" si="76"/>
-        <v>-1.119594560945996E-4</v>
-      </c>
-      <c r="C79">
+        <v>-1.6098497560477001E-3</v>
+      </c>
+      <c r="D79">
         <f t="shared" si="77"/>
-        <v>-1.6098497560477001E-3</v>
-      </c>
-      <c r="D79">
+        <v>4.5021567707163E-3</v>
+      </c>
+      <c r="E79">
         <f t="shared" si="78"/>
-        <v>4.5021567707163E-3</v>
-      </c>
-      <c r="E79">
+        <v>-2.0260084782363897E-2</v>
+      </c>
+      <c r="F79">
         <f t="shared" si="79"/>
-        <v>-2.0260084782363897E-2</v>
-      </c>
-      <c r="F79">
+        <v>-6.6473591816577013E-3</v>
+      </c>
+      <c r="G79">
         <f t="shared" si="80"/>
-        <v>-6.6473591816577013E-3</v>
-      </c>
-      <c r="G79">
-        <f t="shared" si="81"/>
         <v>1.2919295046574998E-2</v>
       </c>
       <c r="H79">
@@ -59085,27 +59040,27 @@
         <v>167</v>
       </c>
       <c r="B80">
+        <f t="shared" si="82"/>
+        <v>-4.8506078101632003E-3</v>
+      </c>
+      <c r="C80">
         <f t="shared" si="76"/>
-        <v>-4.8506078101632003E-3</v>
-      </c>
-      <c r="C80">
+        <v>-8.1575177016604966E-3</v>
+      </c>
+      <c r="D80">
         <f t="shared" si="77"/>
-        <v>-8.1575177016604966E-3</v>
-      </c>
-      <c r="D80">
+        <v>1.2438124777419193E-2</v>
+      </c>
+      <c r="E80">
         <f t="shared" si="78"/>
-        <v>1.2438124777419193E-2</v>
-      </c>
-      <c r="E80">
+        <v>-5.887753859392629E-2</v>
+      </c>
+      <c r="F80">
         <f t="shared" si="79"/>
-        <v>-5.887753859392629E-2</v>
-      </c>
-      <c r="F80">
+        <v>-4.4260027211415101E-2</v>
+      </c>
+      <c r="G80">
         <f t="shared" si="80"/>
-        <v>-4.4260027211415101E-2</v>
-      </c>
-      <c r="G80">
-        <f t="shared" si="81"/>
         <v>-2.6024212754340026E-3</v>
       </c>
       <c r="H80">
@@ -59126,27 +59081,27 @@
         <v>168</v>
       </c>
       <c r="B81">
+        <f t="shared" si="82"/>
+        <v>4.6299019847542994E-3</v>
+      </c>
+      <c r="C81">
         <f t="shared" si="76"/>
-        <v>4.6299019847542994E-3</v>
-      </c>
-      <c r="C81">
+        <v>8.5819042135779934E-4</v>
+      </c>
+      <c r="D81">
         <f t="shared" si="77"/>
-        <v>8.5819042135779934E-4</v>
-      </c>
-      <c r="D81">
+        <v>6.5986898043766985E-3</v>
+      </c>
+      <c r="E81">
         <f t="shared" si="78"/>
-        <v>6.5986898043766985E-3</v>
-      </c>
-      <c r="E81">
+        <v>2.6057153799766974E-3</v>
+      </c>
+      <c r="F81">
         <f t="shared" si="79"/>
-        <v>2.6057153799766974E-3</v>
-      </c>
-      <c r="F81">
+        <v>1.6877325281983598E-2</v>
+      </c>
+      <c r="G81">
         <f t="shared" si="80"/>
-        <v>1.6877325281983598E-2</v>
-      </c>
-      <c r="G81">
-        <f t="shared" si="81"/>
         <v>-3.3187825202193044E-3</v>
       </c>
       <c r="H81">
@@ -59167,27 +59122,27 @@
         <v>169</v>
       </c>
       <c r="B82">
+        <f t="shared" si="82"/>
+        <v>2.8456666773405026E-2</v>
+      </c>
+      <c r="C82">
         <f t="shared" si="76"/>
-        <v>2.8456666773405026E-2</v>
-      </c>
-      <c r="C82">
+        <v>2.0061085137054013E-2</v>
+      </c>
+      <c r="D82">
         <f t="shared" si="77"/>
-        <v>2.0061085137054013E-2</v>
-      </c>
-      <c r="D82">
+        <v>5.2242335970780984E-2</v>
+      </c>
+      <c r="E82">
         <f t="shared" si="78"/>
-        <v>5.2242335970780984E-2</v>
-      </c>
-      <c r="E82">
+        <v>0.12788966091492399</v>
+      </c>
+      <c r="F82">
         <f t="shared" si="79"/>
-        <v>0.12788966091492399</v>
-      </c>
-      <c r="F82">
+        <v>5.1013693175442965E-2</v>
+      </c>
+      <c r="G82">
         <f t="shared" si="80"/>
-        <v>5.1013693175442965E-2</v>
-      </c>
-      <c r="G82">
-        <f t="shared" si="81"/>
         <v>4.5329556250393976E-2</v>
       </c>
       <c r="H82">
@@ -59208,27 +59163,27 @@
         <v>170</v>
       </c>
       <c r="B83">
+        <f t="shared" si="82"/>
+        <v>-3.5544347341054904E-2</v>
+      </c>
+      <c r="C83">
         <f t="shared" si="76"/>
-        <v>-3.5544347341054904E-2</v>
-      </c>
-      <c r="C83">
+        <v>6.5244777169682494E-2</v>
+      </c>
+      <c r="D83">
         <f t="shared" si="77"/>
-        <v>6.5244777169682494E-2</v>
-      </c>
-      <c r="D83">
+        <v>6.191029933939099E-2</v>
+      </c>
+      <c r="E83">
         <f t="shared" si="78"/>
-        <v>6.191029933939099E-2</v>
-      </c>
-      <c r="E83">
+        <v>-4.4985274270950004E-3</v>
+      </c>
+      <c r="F83">
         <f t="shared" si="79"/>
-        <v>-4.4985274270950004E-3</v>
-      </c>
-      <c r="F83">
+        <v>5.8428341554893015E-2</v>
+      </c>
+      <c r="G83">
         <f t="shared" si="80"/>
-        <v>5.8428341554893015E-2</v>
-      </c>
-      <c r="G83">
-        <f t="shared" si="81"/>
         <v>2.9183859051710004E-2</v>
       </c>
       <c r="H83">
@@ -59249,27 +59204,27 @@
         <v>171</v>
       </c>
       <c r="B84">
+        <f t="shared" si="82"/>
+        <v>4.4103864439636042E-3</v>
+      </c>
+      <c r="C84">
         <f t="shared" si="76"/>
-        <v>4.4103864439636042E-3</v>
-      </c>
-      <c r="C84">
+        <v>-3.0420048077298145E-4</v>
+      </c>
+      <c r="D84">
         <f t="shared" si="77"/>
-        <v>-3.0420048077298145E-4</v>
-      </c>
-      <c r="D84">
+        <v>4.2866215444997996E-2</v>
+      </c>
+      <c r="E84">
         <f t="shared" si="78"/>
-        <v>4.2866215444997996E-2</v>
-      </c>
-      <c r="E84">
+        <v>4.6793039541387305E-2</v>
+      </c>
+      <c r="F84">
         <f t="shared" si="79"/>
-        <v>4.6793039541387305E-2</v>
-      </c>
-      <c r="F84">
+        <v>6.6865107500427984E-2</v>
+      </c>
+      <c r="G84">
         <f t="shared" si="80"/>
-        <v>6.6865107500427984E-2</v>
-      </c>
-      <c r="G84">
-        <f t="shared" si="81"/>
         <v>1.4855884845313E-2</v>
       </c>
       <c r="H84">
@@ -59290,27 +59245,27 @@
         <v>172</v>
       </c>
       <c r="B85">
+        <f t="shared" si="82"/>
+        <v>3.7250500623951993E-2</v>
+      </c>
+      <c r="C85">
         <f t="shared" si="76"/>
-        <v>3.7250500623951993E-2</v>
-      </c>
-      <c r="C85">
+        <v>-6.5150882588398018E-2</v>
+      </c>
+      <c r="D85">
         <f t="shared" si="77"/>
-        <v>-6.5150882588398018E-2</v>
-      </c>
-      <c r="D85">
+        <v>6.4496655369922024E-2</v>
+      </c>
+      <c r="E85">
         <f t="shared" si="78"/>
-        <v>6.4496655369922024E-2</v>
-      </c>
-      <c r="E85">
+        <v>2.8991867869063992E-2</v>
+      </c>
+      <c r="F85">
         <f t="shared" si="79"/>
-        <v>2.8991867869063992E-2</v>
-      </c>
-      <c r="F85">
+        <v>5.0256828958442995E-2</v>
+      </c>
+      <c r="G85">
         <f t="shared" si="80"/>
-        <v>5.0256828958442995E-2</v>
-      </c>
-      <c r="G85">
-        <f t="shared" si="81"/>
         <v>-3.3853173690790994E-2</v>
       </c>
       <c r="H85">
@@ -59331,27 +59286,27 @@
         <v>173</v>
       </c>
       <c r="B86">
+        <f t="shared" si="82"/>
+        <v>1.4921727003982095E-2</v>
+      </c>
+      <c r="C86">
         <f t="shared" si="76"/>
-        <v>1.4921727003982095E-2</v>
-      </c>
-      <c r="C86">
+        <v>1.1498153337649905E-2</v>
+      </c>
+      <c r="D86">
         <f t="shared" si="77"/>
-        <v>1.1498153337649905E-2</v>
-      </c>
-      <c r="D86">
+        <v>3.1847405893790398E-2</v>
+      </c>
+      <c r="E86">
         <f t="shared" si="78"/>
-        <v>3.1847405893790398E-2</v>
-      </c>
-      <c r="E86">
+        <v>-1.4256583594375982E-2</v>
+      </c>
+      <c r="F86">
         <f t="shared" si="79"/>
-        <v>-1.4256583594375982E-2</v>
-      </c>
-      <c r="F86">
+        <v>4.7958838354516045E-3</v>
+      </c>
+      <c r="G86">
         <f t="shared" si="80"/>
-        <v>4.7958838354516045E-3</v>
-      </c>
-      <c r="G86">
-        <f t="shared" si="81"/>
         <v>6.4849065890250079E-3</v>
       </c>
       <c r="H86">
@@ -59372,27 +59327,27 @@
         <v>174</v>
       </c>
       <c r="B87">
+        <f t="shared" si="82"/>
+        <v>3.9966238379833041E-2</v>
+      </c>
+      <c r="C87">
         <f t="shared" si="76"/>
-        <v>3.9966238379833041E-2</v>
-      </c>
-      <c r="C87">
+        <v>4.9364909214616004E-2</v>
+      </c>
+      <c r="D87">
         <f t="shared" si="77"/>
-        <v>4.9364909214616004E-2</v>
-      </c>
-      <c r="D87">
+        <v>3.6312564585198992E-2</v>
+      </c>
+      <c r="E87">
         <f t="shared" si="78"/>
-        <v>3.6312564585198992E-2</v>
-      </c>
-      <c r="E87">
+        <v>-9.1237025620990453E-3</v>
+      </c>
+      <c r="F87">
         <f t="shared" si="79"/>
-        <v>-9.1237025620990453E-3</v>
-      </c>
-      <c r="F87">
+        <v>-0.24264625032822801</v>
+      </c>
+      <c r="G87">
         <f t="shared" si="80"/>
-        <v>-0.24264625032822801</v>
-      </c>
-      <c r="G87">
-        <f t="shared" si="81"/>
         <v>8.7457760425302067E-2</v>
       </c>
       <c r="H87">
@@ -59413,27 +59368,27 @@
         <v>175</v>
       </c>
       <c r="B88">
+        <f t="shared" si="82"/>
+        <v>1.39500073732228E-2</v>
+      </c>
+      <c r="C88">
         <f t="shared" si="76"/>
-        <v>1.39500073732228E-2</v>
-      </c>
-      <c r="C88">
+        <v>4.3809873983283003E-3</v>
+      </c>
+      <c r="D88">
         <f t="shared" si="77"/>
-        <v>4.3809873983283003E-3</v>
-      </c>
-      <c r="D88">
+        <v>1.2063215077105796E-2</v>
+      </c>
+      <c r="E88">
         <f t="shared" si="78"/>
-        <v>1.2063215077105796E-2</v>
-      </c>
-      <c r="E88">
+        <v>9.7488425567582998E-3</v>
+      </c>
+      <c r="F88">
         <f t="shared" si="79"/>
-        <v>9.7488425567582998E-3</v>
-      </c>
-      <c r="F88">
+        <v>-7.9471047311684972E-3</v>
+      </c>
+      <c r="G88">
         <f t="shared" si="80"/>
-        <v>-7.9471047311684972E-3</v>
-      </c>
-      <c r="G88">
-        <f t="shared" si="81"/>
         <v>4.9025881310182998E-3</v>
       </c>
       <c r="H88">
@@ -59454,27 +59409,27 @@
         <v>176</v>
       </c>
       <c r="B89">
+        <f t="shared" si="82"/>
+        <v>-4.2685459837906004E-2</v>
+      </c>
+      <c r="C89">
         <f t="shared" si="76"/>
-        <v>-4.2685459837906004E-2</v>
-      </c>
-      <c r="C89">
+        <v>-8.0751475362517006E-2</v>
+      </c>
+      <c r="D89">
         <f t="shared" si="77"/>
-        <v>-8.0751475362517006E-2</v>
-      </c>
-      <c r="D89">
+        <v>1.5906120089126008E-2</v>
+      </c>
+      <c r="E89">
         <f t="shared" si="78"/>
-        <v>1.5906120089126008E-2</v>
-      </c>
-      <c r="E89">
+        <v>-9.625875615444035E-3</v>
+      </c>
+      <c r="F89">
         <f t="shared" si="79"/>
-        <v>-9.625875615444035E-3</v>
-      </c>
-      <c r="F89">
+        <v>-7.4887324726432003E-2</v>
+      </c>
+      <c r="G89">
         <f t="shared" si="80"/>
-        <v>-7.4887324726432003E-2</v>
-      </c>
-      <c r="G89">
-        <f t="shared" si="81"/>
         <v>3.5473120706627004E-2</v>
       </c>
       <c r="H89">
@@ -59495,27 +59450,27 @@
         <v>177</v>
       </c>
       <c r="B90">
+        <f t="shared" si="82"/>
+        <v>-2.746374923766802E-3</v>
+      </c>
+      <c r="C90">
         <f t="shared" si="76"/>
-        <v>-2.746374923766802E-3</v>
-      </c>
-      <c r="C90">
+        <v>-2.6392551038817991E-3</v>
+      </c>
+      <c r="D90">
         <f t="shared" si="77"/>
-        <v>-2.6392551038817991E-3</v>
-      </c>
-      <c r="D90">
+        <v>-1.0809671169131965E-3</v>
+      </c>
+      <c r="E90">
         <f t="shared" si="78"/>
-        <v>-1.0809671169131965E-3</v>
-      </c>
-      <c r="E90">
+        <v>3.5813772240972E-2</v>
+      </c>
+      <c r="F90">
         <f t="shared" si="79"/>
-        <v>3.5813772240972E-2</v>
-      </c>
-      <c r="F90">
+        <v>-1.5070555759201992E-2</v>
+      </c>
+      <c r="G90">
         <f t="shared" si="80"/>
-        <v>-1.5070555759201992E-2</v>
-      </c>
-      <c r="G90">
-        <f t="shared" si="81"/>
         <v>1.4979237849778802E-2</v>
       </c>
       <c r="H90">
@@ -59536,27 +59491,27 @@
         <v>178</v>
       </c>
       <c r="B91">
+        <f t="shared" si="82"/>
+        <v>4.8710057793996953E-3</v>
+      </c>
+      <c r="C91">
         <f t="shared" si="76"/>
-        <v>4.8710057793996953E-3</v>
-      </c>
-      <c r="C91">
+        <v>-2.219848572078395E-3</v>
+      </c>
+      <c r="D91">
         <f t="shared" si="77"/>
-        <v>-2.219848572078395E-3</v>
-      </c>
-      <c r="D91">
+        <v>8.3726169316141047E-3</v>
+      </c>
+      <c r="E91">
         <f t="shared" si="78"/>
-        <v>8.3726169316141047E-3</v>
-      </c>
-      <c r="E91">
+        <v>3.2840450104303004E-2</v>
+      </c>
+      <c r="F91">
         <f t="shared" si="79"/>
-        <v>3.2840450104303004E-2</v>
-      </c>
-      <c r="F91">
+        <v>4.0229219045176998E-2</v>
+      </c>
+      <c r="G91">
         <f t="shared" si="80"/>
-        <v>4.0229219045176998E-2</v>
-      </c>
-      <c r="G91">
-        <f t="shared" si="81"/>
         <v>3.3833267382030047E-3</v>
       </c>
       <c r="H91">
@@ -59577,27 +59532,27 @@
         <v>179</v>
       </c>
       <c r="B92">
+        <f t="shared" si="82"/>
+        <v>-9.2342115537791258E-4</v>
+      </c>
+      <c r="C92">
         <f t="shared" si="76"/>
-        <v>-9.2342115537791258E-4</v>
-      </c>
-      <c r="C92">
+        <v>1.0521983177584016E-2</v>
+      </c>
+      <c r="D92">
         <f t="shared" si="77"/>
-        <v>1.0521983177584016E-2</v>
-      </c>
-      <c r="D92">
+        <v>3.3662770906472961E-2</v>
+      </c>
+      <c r="E92">
         <f t="shared" si="78"/>
-        <v>3.3662770906472961E-2</v>
-      </c>
-      <c r="E92">
+        <v>0.21645373475839103</v>
+      </c>
+      <c r="F92">
         <f t="shared" si="79"/>
-        <v>0.21645373475839103</v>
-      </c>
-      <c r="F92">
+        <v>5.2932053582818939E-2</v>
+      </c>
+      <c r="G92">
         <f t="shared" si="80"/>
-        <v>5.2932053582818939E-2</v>
-      </c>
-      <c r="G92">
-        <f t="shared" si="81"/>
         <v>0.12853014820037401</v>
       </c>
       <c r="H92">
@@ -59618,27 +59573,27 @@
         <v>180</v>
       </c>
       <c r="B93">
+        <f t="shared" si="82"/>
+        <v>-6.2920820849140247E-3</v>
+      </c>
+      <c r="C93">
         <f t="shared" si="76"/>
-        <v>-6.2920820849140247E-3</v>
-      </c>
-      <c r="C93">
+        <v>-7.9798133784400038E-3</v>
+      </c>
+      <c r="D93">
         <f t="shared" si="77"/>
-        <v>-7.9798133784400038E-3</v>
-      </c>
-      <c r="D93">
+        <v>-3.5138425882634994E-2</v>
+      </c>
+      <c r="E93">
         <f t="shared" si="78"/>
-        <v>-3.5138425882634994E-2</v>
-      </c>
-      <c r="E93">
+        <v>4.8631961276864991E-2</v>
+      </c>
+      <c r="F93">
         <f t="shared" si="79"/>
-        <v>4.8631961276864991E-2</v>
-      </c>
-      <c r="F93">
+        <v>6.5285739783556979E-2</v>
+      </c>
+      <c r="G93">
         <f t="shared" si="80"/>
-        <v>6.5285739783556979E-2</v>
-      </c>
-      <c r="G93">
-        <f t="shared" si="81"/>
         <v>3.0838421862053017E-2</v>
       </c>
       <c r="H93">
@@ -59656,43 +59611,43 @@
     </row>
     <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>250</v>
+        <v>278</v>
       </c>
       <c r="B94">
-        <f>AVERAGE(B71:B73)</f>
-        <v>4.1992247185099134E-2</v>
+        <f>SUM(B71:B73)</f>
+        <v>0.12597674155529739</v>
       </c>
       <c r="C94">
-        <f t="shared" ref="C94:H94" si="98">AVERAGE(C71:C73)</f>
-        <v>8.1472474993935038E-3</v>
+        <f t="shared" ref="C94:H94" si="98">SUM(C71:C73)</f>
+        <v>2.4441742498180513E-2</v>
       </c>
       <c r="D94">
         <f t="shared" si="98"/>
-        <v>6.2288265320269987E-3</v>
+        <v>1.8686479596080996E-2</v>
       </c>
       <c r="E94">
         <f t="shared" si="98"/>
-        <v>3.4412057139585998E-2</v>
+        <v>0.10323617141875799</v>
       </c>
       <c r="F94">
         <f t="shared" si="98"/>
-        <v>1.6383116817407128E-2</v>
+        <v>4.914935045222138E-2</v>
       </c>
       <c r="G94">
         <f t="shared" si="98"/>
-        <v>1.1372783339787945E-2</v>
+        <v>3.4118350019363836E-2</v>
       </c>
       <c r="H94">
         <f t="shared" si="98"/>
-        <v>2.3511979380715333E-2</v>
+        <v>7.0535938142145996E-2</v>
       </c>
       <c r="I94">
         <f>AVERAGE(B94:H94)</f>
-        <v>2.029260827057372E-2</v>
+        <v>6.0877824811721153E-2</v>
       </c>
       <c r="K94">
-        <f t="shared" si="85"/>
-        <v>4.782503530621836E-3</v>
+        <f>_xlfn.STDEV.P(B94:H94)/SQRT(COUNT(B94:H94))</f>
+        <v>1.4347510591865507E-2</v>
       </c>
     </row>
     <row r="225" spans="1:11" x14ac:dyDescent="0.25">
@@ -61381,43 +61336,43 @@
       </c>
       <c r="B267">
         <f>B94/B$50*100</f>
-        <v>0.35324973678644972</v>
+        <v>1.0597492103593491</v>
       </c>
       <c r="C267">
         <f t="shared" ref="C267:H267" si="105">C94/C$50*100</f>
-        <v>7.4386514212211124E-2</v>
+        <v>0.2231595426366334</v>
       </c>
       <c r="D267">
         <f t="shared" si="105"/>
-        <v>5.681840569924819E-2</v>
+        <v>0.17045521709774461</v>
       </c>
       <c r="E267">
         <f t="shared" si="105"/>
-        <v>0.33550577289007288</v>
+        <v>1.0065173186702185</v>
       </c>
       <c r="F267">
         <f t="shared" si="105"/>
-        <v>0.1414745468087141</v>
+        <v>0.42442364042614222</v>
       </c>
       <c r="G267">
         <f t="shared" si="105"/>
-        <v>9.1700130183428902E-2</v>
+        <v>0.27510039055028673</v>
       </c>
       <c r="H267">
         <f t="shared" si="105"/>
-        <v>0.1765176173510343</v>
+        <v>0.52955285205310287</v>
       </c>
       <c r="I267">
         <f t="shared" si="101"/>
-        <v>0.17566467484730847</v>
+        <v>0.52699402454192534</v>
       </c>
       <c r="K267">
         <f t="shared" si="100"/>
-        <v>4.2782570713591588E-2</v>
+        <v>0.12834771214077476</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="BY26:BY32">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="BY26:BY32">
     <sortCondition ref="BY26"/>
   </sortState>
   <hyperlinks>

</xml_diff>